<commit_message>
[Fonds de solidarite] Add 2020-05-25 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -597,10 +597,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>23877</v>
+        <v>24092</v>
       </c>
       <c r="D2">
-        <v>34851567</v>
+        <v>35156499</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -623,10 +623,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>60223</v>
+        <v>60804</v>
       </c>
       <c r="D3">
-        <v>89123815</v>
+        <v>89956419</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -649,10 +649,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>20440</v>
+        <v>20679</v>
       </c>
       <c r="D4">
-        <v>30493309</v>
+        <v>30842893</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -675,10 +675,10 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>5388</v>
+        <v>5454</v>
       </c>
       <c r="D5">
-        <v>8058820</v>
+        <v>8155097</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -701,10 +701,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>1073</v>
+        <v>1090</v>
       </c>
       <c r="D6">
-        <v>1607197</v>
+        <v>1632697</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -727,10 +727,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D7">
-        <v>99000</v>
+        <v>100500</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -805,10 +805,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>25604</v>
+        <v>25848</v>
       </c>
       <c r="D10">
-        <v>35364098</v>
+        <v>35682192</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -831,10 +831,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>6269</v>
+        <v>6307</v>
       </c>
       <c r="D11">
-        <v>9169063</v>
+        <v>9222147</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -857,10 +857,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>17677</v>
+        <v>17838</v>
       </c>
       <c r="D12">
-        <v>26137883</v>
+        <v>26365522</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -883,10 +883,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>5509</v>
+        <v>5580</v>
       </c>
       <c r="D13">
-        <v>8225163</v>
+        <v>8327171</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -909,10 +909,10 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>1305</v>
+        <v>1326</v>
       </c>
       <c r="D14">
-        <v>1952095</v>
+        <v>1981619</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
@@ -935,10 +935,10 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D15">
-        <v>351266</v>
+        <v>355766</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -987,10 +987,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>6424</v>
+        <v>6495</v>
       </c>
       <c r="D17">
-        <v>8691614</v>
+        <v>8782368</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -1013,10 +1013,10 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>8710</v>
+        <v>8766</v>
       </c>
       <c r="D18">
-        <v>12695451</v>
+        <v>12766330</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1039,10 +1039,10 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>21621</v>
+        <v>21796</v>
       </c>
       <c r="D19">
-        <v>31997208</v>
+        <v>32240515</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1065,10 +1065,10 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>6874</v>
+        <v>6943</v>
       </c>
       <c r="D20">
-        <v>10269407</v>
+        <v>10369461</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1091,10 +1091,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>1650</v>
+        <v>1676</v>
       </c>
       <c r="D21">
-        <v>2469802</v>
+        <v>2508668</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -1117,10 +1117,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D22">
-        <v>362624</v>
+        <v>368624</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -1169,10 +1169,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>7472</v>
+        <v>7537</v>
       </c>
       <c r="D24">
-        <v>10211253</v>
+        <v>10297479</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -1195,10 +1195,10 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>4940</v>
+        <v>4972</v>
       </c>
       <c r="D25">
-        <v>7205853</v>
+        <v>7249883</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -1221,10 +1221,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>15237</v>
+        <v>15360</v>
       </c>
       <c r="D26">
-        <v>22538519</v>
+        <v>22715206</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
@@ -1247,10 +1247,10 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>5192</v>
+        <v>5240</v>
       </c>
       <c r="D27">
-        <v>7759432</v>
+        <v>7829969</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
@@ -1273,10 +1273,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>1250</v>
+        <v>1264</v>
       </c>
       <c r="D28">
-        <v>1874491</v>
+        <v>1894837</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
@@ -1299,10 +1299,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D29">
-        <v>277500</v>
+        <v>279000</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
@@ -1351,10 +1351,10 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>5287</v>
+        <v>5348</v>
       </c>
       <c r="D31">
-        <v>7096203</v>
+        <v>7174117</v>
       </c>
       <c r="E31" t="s">
         <v>13</v>
@@ -1377,10 +1377,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>1744</v>
+        <v>1756</v>
       </c>
       <c r="D32">
-        <v>2513803</v>
+        <v>2530919</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
@@ -1403,10 +1403,10 @@
         <v>9</v>
       </c>
       <c r="C33">
-        <v>4600</v>
+        <v>4642</v>
       </c>
       <c r="D33">
-        <v>6755754</v>
+        <v>6815591</v>
       </c>
       <c r="E33" t="s">
         <v>14</v>
@@ -1429,10 +1429,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>1873</v>
+        <v>1887</v>
       </c>
       <c r="D34">
-        <v>2786851</v>
+        <v>2807851</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
@@ -1455,10 +1455,10 @@
         <v>9</v>
       </c>
       <c r="C35">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="D35">
-        <v>727041</v>
+        <v>739041</v>
       </c>
       <c r="E35" t="s">
         <v>14</v>
@@ -1533,10 +1533,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>1181</v>
+        <v>1195</v>
       </c>
       <c r="D38">
-        <v>1607948</v>
+        <v>1627872</v>
       </c>
       <c r="E38" t="s">
         <v>14</v>
@@ -1559,10 +1559,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>11137</v>
+        <v>11230</v>
       </c>
       <c r="D39">
-        <v>16233908</v>
+        <v>16367634</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -1585,10 +1585,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>34330</v>
+        <v>34685</v>
       </c>
       <c r="D40">
-        <v>50737254</v>
+        <v>51234896</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
@@ -1611,10 +1611,10 @@
         <v>9</v>
       </c>
       <c r="C41">
-        <v>12742</v>
+        <v>12860</v>
       </c>
       <c r="D41">
-        <v>19033677</v>
+        <v>19204635</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -1637,10 +1637,10 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>3533</v>
+        <v>3575</v>
       </c>
       <c r="D42">
-        <v>5288416</v>
+        <v>5350598</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
@@ -1663,10 +1663,10 @@
         <v>9</v>
       </c>
       <c r="C43">
-        <v>615</v>
+        <v>627</v>
       </c>
       <c r="D43">
-        <v>921436</v>
+        <v>937953</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -1741,10 +1741,10 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>10435</v>
+        <v>10541</v>
       </c>
       <c r="D46">
-        <v>14205878</v>
+        <v>14335991</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
@@ -1767,10 +1767,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="D47">
-        <v>1467198</v>
+        <v>1470198</v>
       </c>
       <c r="E47" t="s">
         <v>16</v>
@@ -1793,10 +1793,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>3787</v>
+        <v>3808</v>
       </c>
       <c r="D48">
-        <v>5584834</v>
+        <v>5613489</v>
       </c>
       <c r="E48" t="s">
         <v>16</v>
@@ -1819,10 +1819,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>1409</v>
+        <v>1419</v>
       </c>
       <c r="D49">
-        <v>2106464</v>
+        <v>2121464</v>
       </c>
       <c r="E49" t="s">
         <v>16</v>
@@ -1845,10 +1845,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D50">
-        <v>654500</v>
+        <v>656000</v>
       </c>
       <c r="E50" t="s">
         <v>16</v>
@@ -1897,10 +1897,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>2503</v>
+        <v>2533</v>
       </c>
       <c r="D52">
-        <v>3482429</v>
+        <v>3521757</v>
       </c>
       <c r="E52" t="s">
         <v>16</v>
@@ -1923,10 +1923,10 @@
         <v>9</v>
       </c>
       <c r="C53">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="D53">
-        <v>517784</v>
+        <v>526784</v>
       </c>
       <c r="E53" t="s">
         <v>17</v>
@@ -1949,10 +1949,10 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>963</v>
+        <v>970</v>
       </c>
       <c r="D54">
-        <v>1426244</v>
+        <v>1436744</v>
       </c>
       <c r="E54" t="s">
         <v>17</v>
@@ -1975,10 +1975,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="D55">
-        <v>588572</v>
+        <v>593072</v>
       </c>
       <c r="E55" t="s">
         <v>17</v>
@@ -2079,10 +2079,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="D59">
-        <v>666625</v>
+        <v>675625</v>
       </c>
       <c r="E59" t="s">
         <v>17</v>
@@ -2105,10 +2105,10 @@
         <v>9</v>
       </c>
       <c r="C60">
-        <v>10069</v>
+        <v>10140</v>
       </c>
       <c r="D60">
-        <v>14625136</v>
+        <v>14728746</v>
       </c>
       <c r="E60" t="s">
         <v>18</v>
@@ -2131,10 +2131,10 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <v>30695</v>
+        <v>30932</v>
       </c>
       <c r="D61">
-        <v>45282625</v>
+        <v>45626014</v>
       </c>
       <c r="E61" t="s">
         <v>18</v>
@@ -2157,10 +2157,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>10677</v>
+        <v>10789</v>
       </c>
       <c r="D62">
-        <v>15954655</v>
+        <v>16119058</v>
       </c>
       <c r="E62" t="s">
         <v>18</v>
@@ -2183,10 +2183,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>2960</v>
+        <v>2993</v>
       </c>
       <c r="D63">
-        <v>4430138</v>
+        <v>4478160</v>
       </c>
       <c r="E63" t="s">
         <v>18</v>
@@ -2209,10 +2209,10 @@
         <v>9</v>
       </c>
       <c r="C64">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="D64">
-        <v>781931</v>
+        <v>795431</v>
       </c>
       <c r="E64" t="s">
         <v>18</v>
@@ -2261,10 +2261,10 @@
         <v>9</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D66">
-        <v>6287</v>
+        <v>7787</v>
       </c>
       <c r="E66" t="s">
         <v>18</v>
@@ -2287,10 +2287,10 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>9978</v>
+        <v>10053</v>
       </c>
       <c r="D67">
-        <v>13368699</v>
+        <v>13461327</v>
       </c>
       <c r="E67" t="s">
         <v>18</v>
@@ -2313,10 +2313,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>2746</v>
+        <v>2774</v>
       </c>
       <c r="D68">
-        <v>4005992</v>
+        <v>4045452</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
@@ -2339,10 +2339,10 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>7449</v>
+        <v>7509</v>
       </c>
       <c r="D69">
-        <v>10989910</v>
+        <v>11073769</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
@@ -2365,10 +2365,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>2641</v>
+        <v>2660</v>
       </c>
       <c r="D70">
-        <v>3945983</v>
+        <v>3974483</v>
       </c>
       <c r="E70" t="s">
         <v>19</v>
@@ -2391,10 +2391,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>868</v>
+        <v>878</v>
       </c>
       <c r="D71">
-        <v>1300049</v>
+        <v>1315049</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
@@ -2417,10 +2417,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D72">
-        <v>259612</v>
+        <v>261112</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
@@ -2469,10 +2469,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>2903</v>
+        <v>2950</v>
       </c>
       <c r="D74">
-        <v>3956945</v>
+        <v>4016747</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
@@ -2495,10 +2495,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>881</v>
+        <v>886</v>
       </c>
       <c r="D75">
-        <v>1278393</v>
+        <v>1284391</v>
       </c>
       <c r="E75" t="s">
         <v>20</v>
@@ -2521,10 +2521,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>3015</v>
+        <v>3031</v>
       </c>
       <c r="D76">
-        <v>4453499</v>
+        <v>4476858</v>
       </c>
       <c r="E76" t="s">
         <v>20</v>
@@ -2547,10 +2547,10 @@
         <v>9</v>
       </c>
       <c r="C77">
-        <v>1201</v>
+        <v>1207</v>
       </c>
       <c r="D77">
-        <v>1796939</v>
+        <v>1805939</v>
       </c>
       <c r="E77" t="s">
         <v>20</v>
@@ -2573,10 +2573,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="D78">
-        <v>619500</v>
+        <v>627000</v>
       </c>
       <c r="E78" t="s">
         <v>20</v>
@@ -2651,10 +2651,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>1797</v>
+        <v>1810</v>
       </c>
       <c r="D81">
-        <v>2413902</v>
+        <v>2432059</v>
       </c>
       <c r="E81" t="s">
         <v>20</v>
@@ -2677,10 +2677,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D82">
-        <v>459689</v>
+        <v>462689</v>
       </c>
       <c r="E82" t="s">
         <v>21</v>
@@ -2703,10 +2703,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D83">
-        <v>163110</v>
+        <v>164610</v>
       </c>
       <c r="E83" t="s">
         <v>21</v>
@@ -2755,10 +2755,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D85">
-        <v>22500</v>
+        <v>25500</v>
       </c>
       <c r="E85" t="s">
         <v>21</v>
@@ -2807,10 +2807,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>7079</v>
+        <v>7128</v>
       </c>
       <c r="D87">
-        <v>10353049</v>
+        <v>10425054</v>
       </c>
       <c r="E87" t="s">
         <v>22</v>
@@ -2833,10 +2833,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>20363</v>
+        <v>20512</v>
       </c>
       <c r="D88">
-        <v>30122799</v>
+        <v>30341239</v>
       </c>
       <c r="E88" t="s">
         <v>22</v>
@@ -2859,10 +2859,10 @@
         <v>9</v>
       </c>
       <c r="C89">
-        <v>6696</v>
+        <v>6756</v>
       </c>
       <c r="D89">
-        <v>10007887</v>
+        <v>10095322</v>
       </c>
       <c r="E89" t="s">
         <v>22</v>
@@ -2885,10 +2885,10 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>1769</v>
+        <v>1788</v>
       </c>
       <c r="D90">
-        <v>2648271</v>
+        <v>2676771</v>
       </c>
       <c r="E90" t="s">
         <v>22</v>
@@ -2911,10 +2911,10 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="D91">
-        <v>424310</v>
+        <v>431810</v>
       </c>
       <c r="E91" t="s">
         <v>22</v>
@@ -2937,10 +2937,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D92">
-        <v>34500</v>
+        <v>36000</v>
       </c>
       <c r="E92" t="s">
         <v>22</v>
@@ -2989,10 +2989,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>6356</v>
+        <v>6403</v>
       </c>
       <c r="D94">
-        <v>8570116</v>
+        <v>8621161</v>
       </c>
       <c r="E94" t="s">
         <v>22</v>
@@ -3015,10 +3015,10 @@
         <v>9</v>
       </c>
       <c r="C95">
-        <v>19448</v>
+        <v>19580</v>
       </c>
       <c r="D95">
-        <v>28242536</v>
+        <v>28434203</v>
       </c>
       <c r="E95" t="s">
         <v>23</v>
@@ -3041,10 +3041,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>45186</v>
+        <v>45564</v>
       </c>
       <c r="D96">
-        <v>66645947</v>
+        <v>67186825</v>
       </c>
       <c r="E96" t="s">
         <v>23</v>
@@ -3067,10 +3067,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>14471</v>
+        <v>14616</v>
       </c>
       <c r="D97">
-        <v>21604981</v>
+        <v>21815946</v>
       </c>
       <c r="E97" t="s">
         <v>23</v>
@@ -3093,10 +3093,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>3873</v>
+        <v>3926</v>
       </c>
       <c r="D98">
-        <v>5794340</v>
+        <v>5871908</v>
       </c>
       <c r="E98" t="s">
         <v>23</v>
@@ -3119,10 +3119,10 @@
         <v>9</v>
       </c>
       <c r="C99">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="D99">
-        <v>989862</v>
+        <v>992862</v>
       </c>
       <c r="E99" t="s">
         <v>23</v>
@@ -3171,10 +3171,10 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D101">
-        <v>12000</v>
+        <v>13500</v>
       </c>
       <c r="E101" t="s">
         <v>23</v>
@@ -3197,10 +3197,10 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>16646</v>
+        <v>16771</v>
       </c>
       <c r="D102">
-        <v>22609010</v>
+        <v>22775050</v>
       </c>
       <c r="E102" t="s">
         <v>23</v>
@@ -3223,10 +3223,10 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>22224</v>
+        <v>22396</v>
       </c>
       <c r="D103">
-        <v>32313700</v>
+        <v>32551921</v>
       </c>
       <c r="E103" t="s">
         <v>24</v>
@@ -3249,10 +3249,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>50288</v>
+        <v>50723</v>
       </c>
       <c r="D104">
-        <v>74090263</v>
+        <v>74715644</v>
       </c>
       <c r="E104" t="s">
         <v>24</v>
@@ -3275,10 +3275,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>15749</v>
+        <v>15914</v>
       </c>
       <c r="D105">
-        <v>23482059</v>
+        <v>23717248</v>
       </c>
       <c r="E105" t="s">
         <v>24</v>
@@ -3301,10 +3301,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>4021</v>
+        <v>4070</v>
       </c>
       <c r="D106">
-        <v>6007501</v>
+        <v>6079501</v>
       </c>
       <c r="E106" t="s">
         <v>24</v>
@@ -3327,10 +3327,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>656</v>
+        <v>667</v>
       </c>
       <c r="D107">
-        <v>981054</v>
+        <v>997554</v>
       </c>
       <c r="E107" t="s">
         <v>24</v>
@@ -3353,10 +3353,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D108">
-        <v>43228</v>
+        <v>44728</v>
       </c>
       <c r="E108" t="s">
         <v>24</v>
@@ -3405,10 +3405,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>19712</v>
+        <v>19904</v>
       </c>
       <c r="D110">
-        <v>26585844</v>
+        <v>26845223</v>
       </c>
       <c r="E110" t="s">
         <v>24</v>
@@ -3431,10 +3431,10 @@
         <v>9</v>
       </c>
       <c r="C111">
-        <v>8643</v>
+        <v>8701</v>
       </c>
       <c r="D111">
-        <v>12623139</v>
+        <v>12706185</v>
       </c>
       <c r="E111" t="s">
         <v>25</v>
@@ -3457,10 +3457,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>22405</v>
+        <v>22577</v>
       </c>
       <c r="D112">
-        <v>33157573</v>
+        <v>33399155</v>
       </c>
       <c r="E112" t="s">
         <v>25</v>
@@ -3483,10 +3483,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>7794</v>
+        <v>7872</v>
       </c>
       <c r="D113">
-        <v>11635128</v>
+        <v>11749723</v>
       </c>
       <c r="E113" t="s">
         <v>25</v>
@@ -3509,10 +3509,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>1885</v>
+        <v>1914</v>
       </c>
       <c r="D114">
-        <v>2819669</v>
+        <v>2861601</v>
       </c>
       <c r="E114" t="s">
         <v>25</v>
@@ -3535,10 +3535,10 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D115">
-        <v>400762</v>
+        <v>406762</v>
       </c>
       <c r="E115" t="s">
         <v>25</v>
@@ -3613,10 +3613,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>7068</v>
+        <v>7130</v>
       </c>
       <c r="D118">
-        <v>9618736</v>
+        <v>9702412</v>
       </c>
       <c r="E118" t="s">
         <v>25</v>
@@ -3639,10 +3639,10 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>21653</v>
+        <v>21830</v>
       </c>
       <c r="D119">
-        <v>31479362</v>
+        <v>31733694</v>
       </c>
       <c r="E119" t="s">
         <v>26</v>
@@ -3665,10 +3665,10 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>53421</v>
+        <v>53844</v>
       </c>
       <c r="D120">
-        <v>78781854</v>
+        <v>79382968</v>
       </c>
       <c r="E120" t="s">
         <v>26</v>
@@ -3691,10 +3691,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>16119</v>
+        <v>16277</v>
       </c>
       <c r="D121">
-        <v>24072780</v>
+        <v>24301440</v>
       </c>
       <c r="E121" t="s">
         <v>26</v>
@@ -3717,10 +3717,10 @@
         <v>9</v>
       </c>
       <c r="C122">
-        <v>4005</v>
+        <v>4048</v>
       </c>
       <c r="D122">
-        <v>5990997</v>
+        <v>6055497</v>
       </c>
       <c r="E122" t="s">
         <v>26</v>
@@ -3743,10 +3743,10 @@
         <v>9</v>
       </c>
       <c r="C123">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="D123">
-        <v>1216212</v>
+        <v>1222212</v>
       </c>
       <c r="E123" t="s">
         <v>26</v>
@@ -3821,10 +3821,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>18424</v>
+        <v>18558</v>
       </c>
       <c r="D126">
-        <v>25314565</v>
+        <v>25486511</v>
       </c>
       <c r="E126" t="s">
         <v>26</v>
@@ -3847,10 +3847,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>29809</v>
+        <v>30060</v>
       </c>
       <c r="D127">
-        <v>43654042</v>
+        <v>44011111</v>
       </c>
       <c r="E127" t="s">
         <v>27</v>
@@ -3873,10 +3873,10 @@
         <v>9</v>
       </c>
       <c r="C128">
-        <v>89658</v>
+        <v>90469</v>
       </c>
       <c r="D128">
-        <v>132797538</v>
+        <v>133983971</v>
       </c>
       <c r="E128" t="s">
         <v>27</v>
@@ -3899,10 +3899,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>39824</v>
+        <v>40169</v>
       </c>
       <c r="D129">
-        <v>59518407</v>
+        <v>60029201</v>
       </c>
       <c r="E129" t="s">
         <v>27</v>
@@ -3925,10 +3925,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>12413</v>
+        <v>12503</v>
       </c>
       <c r="D130">
-        <v>18591962</v>
+        <v>18726517</v>
       </c>
       <c r="E130" t="s">
         <v>27</v>
@@ -3951,10 +3951,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>2533</v>
+        <v>2576</v>
       </c>
       <c r="D131">
-        <v>3793255</v>
+        <v>3856006</v>
       </c>
       <c r="E131" t="s">
         <v>27</v>
@@ -3977,10 +3977,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D132">
-        <v>200212</v>
+        <v>203212</v>
       </c>
       <c r="E132" t="s">
         <v>27</v>
@@ -4055,10 +4055,10 @@
         <v>9</v>
       </c>
       <c r="C135">
-        <v>29310</v>
+        <v>29560</v>
       </c>
       <c r="D135">
-        <v>40855546</v>
+        <v>41176828</v>
       </c>
       <c r="E135" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
[Fonds de solidarite] Fix missing 2020-06-25 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -66,6 +66,74 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:H146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,10 +488,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34545</v>
+        <v>34666</v>
       </c>
       <c r="D2" t="n">
-        <v>50057484</v>
+        <v>50224732</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +526,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>84645</v>
+        <v>84958</v>
       </c>
       <c r="D3" t="n">
-        <v>124268474</v>
+        <v>124713672</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +564,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>28995</v>
+        <v>29125</v>
       </c>
       <c r="D4" t="n">
-        <v>42985902</v>
+        <v>43179227</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -534,10 +602,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7968</v>
+        <v>8002</v>
       </c>
       <c r="D5" t="n">
-        <v>11851691</v>
+        <v>11902197</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -572,10 +640,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1684</v>
+        <v>1696</v>
       </c>
       <c r="D6" t="n">
-        <v>2506354</v>
+        <v>2524354</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -610,10 +678,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D7" t="n">
-        <v>178093</v>
+        <v>182593</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -686,10 +754,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>9000</v>
+        <v>4500</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -703,12 +771,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1 000 à 1 999 salariés</t>
+          <t>100 à 199 salariés</t>
         </is>
       </c>
     </row>
@@ -724,10 +792,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>37883</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>51582135</v>
+        <v>9000</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -741,12 +809,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>42</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>1 000 à 1 999 salariés</t>
         </is>
       </c>
     </row>
@@ -762,29 +830,29 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8893</v>
+        <v>38026</v>
       </c>
       <c r="D11" t="n">
-        <v>12882707</v>
+        <v>51776857</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>84</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Bourgogne-Franche-Comté</t>
+          <t>Auvergne-Rhône-Alpes</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -800,10 +868,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>24376</v>
+        <v>8916</v>
       </c>
       <c r="D12" t="n">
-        <v>35792139</v>
+        <v>12914245</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -817,12 +885,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -838,10 +906,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7765</v>
+        <v>24474</v>
       </c>
       <c r="D13" t="n">
-        <v>11538413</v>
+        <v>35927448</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -855,12 +923,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -876,10 +944,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1962</v>
+        <v>7794</v>
       </c>
       <c r="D14" t="n">
-        <v>2918476</v>
+        <v>11580874</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -893,12 +961,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -914,10 +982,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>354</v>
+        <v>1971</v>
       </c>
       <c r="D15" t="n">
-        <v>521443</v>
+        <v>2931976</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -931,12 +999,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -952,10 +1020,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>28</v>
+        <v>358</v>
       </c>
       <c r="D16" t="n">
-        <v>42000</v>
+        <v>526123</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -969,12 +1037,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -990,10 +1058,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D17" t="n">
-        <v>7500</v>
+        <v>42000</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1007,12 +1075,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -1028,10 +1096,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>9402</v>
+        <v>5</v>
       </c>
       <c r="D18" t="n">
-        <v>12505788</v>
+        <v>7500</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1045,12 +1113,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -1066,29 +1134,29 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>12445</v>
+        <v>9455</v>
       </c>
       <c r="D19" t="n">
-        <v>17986503</v>
+        <v>12569388</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Bretagne</t>
+          <t>Bourgogne-Franche-Comté</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -1104,10 +1172,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>29773</v>
+        <v>12475</v>
       </c>
       <c r="D20" t="n">
-        <v>43757824</v>
+        <v>18028336</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1121,12 +1189,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -1142,10 +1210,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>9681</v>
+        <v>29871</v>
       </c>
       <c r="D21" t="n">
-        <v>14400084</v>
+        <v>43899622</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1159,12 +1227,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -1180,10 +1248,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2438</v>
+        <v>9714</v>
       </c>
       <c r="D22" t="n">
-        <v>3630312</v>
+        <v>14449584</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1197,12 +1265,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -1218,10 +1286,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>423</v>
+        <v>2447</v>
       </c>
       <c r="D23" t="n">
-        <v>629805</v>
+        <v>3641812</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1235,12 +1303,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -1256,10 +1324,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>427</v>
       </c>
       <c r="D24" t="n">
-        <v>39953</v>
+        <v>634845</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1273,12 +1341,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -1294,10 +1362,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>10848</v>
+        <v>28</v>
       </c>
       <c r="D25" t="n">
-        <v>14584134</v>
+        <v>41453</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1311,12 +1379,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -1332,29 +1400,29 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>7083</v>
+        <v>10893</v>
       </c>
       <c r="D26" t="n">
-        <v>10270095</v>
+        <v>14641323</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>53</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Centre-Val de Loire</t>
+          <t>Bretagne</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -1370,10 +1438,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>21095</v>
+        <v>7099</v>
       </c>
       <c r="D27" t="n">
-        <v>31000075</v>
+        <v>10293959</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1387,12 +1455,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -1408,10 +1476,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>7342</v>
+        <v>21147</v>
       </c>
       <c r="D28" t="n">
-        <v>10930142</v>
+        <v>31076129</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1425,12 +1493,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -1446,10 +1514,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1806</v>
+        <v>7360</v>
       </c>
       <c r="D29" t="n">
-        <v>2700286</v>
+        <v>10955797</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1463,12 +1531,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -1484,10 +1552,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>289</v>
+        <v>1810</v>
       </c>
       <c r="D30" t="n">
-        <v>430915</v>
+        <v>2706286</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1501,12 +1569,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -1522,10 +1590,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>25</v>
+        <v>295</v>
       </c>
       <c r="D31" t="n">
-        <v>37393</v>
+        <v>439915</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1539,12 +1607,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -1560,10 +1628,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>7658</v>
+        <v>25</v>
       </c>
       <c r="D32" t="n">
-        <v>10165367</v>
+        <v>37393</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1577,12 +1645,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -1598,29 +1666,29 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2750</v>
+        <v>7675</v>
       </c>
       <c r="D33" t="n">
-        <v>3968754</v>
+        <v>10186334</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Corse</t>
+          <t>Centre-Val de Loire</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -1636,10 +1704,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>6931</v>
+        <v>2763</v>
       </c>
       <c r="D34" t="n">
-        <v>10129704</v>
+        <v>3986490</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1653,12 +1721,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -1674,10 +1742,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2810</v>
+        <v>6956</v>
       </c>
       <c r="D35" t="n">
-        <v>4160023</v>
+        <v>10166222</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1691,12 +1759,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -1712,10 +1780,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>752</v>
+        <v>2822</v>
       </c>
       <c r="D36" t="n">
-        <v>1120763</v>
+        <v>4178023</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1729,12 +1797,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -1750,10 +1818,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>129</v>
+        <v>761</v>
       </c>
       <c r="D37" t="n">
-        <v>192804</v>
+        <v>1134263</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1767,12 +1835,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -1788,10 +1856,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="D38" t="n">
-        <v>6000</v>
+        <v>194304</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1805,12 +1873,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -1826,10 +1894,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2129</v>
+        <v>4</v>
       </c>
       <c r="D39" t="n">
-        <v>2870482</v>
+        <v>6000</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1843,12 +1911,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -1864,29 +1932,29 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>15882</v>
+        <v>2138</v>
       </c>
       <c r="D40" t="n">
-        <v>22998460</v>
+        <v>2882432</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>94</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Grand Est</t>
+          <t>Corse</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -1902,10 +1970,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>47787</v>
+        <v>15956</v>
       </c>
       <c r="D41" t="n">
-        <v>70130771</v>
+        <v>23103331</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1919,12 +1987,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -1940,10 +2008,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>17899</v>
+        <v>47963</v>
       </c>
       <c r="D42" t="n">
-        <v>26597840</v>
+        <v>70383427</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1957,12 +2025,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -1978,10 +2046,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5180</v>
+        <v>17982</v>
       </c>
       <c r="D43" t="n">
-        <v>7721916</v>
+        <v>26718524</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1995,12 +2063,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -2016,10 +2084,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>996</v>
+        <v>5196</v>
       </c>
       <c r="D44" t="n">
-        <v>1488353</v>
+        <v>7745916</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2033,12 +2101,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -2054,10 +2122,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>51</v>
+        <v>1017</v>
       </c>
       <c r="D45" t="n">
-        <v>75691</v>
+        <v>1517684</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2071,12 +2139,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -2092,10 +2160,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D46" t="n">
-        <v>13500</v>
+        <v>77191</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2109,12 +2177,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -2130,10 +2198,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D47" t="n">
-        <v>4500</v>
+        <v>15000</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2147,12 +2215,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>100 à 199 salariés</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -2168,10 +2236,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>15326</v>
+        <v>3</v>
       </c>
       <c r="D48" t="n">
-        <v>20498314</v>
+        <v>4500</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2185,12 +2253,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>100 à 199 salariés</t>
         </is>
       </c>
     </row>
@@ -2206,29 +2274,29 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1655</v>
+        <v>15387</v>
       </c>
       <c r="D49" t="n">
-        <v>2402294</v>
+        <v>20575600</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Guadeloupe</t>
+          <t>Grand Est</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -2244,10 +2312,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>5846</v>
+        <v>1664</v>
       </c>
       <c r="D50" t="n">
-        <v>8611745</v>
+        <v>2415094</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2261,12 +2329,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -2282,10 +2350,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2058</v>
+        <v>5872</v>
       </c>
       <c r="D51" t="n">
-        <v>3075015</v>
+        <v>8648593</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2299,12 +2367,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -2320,10 +2388,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>672</v>
+        <v>2063</v>
       </c>
       <c r="D52" t="n">
-        <v>1003305</v>
+        <v>3081370</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2337,12 +2405,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -2358,10 +2426,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>150</v>
+        <v>672</v>
       </c>
       <c r="D53" t="n">
-        <v>222611</v>
+        <v>1003305</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2375,12 +2443,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -2396,10 +2464,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>13</v>
+        <v>150</v>
       </c>
       <c r="D54" t="n">
-        <v>19500</v>
+        <v>222611</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2413,12 +2481,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -2434,10 +2502,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>5192</v>
+        <v>13</v>
       </c>
       <c r="D55" t="n">
-        <v>7174702</v>
+        <v>19500</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2451,12 +2519,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -2472,29 +2540,29 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>660</v>
+        <v>5242</v>
       </c>
       <c r="D56" t="n">
-        <v>967645</v>
+        <v>7244775</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>01</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Guyane</t>
+          <t>Guadeloupe</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -2510,10 +2578,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1658</v>
+        <v>663</v>
       </c>
       <c r="D57" t="n">
-        <v>2456107</v>
+        <v>971011</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2527,12 +2595,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -2548,10 +2616,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>662</v>
+        <v>1673</v>
       </c>
       <c r="D58" t="n">
-        <v>987219</v>
+        <v>2478607</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2565,12 +2633,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -2586,10 +2654,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>221</v>
+        <v>662</v>
       </c>
       <c r="D59" t="n">
-        <v>331258</v>
+        <v>987219</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2603,12 +2671,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -2624,10 +2692,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>44</v>
+        <v>223</v>
       </c>
       <c r="D60" t="n">
-        <v>66000</v>
+        <v>334258</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2641,12 +2709,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -2662,10 +2730,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D61" t="n">
-        <v>13500</v>
+        <v>67500</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2679,12 +2747,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -2700,10 +2768,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>968</v>
+        <v>9</v>
       </c>
       <c r="D62" t="n">
-        <v>1370542</v>
+        <v>13500</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2717,12 +2785,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -2738,29 +2806,29 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>14181</v>
+        <v>971</v>
       </c>
       <c r="D63" t="n">
-        <v>20506992</v>
+        <v>1375042</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>03</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Hauts-de-France</t>
+          <t>Guyane</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -2776,10 +2844,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>42019</v>
+        <v>14224</v>
       </c>
       <c r="D64" t="n">
-        <v>61557627</v>
+        <v>20567531</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2793,12 +2861,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -2814,10 +2882,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>14817</v>
+        <v>42152</v>
       </c>
       <c r="D65" t="n">
-        <v>22033895</v>
+        <v>61743623</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2831,12 +2899,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -2852,10 +2920,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>4245</v>
+        <v>14871</v>
       </c>
       <c r="D66" t="n">
-        <v>6325607</v>
+        <v>22114347</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2869,12 +2937,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -2890,10 +2958,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>804</v>
+        <v>4260</v>
       </c>
       <c r="D67" t="n">
-        <v>1198739</v>
+        <v>6346793</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2907,12 +2975,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -2928,10 +2996,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>67</v>
+        <v>814</v>
       </c>
       <c r="D68" t="n">
-        <v>99189</v>
+        <v>1213739</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2945,12 +3013,12 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -2966,10 +3034,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="D69" t="n">
-        <v>10787</v>
+        <v>99189</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2983,12 +3051,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -3004,10 +3072,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>14074</v>
+        <v>8</v>
       </c>
       <c r="D70" t="n">
-        <v>18643374</v>
+        <v>10787</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3021,12 +3089,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -3042,29 +3110,29 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>44936</v>
+        <v>14116</v>
       </c>
       <c r="D71" t="n">
-        <v>65445389</v>
+        <v>18699197</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>32</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Île-de-France</t>
+          <t>Hauts-de-France</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -3080,10 +3148,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>130752</v>
+        <v>45107</v>
       </c>
       <c r="D72" t="n">
-        <v>192800826</v>
+        <v>65690488</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3097,12 +3165,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -3118,10 +3186,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>57514</v>
+        <v>131218</v>
       </c>
       <c r="D73" t="n">
-        <v>85740251</v>
+        <v>193481298</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3135,12 +3203,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -3156,10 +3224,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>18212</v>
+        <v>57720</v>
       </c>
       <c r="D74" t="n">
-        <v>27217899</v>
+        <v>86047028</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3173,12 +3241,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -3194,10 +3262,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>3980</v>
+        <v>18295</v>
       </c>
       <c r="D75" t="n">
-        <v>5947170</v>
+        <v>27342349</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3211,12 +3279,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -3232,10 +3300,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>208</v>
+        <v>4026</v>
       </c>
       <c r="D76" t="n">
-        <v>307170</v>
+        <v>6016170</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3249,12 +3317,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -3270,10 +3338,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>17</v>
+        <v>213</v>
       </c>
       <c r="D77" t="n">
-        <v>24405</v>
+        <v>314670</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3287,12 +3355,12 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -3308,10 +3376,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D78" t="n">
-        <v>8125</v>
+        <v>24405</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3325,12 +3393,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>100 à 199 salariés</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -3346,10 +3414,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D79" t="n">
-        <v>4500</v>
+        <v>8125</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3363,12 +3431,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>200 à 249 salariés</t>
+          <t>100 à 199 salariés</t>
         </is>
       </c>
     </row>
@@ -3401,12 +3469,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>31</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>250 à 499 salariés</t>
+          <t>200 à 249 salariés</t>
         </is>
       </c>
     </row>
@@ -3439,12 +3507,12 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>32</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>10 000 salariés et plus</t>
+          <t>250 à 499 salariés</t>
         </is>
       </c>
     </row>
@@ -3460,10 +3528,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>44512</v>
+        <v>3</v>
       </c>
       <c r="D82" t="n">
-        <v>60965825</v>
+        <v>4500</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3477,12 +3545,12 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>53</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>10 000 salariés et plus</t>
         </is>
       </c>
     </row>
@@ -3498,29 +3566,29 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4044</v>
+        <v>44636</v>
       </c>
       <c r="D83" t="n">
-        <v>5865730</v>
+        <v>61129665</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>La Réunion</t>
+          <t>Île-de-France</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -3536,10 +3604,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>10472</v>
+        <v>4056</v>
       </c>
       <c r="D84" t="n">
-        <v>15396877</v>
+        <v>5883360</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3553,12 +3621,12 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -3574,10 +3642,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3587</v>
+        <v>10514</v>
       </c>
       <c r="D85" t="n">
-        <v>5347696</v>
+        <v>15459077</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3591,12 +3659,12 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -3612,10 +3680,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1240</v>
+        <v>3605</v>
       </c>
       <c r="D86" t="n">
-        <v>1854591</v>
+        <v>5374696</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3629,12 +3697,12 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -3650,10 +3718,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>250</v>
+        <v>1247</v>
       </c>
       <c r="D87" t="n">
-        <v>373112</v>
+        <v>1865091</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3667,12 +3735,12 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -3688,10 +3756,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>19</v>
+        <v>252</v>
       </c>
       <c r="D88" t="n">
-        <v>28402</v>
+        <v>376112</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3705,12 +3773,12 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -3726,10 +3794,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D89" t="n">
-        <v>6000</v>
+        <v>29902</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3743,12 +3811,12 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -3764,10 +3832,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4682</v>
+        <v>4</v>
       </c>
       <c r="D90" t="n">
-        <v>6321763</v>
+        <v>6000</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3781,12 +3849,12 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -3802,29 +3870,29 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1367</v>
+        <v>4704</v>
       </c>
       <c r="D91" t="n">
-        <v>1976158</v>
+        <v>6351787</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>04</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Martinique</t>
+          <t>La Réunion</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -3840,10 +3908,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>4508</v>
+        <v>1369</v>
       </c>
       <c r="D92" t="n">
-        <v>6642665</v>
+        <v>1978090</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3857,12 +3925,12 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -3878,10 +3946,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1749</v>
+        <v>4533</v>
       </c>
       <c r="D93" t="n">
-        <v>2608116</v>
+        <v>6679000</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3895,12 +3963,12 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -3916,10 +3984,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>614</v>
+        <v>1761</v>
       </c>
       <c r="D94" t="n">
-        <v>920141</v>
+        <v>2626116</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3933,12 +4001,12 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -3954,10 +4022,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>148</v>
+        <v>615</v>
       </c>
       <c r="D95" t="n">
-        <v>221569</v>
+        <v>921641</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3971,12 +4039,12 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -3992,10 +4060,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="D96" t="n">
-        <v>25500</v>
+        <v>223069</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4009,12 +4077,12 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -4030,10 +4098,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D97" t="n">
-        <v>7500</v>
+        <v>25500</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4047,12 +4115,12 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -4068,10 +4136,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>2967</v>
+        <v>5</v>
       </c>
       <c r="D98" t="n">
-        <v>3937313</v>
+        <v>7500</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4085,12 +4153,12 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -4106,29 +4174,29 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>508</v>
+        <v>2985</v>
       </c>
       <c r="D99" t="n">
-        <v>757464</v>
+        <v>3960717</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>02</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Mayotte</t>
+          <t>Martinique</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -4144,10 +4212,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>255</v>
+        <v>508</v>
       </c>
       <c r="D100" t="n">
-        <v>380765</v>
+        <v>757464</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4161,12 +4229,12 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -4182,10 +4250,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>84</v>
+        <v>255</v>
       </c>
       <c r="D101" t="n">
-        <v>126000</v>
+        <v>380765</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4199,12 +4267,12 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -4220,10 +4288,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="D102" t="n">
-        <v>55500</v>
+        <v>130500</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4237,12 +4305,12 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -4258,10 +4326,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D103" t="n">
-        <v>25500</v>
+        <v>55500</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4275,12 +4343,12 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -4296,29 +4364,29 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>9954</v>
+        <v>17</v>
       </c>
       <c r="D104" t="n">
-        <v>14468450</v>
+        <v>25500</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>06</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Normandie</t>
+          <t>Mayotte</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -4334,10 +4402,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>27532</v>
+        <v>9984</v>
       </c>
       <c r="D105" t="n">
-        <v>40492435</v>
+        <v>14510852</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4351,12 +4419,12 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -4372,10 +4440,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>9234</v>
+        <v>27624</v>
       </c>
       <c r="D106" t="n">
-        <v>13734660</v>
+        <v>40622727</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4389,12 +4457,12 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -4410,10 +4478,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>2506</v>
+        <v>9254</v>
       </c>
       <c r="D107" t="n">
-        <v>3736944</v>
+        <v>13764660</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4427,12 +4495,12 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -4448,10 +4516,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>419</v>
+        <v>2512</v>
       </c>
       <c r="D108" t="n">
-        <v>625982</v>
+        <v>3745410</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4465,12 +4533,12 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -4486,10 +4554,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>39</v>
+        <v>425</v>
       </c>
       <c r="D109" t="n">
-        <v>58500</v>
+        <v>634982</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4503,12 +4571,12 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -4524,10 +4592,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D110" t="n">
-        <v>9000</v>
+        <v>58500</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4541,12 +4609,12 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -4562,10 +4630,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>9075</v>
+        <v>6</v>
       </c>
       <c r="D111" t="n">
-        <v>12030486</v>
+        <v>9000</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4579,12 +4647,12 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -4600,29 +4668,29 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>28000</v>
+        <v>9091</v>
       </c>
       <c r="D112" t="n">
-        <v>40436915</v>
+        <v>12052206</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Nouvelle-Aquitaine</t>
+          <t>Normandie</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -4638,10 +4706,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>62041</v>
+        <v>28065</v>
       </c>
       <c r="D113" t="n">
-        <v>90908653</v>
+        <v>40525965</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4655,12 +4723,12 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -4676,10 +4744,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>20083</v>
+        <v>62190</v>
       </c>
       <c r="D114" t="n">
-        <v>29870074</v>
+        <v>91117616</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4693,12 +4761,12 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -4714,10 +4782,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>5608</v>
+        <v>20150</v>
       </c>
       <c r="D115" t="n">
-        <v>8360909</v>
+        <v>29967937</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4731,12 +4799,12 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -4752,10 +4820,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>986</v>
+        <v>5632</v>
       </c>
       <c r="D116" t="n">
-        <v>1474993</v>
+        <v>8396116</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4769,12 +4837,12 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -4790,10 +4858,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>56</v>
+        <v>995</v>
       </c>
       <c r="D117" t="n">
-        <v>81420</v>
+        <v>1488493</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4807,12 +4875,12 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -4828,10 +4896,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="D118" t="n">
-        <v>18000</v>
+        <v>82920</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4845,12 +4913,12 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -4866,10 +4934,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D119" t="n">
-        <v>6070</v>
+        <v>18000</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4883,12 +4951,12 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>100 à 199 salariés</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -4904,10 +4972,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>23839</v>
+        <v>5</v>
       </c>
       <c r="D120" t="n">
-        <v>31957087</v>
+        <v>6070</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -4921,12 +4989,12 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>100 à 199 salariés</t>
         </is>
       </c>
     </row>
@@ -4942,29 +5010,29 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>32578</v>
+        <v>23907</v>
       </c>
       <c r="D121" t="n">
-        <v>47094864</v>
+        <v>32042607</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>75</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Occitanie</t>
+          <t>Nouvelle-Aquitaine</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -4980,10 +5048,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>70984</v>
+        <v>32716</v>
       </c>
       <c r="D122" t="n">
-        <v>103950547</v>
+        <v>47284243</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -4997,12 +5065,12 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -5018,10 +5086,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>22206</v>
+        <v>71316</v>
       </c>
       <c r="D123" t="n">
-        <v>32981113</v>
+        <v>104419753</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5035,12 +5103,12 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -5056,10 +5124,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>5864</v>
+        <v>22318</v>
       </c>
       <c r="D124" t="n">
-        <v>8720966</v>
+        <v>33142440</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5073,12 +5141,12 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -5094,10 +5162,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1052</v>
+        <v>5893</v>
       </c>
       <c r="D125" t="n">
-        <v>1568269</v>
+        <v>8764044</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5111,12 +5179,12 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -5132,10 +5200,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>52</v>
+        <v>1059</v>
       </c>
       <c r="D126" t="n">
-        <v>76228</v>
+        <v>1578769</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5149,12 +5217,12 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -5170,10 +5238,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="D127" t="n">
-        <v>21000</v>
+        <v>76228</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5187,12 +5255,12 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -5208,10 +5276,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D128" t="n">
-        <v>2100</v>
+        <v>21000</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5225,12 +5293,12 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>250 à 499 salariés</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -5246,10 +5314,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>28860</v>
+        <v>3</v>
       </c>
       <c r="D129" t="n">
-        <v>38463338</v>
+        <v>2100</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5263,12 +5331,12 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>32</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>250 à 499 salariés</t>
         </is>
       </c>
     </row>
@@ -5284,29 +5352,29 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>12223</v>
+        <v>28965</v>
       </c>
       <c r="D130" t="n">
-        <v>17715005</v>
+        <v>38606008</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>76</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Pays de la Loire</t>
+          <t>Occitanie</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -5322,10 +5390,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>30474</v>
+        <v>12255</v>
       </c>
       <c r="D131" t="n">
-        <v>44803283</v>
+        <v>17759825</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5339,12 +5407,12 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -5360,10 +5428,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>10843</v>
+        <v>30553</v>
       </c>
       <c r="D132" t="n">
-        <v>16116895</v>
+        <v>44917872</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5377,12 +5445,12 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -5398,10 +5466,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>2729</v>
+        <v>10878</v>
       </c>
       <c r="D133" t="n">
-        <v>4071205</v>
+        <v>16168639</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5415,12 +5483,12 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -5436,10 +5504,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>429</v>
+        <v>2747</v>
       </c>
       <c r="D134" t="n">
-        <v>637490</v>
+        <v>4096791</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5453,12 +5521,12 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -5474,10 +5542,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>28</v>
+        <v>433</v>
       </c>
       <c r="D135" t="n">
-        <v>41964</v>
+        <v>643490</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5491,12 +5559,12 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -5512,10 +5580,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D136" t="n">
-        <v>12000</v>
+        <v>43464</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5529,12 +5597,12 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -5550,10 +5618,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>10057</v>
+        <v>8</v>
       </c>
       <c r="D137" t="n">
-        <v>13485979</v>
+        <v>12000</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5567,12 +5635,12 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>50 à 99 salariés</t>
         </is>
       </c>
     </row>
@@ -5588,29 +5656,29 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>31816</v>
+        <v>10089</v>
       </c>
       <c r="D138" t="n">
-        <v>45988698</v>
+        <v>13529653</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Provence-Alpes-Côte d'Azur</t>
+          <t>Pays de la Loire</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -5626,10 +5694,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>75204</v>
+        <v>31903</v>
       </c>
       <c r="D139" t="n">
-        <v>110273024</v>
+        <v>46114297</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5643,12 +5711,12 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -5664,10 +5732,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>22684</v>
+        <v>75427</v>
       </c>
       <c r="D140" t="n">
-        <v>33740545</v>
+        <v>110593859</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5681,12 +5749,12 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -5702,10 +5770,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>5844</v>
+        <v>22779</v>
       </c>
       <c r="D141" t="n">
-        <v>8724283</v>
+        <v>33878906</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5719,12 +5787,12 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -5740,10 +5808,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1242</v>
+        <v>5860</v>
       </c>
       <c r="D142" t="n">
-        <v>1851482</v>
+        <v>8747348</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5757,12 +5825,12 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -5778,10 +5846,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>65</v>
+        <v>1254</v>
       </c>
       <c r="D143" t="n">
-        <v>97130</v>
+        <v>1869482</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5795,12 +5863,12 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -5816,10 +5884,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D144" t="n">
-        <v>18000</v>
+        <v>100130</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5833,12 +5901,12 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -5854,10 +5922,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>26778</v>
+        <v>12</v>
       </c>
       <c r="D145" t="n">
-        <v>36306768</v>
+        <v>18000</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5871,10 +5939,48 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>50 à 99 salariés</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Fonds de solidarité</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>VOLET1</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>26857</v>
+      </c>
+      <c r="D146" t="n">
+        <v>36407400</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Provence-Alpes-Côte d'Azur</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
           <t>NN</t>
         </is>
       </c>
-      <c r="H145" t="inlineStr">
+      <c r="H146" t="inlineStr">
         <is>
           <t>Etablissement non employeur</t>
         </is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-07-21 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34835</v>
+        <v>35199</v>
       </c>
       <c r="D2" t="n">
-        <v>50453444</v>
+        <v>50977093</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>85403</v>
+        <v>86070</v>
       </c>
       <c r="D3" t="n">
-        <v>125351861</v>
+        <v>126325140</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>29297</v>
+        <v>29509</v>
       </c>
       <c r="D4" t="n">
-        <v>43430308</v>
+        <v>43739115</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>8064</v>
+        <v>8135</v>
       </c>
       <c r="D5" t="n">
-        <v>11990518</v>
+        <v>12097018</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1731</v>
+        <v>1752</v>
       </c>
       <c r="D6" t="n">
-        <v>2573596</v>
+        <v>2605096</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -610,10 +610,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D7" t="n">
-        <v>184093</v>
+        <v>191593</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>38266</v>
+        <v>38674</v>
       </c>
       <c r="D11" t="n">
-        <v>52064898</v>
+        <v>52612658</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8969</v>
+        <v>9078</v>
       </c>
       <c r="D12" t="n">
-        <v>12987230</v>
+        <v>13137536</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>24594</v>
+        <v>24790</v>
       </c>
       <c r="D13" t="n">
-        <v>36096298</v>
+        <v>36383432</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7845</v>
+        <v>7900</v>
       </c>
       <c r="D14" t="n">
-        <v>11653450</v>
+        <v>11734756</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1988</v>
+        <v>2011</v>
       </c>
       <c r="D15" t="n">
-        <v>2957476</v>
+        <v>2991976</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="D16" t="n">
-        <v>532123</v>
+        <v>547123</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" t="n">
-        <v>42000</v>
+        <v>43500</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>9498</v>
+        <v>9584</v>
       </c>
       <c r="D19" t="n">
-        <v>12628286</v>
+        <v>12735739</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>12529</v>
+        <v>12657</v>
       </c>
       <c r="D20" t="n">
-        <v>18105522</v>
+        <v>18290338</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>30017</v>
+        <v>30278</v>
       </c>
       <c r="D21" t="n">
-        <v>44105912</v>
+        <v>44486054</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>9742</v>
+        <v>9809</v>
       </c>
       <c r="D22" t="n">
-        <v>14489310</v>
+        <v>14588251</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2469</v>
+        <v>2482</v>
       </c>
       <c r="D23" t="n">
-        <v>3673763</v>
+        <v>3693263</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>432</v>
+        <v>443</v>
       </c>
       <c r="D24" t="n">
-        <v>642345</v>
+        <v>658845</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D25" t="n">
-        <v>41453</v>
+        <v>42953</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1332,10 +1332,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>10947</v>
+        <v>11047</v>
       </c>
       <c r="D26" t="n">
-        <v>14688423</v>
+        <v>14815702</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>7127</v>
+        <v>7209</v>
       </c>
       <c r="D27" t="n">
-        <v>10332123</v>
+        <v>10449697</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>21254</v>
+        <v>21416</v>
       </c>
       <c r="D28" t="n">
-        <v>31227892</v>
+        <v>31456789</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>7390</v>
+        <v>7452</v>
       </c>
       <c r="D29" t="n">
-        <v>11000651</v>
+        <v>11092709</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1821</v>
+        <v>1839</v>
       </c>
       <c r="D30" t="n">
-        <v>2719986</v>
+        <v>2746986</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D31" t="n">
-        <v>444415</v>
+        <v>448915</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D32" t="n">
-        <v>37393</v>
+        <v>38893</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>7739</v>
+        <v>7844</v>
       </c>
       <c r="D33" t="n">
-        <v>10262641</v>
+        <v>10398358</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2778</v>
+        <v>2831</v>
       </c>
       <c r="D34" t="n">
-        <v>4007836</v>
+        <v>4083581</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>7000</v>
+        <v>7095</v>
       </c>
       <c r="D35" t="n">
-        <v>10230347</v>
+        <v>10370149</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2838</v>
+        <v>2873</v>
       </c>
       <c r="D36" t="n">
-        <v>4202023</v>
+        <v>4253788</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="D37" t="n">
-        <v>1137263</v>
+        <v>1143263</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2159</v>
+        <v>2190</v>
       </c>
       <c r="D40" t="n">
-        <v>2911166</v>
+        <v>2952114</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>16058</v>
+        <v>16221</v>
       </c>
       <c r="D41" t="n">
-        <v>23241051</v>
+        <v>23476842</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>48231</v>
+        <v>48573</v>
       </c>
       <c r="D42" t="n">
-        <v>70766433</v>
+        <v>71264361</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1978,10 +1978,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>18067</v>
+        <v>18156</v>
       </c>
       <c r="D43" t="n">
-        <v>26843123</v>
+        <v>26975421</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5243</v>
+        <v>5270</v>
       </c>
       <c r="D44" t="n">
-        <v>7815108</v>
+        <v>7852784</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1039</v>
+        <v>1054</v>
       </c>
       <c r="D45" t="n">
-        <v>1549719</v>
+        <v>1572219</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D46" t="n">
-        <v>77191</v>
+        <v>80191</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>15507</v>
+        <v>15681</v>
       </c>
       <c r="D49" t="n">
-        <v>20715479</v>
+        <v>20939342</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1682</v>
+        <v>1731</v>
       </c>
       <c r="D50" t="n">
-        <v>2440833</v>
+        <v>2513982</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>5976</v>
+        <v>6137</v>
       </c>
       <c r="D51" t="n">
-        <v>8799326</v>
+        <v>9033194</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2090</v>
+        <v>2120</v>
       </c>
       <c r="D52" t="n">
-        <v>3121750</v>
+        <v>3166750</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>683</v>
+        <v>698</v>
       </c>
       <c r="D53" t="n">
-        <v>1019805</v>
+        <v>1042305</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D54" t="n">
-        <v>227111</v>
+        <v>239111</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5483</v>
+        <v>5628</v>
       </c>
       <c r="D56" t="n">
-        <v>7572623</v>
+        <v>7772522</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>690</v>
+        <v>714</v>
       </c>
       <c r="D57" t="n">
-        <v>1011340</v>
+        <v>1046540</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1743</v>
+        <v>1819</v>
       </c>
       <c r="D58" t="n">
-        <v>2582914</v>
+        <v>2696626</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>695</v>
+        <v>733</v>
       </c>
       <c r="D59" t="n">
-        <v>1036719</v>
+        <v>1091953</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D60" t="n">
-        <v>356758</v>
+        <v>379258</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D61" t="n">
-        <v>76500</v>
+        <v>81000</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D62" t="n">
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1008</v>
+        <v>1058</v>
       </c>
       <c r="D63" t="n">
-        <v>1429765</v>
+        <v>1501861</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>14297</v>
+        <v>14442</v>
       </c>
       <c r="D64" t="n">
-        <v>20669944</v>
+        <v>20877295</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>42359</v>
+        <v>42678</v>
       </c>
       <c r="D65" t="n">
-        <v>62036210</v>
+        <v>62497519</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>14950</v>
+        <v>15043</v>
       </c>
       <c r="D66" t="n">
-        <v>22230375</v>
+        <v>22368115</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4298</v>
+        <v>4343</v>
       </c>
       <c r="D67" t="n">
-        <v>6403793</v>
+        <v>6468716</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>829</v>
+        <v>842</v>
       </c>
       <c r="D68" t="n">
-        <v>1234273</v>
+        <v>1252596</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D69" t="n">
-        <v>99189</v>
+        <v>100689</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>14184</v>
+        <v>14311</v>
       </c>
       <c r="D71" t="n">
-        <v>18782082</v>
+        <v>18943167</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>45574</v>
+        <v>46677</v>
       </c>
       <c r="D72" t="n">
-        <v>66353129</v>
+        <v>67968779</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>132349</v>
+        <v>134630</v>
       </c>
       <c r="D73" t="n">
-        <v>195116962</v>
+        <v>198482495</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>58244</v>
+        <v>58945</v>
       </c>
       <c r="D74" t="n">
-        <v>86820399</v>
+        <v>87865801</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>18482</v>
+        <v>18711</v>
       </c>
       <c r="D75" t="n">
-        <v>27620072</v>
+        <v>27962419</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>4121</v>
+        <v>4203</v>
       </c>
       <c r="D76" t="n">
-        <v>6158120</v>
+        <v>6281120</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="D77" t="n">
-        <v>319170</v>
+        <v>334170</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D78" t="n">
-        <v>24405</v>
+        <v>25905</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D81" t="n">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>45042</v>
+        <v>46135</v>
       </c>
       <c r="D83" t="n">
-        <v>61630269</v>
+        <v>63103026</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>4082</v>
+        <v>4170</v>
       </c>
       <c r="D84" t="n">
-        <v>5920669</v>
+        <v>6047631</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>10585</v>
+        <v>10740</v>
       </c>
       <c r="D85" t="n">
-        <v>15559960</v>
+        <v>15786309</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>3624</v>
+        <v>3667</v>
       </c>
       <c r="D86" t="n">
-        <v>5402081</v>
+        <v>5465993</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>1261</v>
+        <v>1274</v>
       </c>
       <c r="D87" t="n">
-        <v>1886091</v>
+        <v>1904913</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D88" t="n">
-        <v>386612</v>
+        <v>393512</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4747</v>
+        <v>4838</v>
       </c>
       <c r="D91" t="n">
-        <v>6405537</v>
+        <v>6523494</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1385</v>
+        <v>1426</v>
       </c>
       <c r="D92" t="n">
-        <v>2001990</v>
+        <v>2062583</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4588</v>
+        <v>4684</v>
       </c>
       <c r="D93" t="n">
-        <v>6761465</v>
+        <v>6901416</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1778</v>
+        <v>1803</v>
       </c>
       <c r="D94" t="n">
-        <v>2651616</v>
+        <v>2688403</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>624</v>
+        <v>641</v>
       </c>
       <c r="D95" t="n">
-        <v>935141</v>
+        <v>960641</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D96" t="n">
-        <v>232069</v>
+        <v>237613</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D98" t="n">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>3041</v>
+        <v>3106</v>
       </c>
       <c r="D99" t="n">
-        <v>4037232</v>
+        <v>4121729</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="D100" t="n">
-        <v>770964</v>
+        <v>788964</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="D101" t="n">
-        <v>397265</v>
+        <v>412165</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D102" t="n">
-        <v>138000</v>
+        <v>139500</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D103" t="n">
-        <v>55500</v>
+        <v>57000</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D104" t="n">
-        <v>25500</v>
+        <v>27000</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>10043</v>
+        <v>10168</v>
       </c>
       <c r="D105" t="n">
-        <v>14593858</v>
+        <v>14773994</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>27756</v>
+        <v>27984</v>
       </c>
       <c r="D106" t="n">
-        <v>40808961</v>
+        <v>41136250</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>9304</v>
+        <v>9363</v>
       </c>
       <c r="D107" t="n">
-        <v>13839476</v>
+        <v>13925548</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>2530</v>
+        <v>2549</v>
       </c>
       <c r="D108" t="n">
-        <v>3772410</v>
+        <v>3800910</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="D109" t="n">
-        <v>645482</v>
+        <v>652982</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>9150</v>
+        <v>9247</v>
       </c>
       <c r="D112" t="n">
-        <v>12129717</v>
+        <v>12258927</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>28202</v>
+        <v>28576</v>
       </c>
       <c r="D113" t="n">
-        <v>40715452</v>
+        <v>41249120</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>62522</v>
+        <v>63029</v>
       </c>
       <c r="D114" t="n">
-        <v>91579750</v>
+        <v>92320248</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>20271</v>
+        <v>20421</v>
       </c>
       <c r="D115" t="n">
-        <v>30140526</v>
+        <v>30363779</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>5671</v>
+        <v>5721</v>
       </c>
       <c r="D116" t="n">
-        <v>8453861</v>
+        <v>8527458</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1014</v>
+        <v>1023</v>
       </c>
       <c r="D117" t="n">
-        <v>1516993</v>
+        <v>1530493</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D118" t="n">
-        <v>85920</v>
+        <v>87420</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4942,10 +4942,10 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>24047</v>
+        <v>24352</v>
       </c>
       <c r="D121" t="n">
-        <v>32215789</v>
+        <v>32605179</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>32874</v>
+        <v>33305</v>
       </c>
       <c r="D122" t="n">
-        <v>47502784</v>
+        <v>48132950</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>71695</v>
+        <v>72348</v>
       </c>
       <c r="D123" t="n">
-        <v>104952007</v>
+        <v>105902791</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>22444</v>
+        <v>22589</v>
       </c>
       <c r="D124" t="n">
-        <v>33325154</v>
+        <v>33540084</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>5930</v>
+        <v>5976</v>
       </c>
       <c r="D125" t="n">
-        <v>8818054</v>
+        <v>8885761</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1081</v>
+        <v>1094</v>
       </c>
       <c r="D126" t="n">
-        <v>1610551</v>
+        <v>1627646</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>29157</v>
+        <v>29463</v>
       </c>
       <c r="D130" t="n">
-        <v>38850427</v>
+        <v>39244320</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5322,10 +5322,10 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>12319</v>
+        <v>12475</v>
       </c>
       <c r="D131" t="n">
-        <v>17844177</v>
+        <v>18070229</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>30669</v>
+        <v>30903</v>
       </c>
       <c r="D132" t="n">
-        <v>45079415</v>
+        <v>45422752</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>10932</v>
+        <v>11010</v>
       </c>
       <c r="D133" t="n">
-        <v>16244690</v>
+        <v>16361344</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>2759</v>
+        <v>2771</v>
       </c>
       <c r="D134" t="n">
-        <v>4114791</v>
+        <v>4132791</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="D135" t="n">
-        <v>652490</v>
+        <v>661490</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>10131</v>
+        <v>10226</v>
       </c>
       <c r="D138" t="n">
-        <v>13572831</v>
+        <v>13695035</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>32128</v>
+        <v>32557</v>
       </c>
       <c r="D139" t="n">
-        <v>46433342</v>
+        <v>47058800</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5664,10 +5664,10 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>75922</v>
+        <v>76638</v>
       </c>
       <c r="D140" t="n">
-        <v>111305711</v>
+        <v>112359980</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>22915</v>
+        <v>23079</v>
       </c>
       <c r="D141" t="n">
-        <v>34076653</v>
+        <v>34314224</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>5905</v>
+        <v>5963</v>
       </c>
       <c r="D142" t="n">
-        <v>8814848</v>
+        <v>8900822</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1277</v>
+        <v>1296</v>
       </c>
       <c r="D143" t="n">
-        <v>1902186</v>
+        <v>1930686</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D144" t="n">
-        <v>101630</v>
+        <v>103130</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>27034</v>
+        <v>27344</v>
       </c>
       <c r="D146" t="n">
-        <v>36639603</v>
+        <v>37047653</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-13 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>39169</v>
+        <v>39427</v>
       </c>
       <c r="D2" t="n">
-        <v>56622841</v>
+        <v>56990721</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>93827</v>
+        <v>94365</v>
       </c>
       <c r="D3" t="n">
-        <v>137518939</v>
+        <v>138299236</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>31991</v>
+        <v>32179</v>
       </c>
       <c r="D4" t="n">
-        <v>47369138</v>
+        <v>47642976</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9012</v>
+        <v>9071</v>
       </c>
       <c r="D5" t="n">
-        <v>13394746</v>
+        <v>13481753</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2106</v>
+        <v>2134</v>
       </c>
       <c r="D6" t="n">
-        <v>3130971</v>
+        <v>3172971</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -610,10 +610,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D7" t="n">
-        <v>257593</v>
+        <v>266593</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>42553</v>
+        <v>42803</v>
       </c>
       <c r="D12" t="n">
-        <v>57678152</v>
+        <v>58009257</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>9998</v>
+        <v>10052</v>
       </c>
       <c r="D13" t="n">
-        <v>14450961</v>
+        <v>14527718</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>26661</v>
+        <v>26794</v>
       </c>
       <c r="D14" t="n">
-        <v>39082404</v>
+        <v>39274530</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8505</v>
+        <v>8555</v>
       </c>
       <c r="D15" t="n">
-        <v>12622978</v>
+        <v>12696643</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2222</v>
+        <v>2234</v>
       </c>
       <c r="D16" t="n">
-        <v>3301539</v>
+        <v>3318849</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="D17" t="n">
-        <v>638623</v>
+        <v>647623</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18" t="n">
-        <v>55500</v>
+        <v>57000</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>10469</v>
+        <v>10531</v>
       </c>
       <c r="D20" t="n">
-        <v>13843198</v>
+        <v>13911985</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>13803</v>
+        <v>13881</v>
       </c>
       <c r="D21" t="n">
-        <v>19916328</v>
+        <v>20022026</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>32442</v>
+        <v>32600</v>
       </c>
       <c r="D22" t="n">
-        <v>47592718</v>
+        <v>47821836</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>10478</v>
+        <v>10526</v>
       </c>
       <c r="D23" t="n">
-        <v>15572869</v>
+        <v>15643646</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2716</v>
+        <v>2738</v>
       </c>
       <c r="D24" t="n">
-        <v>4038771</v>
+        <v>4071674</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="D25" t="n">
-        <v>822092</v>
+        <v>828092</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1332,10 +1332,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D26" t="n">
-        <v>54953</v>
+        <v>57953</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>11983</v>
+        <v>12054</v>
       </c>
       <c r="D27" t="n">
-        <v>15988915</v>
+        <v>16072402</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>7937</v>
+        <v>7998</v>
       </c>
       <c r="D28" t="n">
-        <v>11485752</v>
+        <v>11573884</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>23163</v>
+        <v>23284</v>
       </c>
       <c r="D29" t="n">
-        <v>33998287</v>
+        <v>34173049</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>7988</v>
+        <v>8024</v>
       </c>
       <c r="D30" t="n">
-        <v>11880892</v>
+        <v>11930241</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2030</v>
+        <v>2038</v>
       </c>
       <c r="D31" t="n">
-        <v>3029251</v>
+        <v>3041251</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D32" t="n">
-        <v>568915</v>
+        <v>570415</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8544</v>
+        <v>8597</v>
       </c>
       <c r="D34" t="n">
-        <v>11282927</v>
+        <v>11355038</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3386</v>
+        <v>3411</v>
       </c>
       <c r="D35" t="n">
-        <v>4889638</v>
+        <v>4925201</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>8089</v>
+        <v>8173</v>
       </c>
       <c r="D36" t="n">
-        <v>11815436</v>
+        <v>11939222</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3250</v>
+        <v>3263</v>
       </c>
       <c r="D37" t="n">
-        <v>4817961</v>
+        <v>4837461</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="D38" t="n">
-        <v>1254055</v>
+        <v>1258555</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2551</v>
+        <v>2574</v>
       </c>
       <c r="D41" t="n">
-        <v>3447067</v>
+        <v>3478381</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>17874</v>
+        <v>17968</v>
       </c>
       <c r="D42" t="n">
-        <v>25836666</v>
+        <v>25965762</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1978,10 +1978,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>52570</v>
+        <v>52808</v>
       </c>
       <c r="D43" t="n">
-        <v>77046509</v>
+        <v>77387689</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>19405</v>
+        <v>19467</v>
       </c>
       <c r="D44" t="n">
-        <v>28814623</v>
+        <v>28904864</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5784</v>
+        <v>5815</v>
       </c>
       <c r="D45" t="n">
-        <v>8608590</v>
+        <v>8654435</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1273</v>
+        <v>1289</v>
       </c>
       <c r="D46" t="n">
-        <v>1900045</v>
+        <v>1923144</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D47" t="n">
-        <v>101568</v>
+        <v>103068</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>17246</v>
+        <v>17335</v>
       </c>
       <c r="D50" t="n">
-        <v>22902417</v>
+        <v>23011303</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2171</v>
+        <v>2196</v>
       </c>
       <c r="D51" t="n">
-        <v>3151376</v>
+        <v>3188096</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7331</v>
+        <v>7399</v>
       </c>
       <c r="D52" t="n">
-        <v>10771031</v>
+        <v>10872534</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2455</v>
+        <v>2471</v>
       </c>
       <c r="D53" t="n">
-        <v>3666572</v>
+        <v>3688644</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="D54" t="n">
-        <v>1160415</v>
+        <v>1163415</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D55" t="n">
-        <v>299226</v>
+        <v>302226</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>7430</v>
+        <v>7487</v>
       </c>
       <c r="D57" t="n">
-        <v>10218337</v>
+        <v>10296246</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1241</v>
+        <v>1294</v>
       </c>
       <c r="D58" t="n">
-        <v>2179084</v>
+        <v>2323507</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3024</v>
+        <v>3160</v>
       </c>
       <c r="D59" t="n">
-        <v>5289247</v>
+        <v>5665955</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1193</v>
+        <v>1258</v>
       </c>
       <c r="D60" t="n">
-        <v>2094053</v>
+        <v>2275566</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="D61" t="n">
-        <v>710383</v>
+        <v>747083</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D62" t="n">
-        <v>238100</v>
+        <v>265100</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1822</v>
+        <v>1933</v>
       </c>
       <c r="D64" t="n">
-        <v>2946722</v>
+        <v>3205583</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>15962</v>
+        <v>16076</v>
       </c>
       <c r="D65" t="n">
-        <v>23053147</v>
+        <v>23218312</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>46073</v>
+        <v>46326</v>
       </c>
       <c r="D66" t="n">
-        <v>67395157</v>
+        <v>67755484</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>16080</v>
+        <v>16172</v>
       </c>
       <c r="D67" t="n">
-        <v>23891544</v>
+        <v>24027361</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4688</v>
+        <v>4730</v>
       </c>
       <c r="D68" t="n">
-        <v>6981788</v>
+        <v>7044788</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>978</v>
+        <v>992</v>
       </c>
       <c r="D69" t="n">
-        <v>1453802</v>
+        <v>1474802</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>15508</v>
+        <v>15586</v>
       </c>
       <c r="D73" t="n">
-        <v>20418869</v>
+        <v>20510197</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>55670</v>
+        <v>56359</v>
       </c>
       <c r="D74" t="n">
-        <v>80993514</v>
+        <v>81971960</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>154858</v>
+        <v>156406</v>
       </c>
       <c r="D75" t="n">
-        <v>228090490</v>
+        <v>230344491</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>66551</v>
+        <v>67144</v>
       </c>
       <c r="D76" t="n">
-        <v>99151049</v>
+        <v>100025650</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>21358</v>
+        <v>21573</v>
       </c>
       <c r="D77" t="n">
-        <v>31912922</v>
+        <v>32232013</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>5132</v>
+        <v>5202</v>
       </c>
       <c r="D78" t="n">
-        <v>7666403</v>
+        <v>7771348</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="D79" t="n">
-        <v>439170</v>
+        <v>452670</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D80" t="n">
-        <v>34905</v>
+        <v>39405</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>54510</v>
+        <v>55128</v>
       </c>
       <c r="D85" t="n">
-        <v>73999555</v>
+        <v>74784341</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4812</v>
+        <v>4849</v>
       </c>
       <c r="D86" t="n">
-        <v>6971864</v>
+        <v>7027173</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>11965</v>
+        <v>12026</v>
       </c>
       <c r="D87" t="n">
-        <v>17574645</v>
+        <v>17665491</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>3985</v>
+        <v>3998</v>
       </c>
       <c r="D88" t="n">
-        <v>5937458</v>
+        <v>5956958</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1382</v>
+        <v>1384</v>
       </c>
       <c r="D89" t="n">
-        <v>2064111</v>
+        <v>2067111</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D90" t="n">
-        <v>446012</v>
+        <v>453512</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>5604</v>
+        <v>5638</v>
       </c>
       <c r="D93" t="n">
-        <v>7529970</v>
+        <v>7573062</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1675</v>
+        <v>1690</v>
       </c>
       <c r="D94" t="n">
-        <v>2414699</v>
+        <v>2436567</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>5400</v>
+        <v>5454</v>
       </c>
       <c r="D95" t="n">
-        <v>7956250</v>
+        <v>8036497</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2001</v>
+        <v>2012</v>
       </c>
       <c r="D96" t="n">
-        <v>2979426</v>
+        <v>2994808</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>713</v>
+        <v>725</v>
       </c>
       <c r="D97" t="n">
-        <v>1068460</v>
+        <v>1086460</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D98" t="n">
-        <v>302113</v>
+        <v>305113</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D99" t="n">
-        <v>28500</v>
+        <v>31500</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3729</v>
+        <v>3750</v>
       </c>
       <c r="D101" t="n">
-        <v>4942658</v>
+        <v>4971238</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>760</v>
+        <v>781</v>
       </c>
       <c r="D102" t="n">
-        <v>1322525</v>
+        <v>1380245</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="D103" t="n">
-        <v>852727</v>
+        <v>885004</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="D104" t="n">
-        <v>306180</v>
+        <v>339789</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4334,10 +4334,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D105" t="n">
-        <v>105000</v>
+        <v>112500</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>11180</v>
+        <v>11277</v>
       </c>
       <c r="D107" t="n">
-        <v>16211131</v>
+        <v>16353792</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>29944</v>
+        <v>30099</v>
       </c>
       <c r="D108" t="n">
-        <v>43972354</v>
+        <v>44197846</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>10034</v>
+        <v>10082</v>
       </c>
       <c r="D109" t="n">
-        <v>14916726</v>
+        <v>14988726</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>2768</v>
+        <v>2776</v>
       </c>
       <c r="D110" t="n">
-        <v>4127080</v>
+        <v>4139080</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="D111" t="n">
-        <v>758546</v>
+        <v>764546</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D112" t="n">
-        <v>87000</v>
+        <v>90000</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>10068</v>
+        <v>10116</v>
       </c>
       <c r="D114" t="n">
-        <v>13284109</v>
+        <v>13338540</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>31488</v>
+        <v>31713</v>
       </c>
       <c r="D115" t="n">
-        <v>45386787</v>
+        <v>45710108</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>67933</v>
+        <v>68291</v>
       </c>
       <c r="D116" t="n">
-        <v>99390441</v>
+        <v>99914945</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>21847</v>
+        <v>21937</v>
       </c>
       <c r="D117" t="n">
-        <v>32460828</v>
+        <v>32593375</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>6213</v>
+        <v>6240</v>
       </c>
       <c r="D118" t="n">
-        <v>9254799</v>
+        <v>9295299</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1174</v>
+        <v>1184</v>
       </c>
       <c r="D119" t="n">
-        <v>1754465</v>
+        <v>1768889</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4904,10 +4904,10 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D120" t="n">
-        <v>126895</v>
+        <v>132895</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>26497</v>
+        <v>26627</v>
       </c>
       <c r="D124" t="n">
-        <v>35356461</v>
+        <v>35524574</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>37361</v>
+        <v>37625</v>
       </c>
       <c r="D125" t="n">
-        <v>53908036</v>
+        <v>54277488</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>79173</v>
+        <v>79598</v>
       </c>
       <c r="D126" t="n">
-        <v>115744948</v>
+        <v>116363478</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>24463</v>
+        <v>24595</v>
       </c>
       <c r="D127" t="n">
-        <v>36307847</v>
+        <v>36502859</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>6566</v>
+        <v>6598</v>
       </c>
       <c r="D128" t="n">
-        <v>9757623</v>
+        <v>9805623</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1316</v>
+        <v>1324</v>
       </c>
       <c r="D129" t="n">
-        <v>1957311</v>
+        <v>1969311</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D130" t="n">
-        <v>98728</v>
+        <v>103228</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>32669</v>
+        <v>32876</v>
       </c>
       <c r="D133" t="n">
-        <v>43359448</v>
+        <v>43622567</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>13745</v>
+        <v>13835</v>
       </c>
       <c r="D134" t="n">
-        <v>19897615</v>
+        <v>20027193</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>33212</v>
+        <v>33398</v>
       </c>
       <c r="D135" t="n">
-        <v>48771376</v>
+        <v>49042832</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>11744</v>
+        <v>11791</v>
       </c>
       <c r="D136" t="n">
-        <v>17449316</v>
+        <v>17519816</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>3056</v>
+        <v>3085</v>
       </c>
       <c r="D137" t="n">
-        <v>4555241</v>
+        <v>4598741</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="D138" t="n">
-        <v>773990</v>
+        <v>778490</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D139" t="n">
-        <v>54325</v>
+        <v>58825</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>11107</v>
+        <v>11161</v>
       </c>
       <c r="D141" t="n">
-        <v>14804113</v>
+        <v>14869749</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>36524</v>
+        <v>36780</v>
       </c>
       <c r="D142" t="n">
-        <v>52752943</v>
+        <v>53119939</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>84150</v>
+        <v>84670</v>
       </c>
       <c r="D143" t="n">
-        <v>123275408</v>
+        <v>124037636</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>25048</v>
+        <v>25177</v>
       </c>
       <c r="D144" t="n">
-        <v>37212458</v>
+        <v>37403613</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>6574</v>
+        <v>6624</v>
       </c>
       <c r="D145" t="n">
-        <v>9809496</v>
+        <v>9884496</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1499</v>
+        <v>1508</v>
       </c>
       <c r="D146" t="n">
-        <v>2230730</v>
+        <v>2244230</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>30085</v>
+        <v>30279</v>
       </c>
       <c r="D149" t="n">
-        <v>40549891</v>
+        <v>40800310</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-27 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>39832</v>
+        <v>39945</v>
       </c>
       <c r="D2" t="n">
-        <v>57545277</v>
+        <v>57709072</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>95204</v>
+        <v>95463</v>
       </c>
       <c r="D3" t="n">
-        <v>139510276</v>
+        <v>139875268</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>32454</v>
+        <v>32518</v>
       </c>
       <c r="D4" t="n">
-        <v>48045053</v>
+        <v>48139554</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9172</v>
+        <v>9204</v>
       </c>
       <c r="D5" t="n">
-        <v>13629008</v>
+        <v>13674869</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2170</v>
+        <v>2187</v>
       </c>
       <c r="D6" t="n">
-        <v>3223148</v>
+        <v>3248648</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -610,10 +610,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D7" t="n">
-        <v>289093</v>
+        <v>293593</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>43192</v>
+        <v>43291</v>
       </c>
       <c r="D12" t="n">
-        <v>58532014</v>
+        <v>58659852</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10132</v>
+        <v>10153</v>
       </c>
       <c r="D13" t="n">
-        <v>14641111</v>
+        <v>14669907</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>26998</v>
+        <v>27053</v>
       </c>
       <c r="D14" t="n">
-        <v>39569623</v>
+        <v>39649723</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8603</v>
+        <v>8618</v>
       </c>
       <c r="D15" t="n">
-        <v>12767484</v>
+        <v>12789365</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2262</v>
+        <v>2271</v>
       </c>
       <c r="D16" t="n">
-        <v>3360653</v>
+        <v>3374153</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>10632</v>
+        <v>10657</v>
       </c>
       <c r="D20" t="n">
-        <v>14039159</v>
+        <v>14065857</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>13991</v>
+        <v>14025</v>
       </c>
       <c r="D21" t="n">
-        <v>20181922</v>
+        <v>20229835</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>32853</v>
+        <v>32904</v>
       </c>
       <c r="D22" t="n">
-        <v>48185134</v>
+        <v>48257367</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>10583</v>
+        <v>10604</v>
       </c>
       <c r="D23" t="n">
-        <v>15727732</v>
+        <v>15759232</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2757</v>
+        <v>2765</v>
       </c>
       <c r="D24" t="n">
-        <v>4100174</v>
+        <v>4112174</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D25" t="n">
-        <v>841592</v>
+        <v>843092</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>12152</v>
+        <v>12171</v>
       </c>
       <c r="D27" t="n">
-        <v>16191909</v>
+        <v>16213937</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>8087</v>
+        <v>8109</v>
       </c>
       <c r="D28" t="n">
-        <v>11695234</v>
+        <v>11727701</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>23479</v>
+        <v>23513</v>
       </c>
       <c r="D29" t="n">
-        <v>34452892</v>
+        <v>34503428</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8082</v>
+        <v>8100</v>
       </c>
       <c r="D30" t="n">
-        <v>12015633</v>
+        <v>12042633</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2045</v>
+        <v>2049</v>
       </c>
       <c r="D31" t="n">
-        <v>3050699</v>
+        <v>3056699</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D32" t="n">
-        <v>579415</v>
+        <v>582415</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8681</v>
+        <v>8701</v>
       </c>
       <c r="D34" t="n">
-        <v>11461889</v>
+        <v>11488796</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3463</v>
+        <v>3485</v>
       </c>
       <c r="D35" t="n">
-        <v>4998597</v>
+        <v>5029994</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>8244</v>
+        <v>8268</v>
       </c>
       <c r="D36" t="n">
-        <v>12043599</v>
+        <v>12077662</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3294</v>
+        <v>3302</v>
       </c>
       <c r="D37" t="n">
-        <v>4883961</v>
+        <v>4895961</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D38" t="n">
-        <v>1267555</v>
+        <v>1269055</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2612</v>
+        <v>2625</v>
       </c>
       <c r="D41" t="n">
-        <v>3530263</v>
+        <v>3544328</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>18128</v>
+        <v>18174</v>
       </c>
       <c r="D42" t="n">
-        <v>26186802</v>
+        <v>26249614</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1978,10 +1978,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>53205</v>
+        <v>53328</v>
       </c>
       <c r="D43" t="n">
-        <v>77961024</v>
+        <v>78139631</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>19576</v>
+        <v>19625</v>
       </c>
       <c r="D44" t="n">
-        <v>29066453</v>
+        <v>29136980</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5856</v>
+        <v>5874</v>
       </c>
       <c r="D45" t="n">
-        <v>8715935</v>
+        <v>8742935</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1310</v>
+        <v>1322</v>
       </c>
       <c r="D46" t="n">
-        <v>1954644</v>
+        <v>1972644</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D47" t="n">
-        <v>109015</v>
+        <v>112015</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>17532</v>
+        <v>17582</v>
       </c>
       <c r="D50" t="n">
-        <v>23257227</v>
+        <v>23322312</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2232</v>
+        <v>2241</v>
       </c>
       <c r="D51" t="n">
-        <v>3238783</v>
+        <v>3251962</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7511</v>
+        <v>7545</v>
       </c>
       <c r="D52" t="n">
-        <v>11035971</v>
+        <v>11086912</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2499</v>
+        <v>2520</v>
       </c>
       <c r="D53" t="n">
-        <v>3730184</v>
+        <v>3761684</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>787</v>
+        <v>795</v>
       </c>
       <c r="D54" t="n">
-        <v>1175415</v>
+        <v>1187415</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>7595</v>
+        <v>7627</v>
       </c>
       <c r="D57" t="n">
-        <v>10446671</v>
+        <v>10491587</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1358</v>
+        <v>1377</v>
       </c>
       <c r="D58" t="n">
-        <v>2494131</v>
+        <v>2545508</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3329</v>
+        <v>3378</v>
       </c>
       <c r="D59" t="n">
-        <v>6128590</v>
+        <v>6263463</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1316</v>
+        <v>1329</v>
       </c>
       <c r="D60" t="n">
-        <v>2433866</v>
+        <v>2466462</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="D61" t="n">
-        <v>816083</v>
+        <v>831083</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D62" t="n">
-        <v>287600</v>
+        <v>299600</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2046</v>
+        <v>2089</v>
       </c>
       <c r="D64" t="n">
-        <v>3467520</v>
+        <v>3567660</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>16245</v>
+        <v>16280</v>
       </c>
       <c r="D65" t="n">
-        <v>23454417</v>
+        <v>23502456</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>46718</v>
+        <v>46826</v>
       </c>
       <c r="D66" t="n">
-        <v>68315298</v>
+        <v>68469913</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>16304</v>
+        <v>16345</v>
       </c>
       <c r="D67" t="n">
-        <v>24223549</v>
+        <v>24285049</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4758</v>
+        <v>4773</v>
       </c>
       <c r="D68" t="n">
-        <v>7086788</v>
+        <v>7109288</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>15683</v>
+        <v>15706</v>
       </c>
       <c r="D73" t="n">
-        <v>20619162</v>
+        <v>20648742</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>57433</v>
+        <v>57706</v>
       </c>
       <c r="D74" t="n">
-        <v>83521746</v>
+        <v>83914689</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>158993</v>
+        <v>159686</v>
       </c>
       <c r="D75" t="n">
-        <v>234091497</v>
+        <v>235102433</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>68186</v>
+        <v>68475</v>
       </c>
       <c r="D76" t="n">
-        <v>101571719</v>
+        <v>102001330</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>21973</v>
+        <v>22085</v>
       </c>
       <c r="D77" t="n">
-        <v>32832013</v>
+        <v>32999453</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>5328</v>
+        <v>5369</v>
       </c>
       <c r="D78" t="n">
-        <v>7958102</v>
+        <v>8019602</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>330</v>
+        <v>347</v>
       </c>
       <c r="D79" t="n">
-        <v>490170</v>
+        <v>515670</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>56445</v>
+        <v>56787</v>
       </c>
       <c r="D85" t="n">
-        <v>76438914</v>
+        <v>76866280</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4916</v>
+        <v>4926</v>
       </c>
       <c r="D86" t="n">
-        <v>7123839</v>
+        <v>7138689</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>12187</v>
+        <v>12210</v>
       </c>
       <c r="D87" t="n">
-        <v>17900881</v>
+        <v>17933935</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4031</v>
+        <v>4032</v>
       </c>
       <c r="D88" t="n">
-        <v>6006458</v>
+        <v>6007958</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1398</v>
+        <v>1402</v>
       </c>
       <c r="D89" t="n">
-        <v>2088111</v>
+        <v>2094111</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="D90" t="n">
-        <v>465512</v>
+        <v>473512</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>5703</v>
+        <v>5722</v>
       </c>
       <c r="D93" t="n">
-        <v>7660268</v>
+        <v>7680595</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1716</v>
+        <v>1720</v>
       </c>
       <c r="D94" t="n">
-        <v>2473136</v>
+        <v>2479136</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>5539</v>
+        <v>5557</v>
       </c>
       <c r="D95" t="n">
-        <v>8160504</v>
+        <v>8187317</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="D96" t="n">
-        <v>3020308</v>
+        <v>3023308</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D98" t="n">
-        <v>305113</v>
+        <v>306613</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3791</v>
+        <v>3803</v>
       </c>
       <c r="D101" t="n">
-        <v>5025440</v>
+        <v>5042690</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>796</v>
+        <v>803</v>
       </c>
       <c r="D102" t="n">
-        <v>1422215</v>
+        <v>1440991</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="D103" t="n">
-        <v>939892</v>
+        <v>972892</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D104" t="n">
-        <v>356289</v>
+        <v>359289</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D106" t="n">
-        <v>61500</v>
+        <v>69000</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>11379</v>
+        <v>11420</v>
       </c>
       <c r="D107" t="n">
-        <v>16498883</v>
+        <v>16556636</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>30288</v>
+        <v>30342</v>
       </c>
       <c r="D108" t="n">
-        <v>44472764</v>
+        <v>44550651</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>10153</v>
+        <v>10178</v>
       </c>
       <c r="D109" t="n">
-        <v>15093945</v>
+        <v>15131445</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>2802</v>
+        <v>2810</v>
       </c>
       <c r="D110" t="n">
-        <v>4177510</v>
+        <v>4189510</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="D111" t="n">
-        <v>783403</v>
+        <v>790903</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>10189</v>
+        <v>10204</v>
       </c>
       <c r="D114" t="n">
-        <v>13430504</v>
+        <v>13449859</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>32020</v>
+        <v>32116</v>
       </c>
       <c r="D115" t="n">
-        <v>46149833</v>
+        <v>46288948</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>68792</v>
+        <v>68951</v>
       </c>
       <c r="D116" t="n">
-        <v>100638176</v>
+        <v>100868930</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>22102</v>
+        <v>22162</v>
       </c>
       <c r="D117" t="n">
-        <v>32836804</v>
+        <v>32925525</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>6296</v>
+        <v>6313</v>
       </c>
       <c r="D118" t="n">
-        <v>9374011</v>
+        <v>9399214</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1200</v>
+        <v>1211</v>
       </c>
       <c r="D119" t="n">
-        <v>1792889</v>
+        <v>1809092</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>26848</v>
+        <v>26912</v>
       </c>
       <c r="D124" t="n">
-        <v>35809087</v>
+        <v>35883617</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>38058</v>
+        <v>38205</v>
       </c>
       <c r="D125" t="n">
-        <v>54889371</v>
+        <v>55101080</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>80347</v>
+        <v>80559</v>
       </c>
       <c r="D126" t="n">
-        <v>117447950</v>
+        <v>117756402</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>24797</v>
+        <v>24845</v>
       </c>
       <c r="D127" t="n">
-        <v>36801270</v>
+        <v>36873144</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>6672</v>
+        <v>6697</v>
       </c>
       <c r="D128" t="n">
-        <v>9915243</v>
+        <v>9951616</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1355</v>
+        <v>1369</v>
       </c>
       <c r="D129" t="n">
-        <v>2010958</v>
+        <v>2030792</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>33166</v>
+        <v>33224</v>
       </c>
       <c r="D133" t="n">
-        <v>43981558</v>
+        <v>44053284</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>13983</v>
+        <v>14013</v>
       </c>
       <c r="D134" t="n">
-        <v>20235093</v>
+        <v>20279388</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>33643</v>
+        <v>33725</v>
       </c>
       <c r="D135" t="n">
-        <v>49395272</v>
+        <v>49515046</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>11879</v>
+        <v>11918</v>
       </c>
       <c r="D136" t="n">
-        <v>17648784</v>
+        <v>17707284</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>3117</v>
+        <v>3130</v>
       </c>
       <c r="D137" t="n">
-        <v>4646741</v>
+        <v>4664875</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="D138" t="n">
-        <v>796490</v>
+        <v>802490</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>11249</v>
+        <v>11275</v>
       </c>
       <c r="D141" t="n">
-        <v>14976934</v>
+        <v>15006382</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>37155</v>
+        <v>37257</v>
       </c>
       <c r="D142" t="n">
-        <v>53655018</v>
+        <v>53802213</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>85461</v>
+        <v>85718</v>
       </c>
       <c r="D143" t="n">
-        <v>125172678</v>
+        <v>125547056</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>25426</v>
+        <v>25511</v>
       </c>
       <c r="D144" t="n">
-        <v>37773178</v>
+        <v>37898430</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>6681</v>
+        <v>6706</v>
       </c>
       <c r="D145" t="n">
-        <v>9966025</v>
+        <v>10003525</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1533</v>
+        <v>1540</v>
       </c>
       <c r="D146" t="n">
-        <v>2278802</v>
+        <v>2289302</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>30552</v>
+        <v>30625</v>
       </c>
       <c r="D149" t="n">
-        <v>41134172</v>
+        <v>41229299</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-09-30 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:H150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>39945</v>
+        <v>40092</v>
       </c>
       <c r="D2" t="n">
-        <v>57709072</v>
+        <v>57919140</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>95463</v>
+        <v>95795</v>
       </c>
       <c r="D3" t="n">
-        <v>139875268</v>
+        <v>140355131</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>32518</v>
+        <v>32649</v>
       </c>
       <c r="D4" t="n">
-        <v>48139554</v>
+        <v>48333378</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9204</v>
+        <v>9251</v>
       </c>
       <c r="D5" t="n">
-        <v>13674869</v>
+        <v>13744690</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2187</v>
+        <v>2215</v>
       </c>
       <c r="D6" t="n">
-        <v>3248648</v>
+        <v>3290648</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -610,10 +610,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D7" t="n">
-        <v>293593</v>
+        <v>299593</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>43291</v>
+        <v>43407</v>
       </c>
       <c r="D12" t="n">
-        <v>58659852</v>
+        <v>58809825</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10153</v>
+        <v>10185</v>
       </c>
       <c r="D13" t="n">
-        <v>14669907</v>
+        <v>14716573</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>27053</v>
+        <v>27127</v>
       </c>
       <c r="D14" t="n">
-        <v>39649723</v>
+        <v>39754821</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8618</v>
+        <v>8646</v>
       </c>
       <c r="D15" t="n">
-        <v>12789365</v>
+        <v>12831365</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2271</v>
+        <v>2281</v>
       </c>
       <c r="D16" t="n">
-        <v>3374153</v>
+        <v>3389153</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D17" t="n">
-        <v>658123</v>
+        <v>664123</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D18" t="n">
-        <v>57000</v>
+        <v>61500</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>10657</v>
+        <v>10684</v>
       </c>
       <c r="D20" t="n">
-        <v>14065857</v>
+        <v>14099364</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14025</v>
+        <v>14067</v>
       </c>
       <c r="D21" t="n">
-        <v>20229835</v>
+        <v>20289486</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>32904</v>
+        <v>32975</v>
       </c>
       <c r="D22" t="n">
-        <v>48257367</v>
+        <v>48358885</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>10604</v>
+        <v>10623</v>
       </c>
       <c r="D23" t="n">
-        <v>15759232</v>
+        <v>15787732</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2765</v>
+        <v>2772</v>
       </c>
       <c r="D24" t="n">
-        <v>4112174</v>
+        <v>4121198</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="D25" t="n">
-        <v>843092</v>
+        <v>847592</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1370,10 +1370,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>12171</v>
+        <v>12191</v>
       </c>
       <c r="D27" t="n">
-        <v>16213937</v>
+        <v>16239617</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>8109</v>
+        <v>8135</v>
       </c>
       <c r="D28" t="n">
-        <v>11727701</v>
+        <v>11765761</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>23513</v>
+        <v>23573</v>
       </c>
       <c r="D29" t="n">
-        <v>34503428</v>
+        <v>34588138</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8100</v>
+        <v>8127</v>
       </c>
       <c r="D30" t="n">
-        <v>12042633</v>
+        <v>12082733</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2049</v>
+        <v>2060</v>
       </c>
       <c r="D31" t="n">
-        <v>3056699</v>
+        <v>3073199</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="D32" t="n">
-        <v>582415</v>
+        <v>589915</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D33" t="n">
-        <v>47893</v>
+        <v>52393</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8701</v>
+        <v>8725</v>
       </c>
       <c r="D34" t="n">
-        <v>11488796</v>
+        <v>11517144</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3485</v>
+        <v>3506</v>
       </c>
       <c r="D35" t="n">
-        <v>5029994</v>
+        <v>5060602</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>8268</v>
+        <v>8309</v>
       </c>
       <c r="D36" t="n">
-        <v>12077662</v>
+        <v>12138062</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3302</v>
+        <v>3325</v>
       </c>
       <c r="D37" t="n">
-        <v>4895961</v>
+        <v>4930461</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="D38" t="n">
-        <v>1269055</v>
+        <v>1273555</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2625</v>
+        <v>2642</v>
       </c>
       <c r="D41" t="n">
-        <v>3544328</v>
+        <v>3565452</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>18174</v>
+        <v>18236</v>
       </c>
       <c r="D42" t="n">
-        <v>26249614</v>
+        <v>26333235</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1978,10 +1978,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>53328</v>
+        <v>53501</v>
       </c>
       <c r="D43" t="n">
-        <v>78139631</v>
+        <v>78389244</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>19625</v>
+        <v>19695</v>
       </c>
       <c r="D44" t="n">
-        <v>29136980</v>
+        <v>29239518</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5874</v>
+        <v>5895</v>
       </c>
       <c r="D45" t="n">
-        <v>8742935</v>
+        <v>8771702</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1322</v>
+        <v>1334</v>
       </c>
       <c r="D46" t="n">
-        <v>1972644</v>
+        <v>1990644</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>17582</v>
+        <v>17673</v>
       </c>
       <c r="D50" t="n">
-        <v>23322312</v>
+        <v>23441560</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2241</v>
+        <v>2248</v>
       </c>
       <c r="D51" t="n">
-        <v>3251962</v>
+        <v>3262462</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7545</v>
+        <v>7586</v>
       </c>
       <c r="D52" t="n">
-        <v>11086912</v>
+        <v>11146270</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2520</v>
+        <v>2533</v>
       </c>
       <c r="D53" t="n">
-        <v>3761684</v>
+        <v>3781184</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>795</v>
+        <v>800</v>
       </c>
       <c r="D54" t="n">
-        <v>1187415</v>
+        <v>1194915</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>7627</v>
+        <v>7661</v>
       </c>
       <c r="D57" t="n">
-        <v>10491587</v>
+        <v>10538911</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1377</v>
+        <v>1393</v>
       </c>
       <c r="D58" t="n">
-        <v>2545508</v>
+        <v>2587823</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3378</v>
+        <v>3423</v>
       </c>
       <c r="D59" t="n">
-        <v>6263463</v>
+        <v>6381344</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1329</v>
+        <v>1342</v>
       </c>
       <c r="D60" t="n">
-        <v>2466462</v>
+        <v>2500312</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="D61" t="n">
-        <v>831083</v>
+        <v>856583</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D62" t="n">
-        <v>299600</v>
+        <v>310100</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D63" t="n">
-        <v>64500</v>
+        <v>67500</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2089</v>
+        <v>2128</v>
       </c>
       <c r="D64" t="n">
-        <v>3567660</v>
+        <v>3660884</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>16280</v>
+        <v>16349</v>
       </c>
       <c r="D65" t="n">
-        <v>23502456</v>
+        <v>23600874</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>46826</v>
+        <v>46958</v>
       </c>
       <c r="D66" t="n">
-        <v>68469913</v>
+        <v>68659095</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2890,10 +2890,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>16345</v>
+        <v>16389</v>
       </c>
       <c r="D67" t="n">
-        <v>24285049</v>
+        <v>24350837</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4773</v>
+        <v>4784</v>
       </c>
       <c r="D68" t="n">
-        <v>7109288</v>
+        <v>7125274</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1013</v>
+        <v>1030</v>
       </c>
       <c r="D69" t="n">
-        <v>1505829</v>
+        <v>1531329</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>15706</v>
+        <v>15739</v>
       </c>
       <c r="D73" t="n">
-        <v>20648742</v>
+        <v>20686486</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>57706</v>
+        <v>58089</v>
       </c>
       <c r="D74" t="n">
-        <v>83914689</v>
+        <v>84454400</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>159686</v>
+        <v>160571</v>
       </c>
       <c r="D75" t="n">
-        <v>235102433</v>
+        <v>236390821</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3232,10 +3232,10 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>68475</v>
+        <v>68880</v>
       </c>
       <c r="D76" t="n">
-        <v>102001330</v>
+        <v>102600993</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -3270,10 +3270,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>22085</v>
+        <v>22248</v>
       </c>
       <c r="D77" t="n">
-        <v>32999453</v>
+        <v>33243128</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>5369</v>
+        <v>5446</v>
       </c>
       <c r="D78" t="n">
-        <v>8019602</v>
+        <v>8131772</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="D79" t="n">
-        <v>515670</v>
+        <v>524670</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>56787</v>
+        <v>57135</v>
       </c>
       <c r="D85" t="n">
-        <v>76866280</v>
+        <v>77307270</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4926</v>
+        <v>4945</v>
       </c>
       <c r="D86" t="n">
-        <v>7138689</v>
+        <v>7165799</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>12210</v>
+        <v>12240</v>
       </c>
       <c r="D87" t="n">
-        <v>17933935</v>
+        <v>17974917</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3688,10 +3688,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4032</v>
+        <v>4039</v>
       </c>
       <c r="D88" t="n">
-        <v>6007958</v>
+        <v>6018458</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1402</v>
+        <v>1410</v>
       </c>
       <c r="D89" t="n">
-        <v>2094111</v>
+        <v>2106111</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D90" t="n">
-        <v>473512</v>
+        <v>475012</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>5722</v>
+        <v>5735</v>
       </c>
       <c r="D93" t="n">
-        <v>7680595</v>
+        <v>7695735</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1720</v>
+        <v>1728</v>
       </c>
       <c r="D94" t="n">
-        <v>2479136</v>
+        <v>2490561</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>5557</v>
+        <v>5579</v>
       </c>
       <c r="D95" t="n">
-        <v>8187317</v>
+        <v>8220117</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2031</v>
+        <v>2038</v>
       </c>
       <c r="D96" t="n">
-        <v>3023308</v>
+        <v>3033181</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4030,10 +4030,10 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="D97" t="n">
-        <v>1107460</v>
+        <v>1110460</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D98" t="n">
-        <v>306613</v>
+        <v>308113</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3803</v>
+        <v>3815</v>
       </c>
       <c r="D101" t="n">
-        <v>5042690</v>
+        <v>5058540</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>803</v>
+        <v>809</v>
       </c>
       <c r="D102" t="n">
-        <v>1440991</v>
+        <v>1457491</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>517</v>
+        <v>528</v>
       </c>
       <c r="D103" t="n">
-        <v>972892</v>
+        <v>1003392</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D104" t="n">
-        <v>359289</v>
+        <v>362234</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>11420</v>
+        <v>11447</v>
       </c>
       <c r="D107" t="n">
-        <v>16556636</v>
+        <v>16596892</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>30342</v>
+        <v>30428</v>
       </c>
       <c r="D108" t="n">
-        <v>44550651</v>
+        <v>44675964</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>10178</v>
+        <v>10203</v>
       </c>
       <c r="D109" t="n">
-        <v>15131445</v>
+        <v>15168945</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4524,10 +4524,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>2810</v>
+        <v>2817</v>
       </c>
       <c r="D110" t="n">
-        <v>4189510</v>
+        <v>4200010</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -4562,10 +4562,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="D111" t="n">
-        <v>790903</v>
+        <v>798403</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4600,10 +4600,10 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D112" t="n">
-        <v>90000</v>
+        <v>93000</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>10204</v>
+        <v>10235</v>
       </c>
       <c r="D114" t="n">
-        <v>13449859</v>
+        <v>13487607</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>32116</v>
+        <v>32219</v>
       </c>
       <c r="D115" t="n">
-        <v>46288948</v>
+        <v>46437249</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>68951</v>
+        <v>69140</v>
       </c>
       <c r="D116" t="n">
-        <v>100868930</v>
+        <v>101138678</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>22162</v>
+        <v>22206</v>
       </c>
       <c r="D117" t="n">
-        <v>32925525</v>
+        <v>32989199</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>6313</v>
+        <v>6336</v>
       </c>
       <c r="D118" t="n">
-        <v>9399214</v>
+        <v>9433714</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4866,10 +4866,10 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1211</v>
+        <v>1214</v>
       </c>
       <c r="D119" t="n">
-        <v>1809092</v>
+        <v>1813592</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>26912</v>
+        <v>26987</v>
       </c>
       <c r="D124" t="n">
-        <v>35883617</v>
+        <v>35979892</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>38205</v>
+        <v>38339</v>
       </c>
       <c r="D125" t="n">
-        <v>55101080</v>
+        <v>55285529</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>80559</v>
+        <v>80847</v>
       </c>
       <c r="D126" t="n">
-        <v>117756402</v>
+        <v>118166679</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>24845</v>
+        <v>24903</v>
       </c>
       <c r="D127" t="n">
-        <v>36873144</v>
+        <v>36957945</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>6697</v>
+        <v>6724</v>
       </c>
       <c r="D128" t="n">
-        <v>9951616</v>
+        <v>9992116</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1369</v>
+        <v>1378</v>
       </c>
       <c r="D129" t="n">
-        <v>2030792</v>
+        <v>2044240</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D130" t="n">
-        <v>107728</v>
+        <v>109228</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>33224</v>
+        <v>33307</v>
       </c>
       <c r="D133" t="n">
-        <v>44053284</v>
+        <v>44159445</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>14013</v>
+        <v>14050</v>
       </c>
       <c r="D134" t="n">
-        <v>20279388</v>
+        <v>20331824</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>33725</v>
+        <v>33790</v>
       </c>
       <c r="D135" t="n">
-        <v>49515046</v>
+        <v>49606810</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>11918</v>
+        <v>11940</v>
       </c>
       <c r="D136" t="n">
-        <v>17707284</v>
+        <v>17740284</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>3130</v>
+        <v>3142</v>
       </c>
       <c r="D137" t="n">
-        <v>4664875</v>
+        <v>4682875</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="D138" t="n">
-        <v>802490</v>
+        <v>809990</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D139" t="n">
-        <v>58825</v>
+        <v>63325</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5702,10 +5702,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>11275</v>
+        <v>3</v>
       </c>
       <c r="D141" t="n">
-        <v>15006382</v>
+        <v>984</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -5719,12 +5719,12 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>NN</t>
+          <t>42</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Etablissement non employeur</t>
+          <t>1 000 à 1 999 salariés</t>
         </is>
       </c>
     </row>
@@ -5740,29 +5740,29 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>37257</v>
+        <v>11303</v>
       </c>
       <c r="D142" t="n">
-        <v>53802213</v>
+        <v>15041834</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Provence-Alpes-Côte d'Azur</t>
+          <t>Pays de la Loire</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>00</t>
+          <t>NN</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>0 salarié</t>
+          <t>Etablissement non employeur</t>
         </is>
       </c>
     </row>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>85718</v>
+        <v>37400</v>
       </c>
       <c r="D143" t="n">
-        <v>125547056</v>
+        <v>54007181</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5795,12 +5795,12 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>1 ou 2 salariés</t>
+          <t>0 salarié</t>
         </is>
       </c>
     </row>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>25511</v>
+        <v>86053</v>
       </c>
       <c r="D144" t="n">
-        <v>37898430</v>
+        <v>126031562</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5833,12 +5833,12 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>3 à 5 salariés</t>
+          <t>1 ou 2 salariés</t>
         </is>
       </c>
     </row>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>6706</v>
+        <v>25615</v>
       </c>
       <c r="D145" t="n">
-        <v>10003525</v>
+        <v>38050518</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5871,12 +5871,12 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>6 à 9 salariés</t>
+          <t>3 à 5 salariés</t>
         </is>
       </c>
     </row>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1540</v>
+        <v>6741</v>
       </c>
       <c r="D146" t="n">
-        <v>2289302</v>
+        <v>10051945</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5909,12 +5909,12 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>03</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>10 à 19 salariés</t>
+          <t>6 à 9 salariés</t>
         </is>
       </c>
     </row>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>92</v>
+        <v>1554</v>
       </c>
       <c r="D147" t="n">
-        <v>137630</v>
+        <v>2310302</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5947,12 +5947,12 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>20 à 49 salariés</t>
+          <t>10 à 19 salariés</t>
         </is>
       </c>
     </row>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="D148" t="n">
-        <v>21000</v>
+        <v>137630</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -5985,12 +5985,12 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>50 à 99 salariés</t>
+          <t>20 à 49 salariés</t>
         </is>
       </c>
     </row>
@@ -6006,10 +6006,10 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>30625</v>
+        <v>14</v>
       </c>
       <c r="D149" t="n">
-        <v>41229299</v>
+        <v>21000</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -6023,10 +6023,48 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>50 à 99 salariés</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Fonds de solidarité</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>VOLET1</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>30707</v>
+      </c>
+      <c r="D150" t="n">
+        <v>41332186</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Provence-Alpes-Côte d'Azur</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
           <t>NN</t>
         </is>
       </c>
-      <c r="H149" t="inlineStr">
+      <c r="H150" t="inlineStr">
         <is>
           <t>Etablissement non employeur</t>
         </is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-24 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>56468</v>
+        <v>55915</v>
       </c>
       <c r="D2" t="n">
-        <v>115550069</v>
+        <v>113485402</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>136920</v>
+        <v>135707</v>
       </c>
       <c r="D3" t="n">
-        <v>322625031</v>
+        <v>317278136</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>49712</v>
+        <v>49236</v>
       </c>
       <c r="D4" t="n">
-        <v>144940080</v>
+        <v>141987150</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15758</v>
+        <v>15539</v>
       </c>
       <c r="D5" t="n">
-        <v>53559040</v>
+        <v>52052979</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5822</v>
+        <v>5702</v>
       </c>
       <c r="D6" t="n">
-        <v>26603907</v>
+        <v>25810653</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -610,10 +610,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1174</v>
+        <v>1117</v>
       </c>
       <c r="D7" t="n">
-        <v>6853421</v>
+        <v>6459386</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D8" t="n">
-        <v>521481</v>
+        <v>428992</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>58820</v>
+        <v>58010</v>
       </c>
       <c r="D12" t="n">
-        <v>93759141</v>
+        <v>92000936</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>14327</v>
+        <v>14188</v>
       </c>
       <c r="D13" t="n">
-        <v>28987514</v>
+        <v>28480154</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>38498</v>
+        <v>38254</v>
       </c>
       <c r="D14" t="n">
-        <v>89053212</v>
+        <v>88040253</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>12786</v>
+        <v>12691</v>
       </c>
       <c r="D15" t="n">
-        <v>35503248</v>
+        <v>34888215</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3685</v>
+        <v>3649</v>
       </c>
       <c r="D16" t="n">
-        <v>11356675</v>
+        <v>11116190</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1208</v>
+        <v>1182</v>
       </c>
       <c r="D17" t="n">
-        <v>5217914</v>
+        <v>5055626</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="D18" t="n">
-        <v>1454775</v>
+        <v>1338825</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1066,10 +1066,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19" t="n">
-        <v>72134</v>
+        <v>52134</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>14367</v>
+        <v>14262</v>
       </c>
       <c r="D20" t="n">
-        <v>22294426</v>
+        <v>22068214</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20108</v>
+        <v>19978</v>
       </c>
       <c r="D21" t="n">
-        <v>42625507</v>
+        <v>42138796</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>47634</v>
+        <v>47324</v>
       </c>
       <c r="D22" t="n">
-        <v>114820550</v>
+        <v>113293011</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>16503</v>
+        <v>16397</v>
       </c>
       <c r="D23" t="n">
-        <v>47761886</v>
+        <v>47106615</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4896</v>
+        <v>4847</v>
       </c>
       <c r="D24" t="n">
-        <v>15898972</v>
+        <v>15594940</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1585</v>
+        <v>1544</v>
       </c>
       <c r="D25" t="n">
-        <v>6689556</v>
+        <v>6387394</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1332,10 +1332,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="D26" t="n">
-        <v>1414002</v>
+        <v>1329889</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>16088</v>
+        <v>15970</v>
       </c>
       <c r="D28" t="n">
-        <v>24838140</v>
+        <v>24590659</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>11384</v>
+        <v>11276</v>
       </c>
       <c r="D29" t="n">
-        <v>23325697</v>
+        <v>22945273</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>32927</v>
+        <v>32704</v>
       </c>
       <c r="D30" t="n">
-        <v>74584031</v>
+        <v>73596715</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>11887</v>
+        <v>11781</v>
       </c>
       <c r="D31" t="n">
-        <v>32281313</v>
+        <v>31640438</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3273</v>
+        <v>3231</v>
       </c>
       <c r="D32" t="n">
-        <v>9868612</v>
+        <v>9601971</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1027</v>
+        <v>1002</v>
       </c>
       <c r="D33" t="n">
-        <v>4356711</v>
+        <v>4181873</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="D34" t="n">
-        <v>973490</v>
+        <v>875838</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D35" t="n">
-        <v>36015</v>
+        <v>16015</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>11641</v>
+        <v>11555</v>
       </c>
       <c r="D36" t="n">
-        <v>18093411</v>
+        <v>17921253</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>5041</v>
+        <v>4994</v>
       </c>
       <c r="D37" t="n">
-        <v>11164450</v>
+        <v>10938734</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>11822</v>
+        <v>11730</v>
       </c>
       <c r="D38" t="n">
-        <v>27585562</v>
+        <v>27133249</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4894</v>
+        <v>4851</v>
       </c>
       <c r="D39" t="n">
-        <v>14012335</v>
+        <v>13734057</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1362</v>
+        <v>1348</v>
       </c>
       <c r="D40" t="n">
-        <v>4482514</v>
+        <v>4392234</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="D41" t="n">
-        <v>2099682</v>
+        <v>2001852</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D42" t="n">
-        <v>370438</v>
+        <v>308741</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3583</v>
+        <v>3550</v>
       </c>
       <c r="D44" t="n">
-        <v>5522446</v>
+        <v>5449398</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>25816</v>
+        <v>25524</v>
       </c>
       <c r="D45" t="n">
-        <v>53520901</v>
+        <v>52528165</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>76565</v>
+        <v>75852</v>
       </c>
       <c r="D46" t="n">
-        <v>181077152</v>
+        <v>178098291</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>29470</v>
+        <v>29165</v>
       </c>
       <c r="D47" t="n">
-        <v>82510586</v>
+        <v>80848056</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>9600</v>
+        <v>9496</v>
       </c>
       <c r="D48" t="n">
-        <v>29401208</v>
+        <v>28792626</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3315</v>
+        <v>3255</v>
       </c>
       <c r="D49" t="n">
-        <v>13404524</v>
+        <v>13039876</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>585</v>
+        <v>551</v>
       </c>
       <c r="D50" t="n">
-        <v>3300708</v>
+        <v>3068714</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2282,10 +2282,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D51" t="n">
-        <v>142961</v>
+        <v>131461</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>26603</v>
+        <v>26029</v>
       </c>
       <c r="D53" t="n">
-        <v>49047371</v>
+        <v>47395017</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2711</v>
+        <v>2700</v>
       </c>
       <c r="D54" t="n">
-        <v>4393992</v>
+        <v>4374322</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>9055</v>
+        <v>9011</v>
       </c>
       <c r="D55" t="n">
-        <v>15074433</v>
+        <v>14896799</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3034</v>
+        <v>3026</v>
       </c>
       <c r="D56" t="n">
-        <v>5349977</v>
+        <v>5326939</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>997</v>
+        <v>987</v>
       </c>
       <c r="D57" t="n">
-        <v>1971844</v>
+        <v>1929685</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D58" t="n">
-        <v>670437</v>
+        <v>655439</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2586,10 +2586,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D59" t="n">
-        <v>161660</v>
+        <v>151660</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>9290</v>
+        <v>9188</v>
       </c>
       <c r="D61" t="n">
-        <v>13848039</v>
+        <v>13607238</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1829</v>
+        <v>1819</v>
       </c>
       <c r="D62" t="n">
-        <v>3996094</v>
+        <v>3966477</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>4327</v>
+        <v>4307</v>
       </c>
       <c r="D63" t="n">
-        <v>9411104</v>
+        <v>9318351</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1732</v>
+        <v>1720</v>
       </c>
       <c r="D64" t="n">
-        <v>3907584</v>
+        <v>3847459</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D66" t="n">
-        <v>477383</v>
+        <v>469987</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2835</v>
+        <v>2812</v>
       </c>
       <c r="D68" t="n">
-        <v>5609862</v>
+        <v>5533335</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>22970</v>
+        <v>22774</v>
       </c>
       <c r="D69" t="n">
-        <v>45569721</v>
+        <v>44898472</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>66659</v>
+        <v>66097</v>
       </c>
       <c r="D70" t="n">
-        <v>152658579</v>
+        <v>150173951</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>24390</v>
+        <v>24135</v>
       </c>
       <c r="D71" t="n">
-        <v>68108753</v>
+        <v>66569505</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>7649</v>
+        <v>7548</v>
       </c>
       <c r="D72" t="n">
-        <v>23329447</v>
+        <v>22667755</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>2477</v>
+        <v>2436</v>
       </c>
       <c r="D73" t="n">
-        <v>10038509</v>
+        <v>9808358</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>519</v>
+        <v>481</v>
       </c>
       <c r="D74" t="n">
-        <v>2941713</v>
+        <v>2660913</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D75" t="n">
-        <v>98942</v>
+        <v>77119</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>21313</v>
+        <v>21110</v>
       </c>
       <c r="D78" t="n">
-        <v>32786319</v>
+        <v>32372822</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>83856</v>
+        <v>82902</v>
       </c>
       <c r="D79" t="n">
-        <v>172913212</v>
+        <v>169492941</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>227756</v>
+        <v>225436</v>
       </c>
       <c r="D80" t="n">
-        <v>515878363</v>
+        <v>505559731</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>102933</v>
+        <v>101708</v>
       </c>
       <c r="D81" t="n">
-        <v>290380864</v>
+        <v>282940570</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>37577</v>
+        <v>37034</v>
       </c>
       <c r="D82" t="n">
-        <v>127265720</v>
+        <v>123494119</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>13895</v>
+        <v>13562</v>
       </c>
       <c r="D83" t="n">
-        <v>63119321</v>
+        <v>60784574</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>2747</v>
+        <v>2615</v>
       </c>
       <c r="D84" t="n">
-        <v>17719212</v>
+        <v>16686344</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D85" t="n">
-        <v>890467</v>
+        <v>874968</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3612,10 +3612,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D86" t="n">
-        <v>152125</v>
+        <v>142125</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -3726,10 +3726,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D89" t="n">
-        <v>28424</v>
+        <v>18424</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>79554</v>
+        <v>78768</v>
       </c>
       <c r="D90" t="n">
-        <v>126626230</v>
+        <v>124817296</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>5649</v>
+        <v>5613</v>
       </c>
       <c r="D91" t="n">
-        <v>8820971</v>
+        <v>8731030</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>13593</v>
+        <v>13532</v>
       </c>
       <c r="D92" t="n">
-        <v>21543978</v>
+        <v>21384010</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4360</v>
+        <v>4349</v>
       </c>
       <c r="D93" t="n">
-        <v>7106451</v>
+        <v>7030128</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="D94" t="n">
-        <v>2569024</v>
+        <v>2567524</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D95" t="n">
-        <v>957812</v>
+        <v>917812</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -3992,10 +3992,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D96" t="n">
-        <v>183975</v>
+        <v>163975</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>6376</v>
+        <v>6343</v>
       </c>
       <c r="D98" t="n">
-        <v>8779773</v>
+        <v>8730476</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>2313</v>
+        <v>2306</v>
       </c>
       <c r="D99" t="n">
-        <v>4292019</v>
+        <v>4271374</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>7349</v>
+        <v>7299</v>
       </c>
       <c r="D100" t="n">
-        <v>14653292</v>
+        <v>14496358</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>2632</v>
+        <v>2622</v>
       </c>
       <c r="D101" t="n">
-        <v>5972509</v>
+        <v>5916686</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4220,10 +4220,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="D102" t="n">
-        <v>2344417</v>
+        <v>2292466</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D103" t="n">
-        <v>1100276</v>
+        <v>1060276</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D104" t="n">
-        <v>334891</v>
+        <v>273559</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>4936</v>
+        <v>4866</v>
       </c>
       <c r="D106" t="n">
-        <v>7229919</v>
+        <v>7075180</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1040</v>
+        <v>1031</v>
       </c>
       <c r="D107" t="n">
-        <v>2364697</v>
+        <v>2321197</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D108" t="n">
-        <v>1835936</v>
+        <v>1825936</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -4486,10 +4486,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D109" t="n">
-        <v>572692</v>
+        <v>569692</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>16451</v>
+        <v>16330</v>
       </c>
       <c r="D113" t="n">
-        <v>34650842</v>
+        <v>34184538</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>43293</v>
+        <v>43018</v>
       </c>
       <c r="D114" t="n">
-        <v>101628508</v>
+        <v>100467273</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>15355</v>
+        <v>15226</v>
       </c>
       <c r="D115" t="n">
-        <v>43064220</v>
+        <v>42326652</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>4752</v>
+        <v>4694</v>
       </c>
       <c r="D116" t="n">
-        <v>15112513</v>
+        <v>14749107</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1478</v>
+        <v>1455</v>
       </c>
       <c r="D117" t="n">
-        <v>6282980</v>
+        <v>6142150</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D118" t="n">
-        <v>1735408</v>
+        <v>1704742</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>13562</v>
+        <v>13467</v>
       </c>
       <c r="D122" t="n">
-        <v>20859594</v>
+        <v>20612761</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>44835</v>
+        <v>44485</v>
       </c>
       <c r="D123" t="n">
-        <v>91128972</v>
+        <v>89847589</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>95961</v>
+        <v>95287</v>
       </c>
       <c r="D124" t="n">
-        <v>216652549</v>
+        <v>213644027</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>32436</v>
+        <v>32190</v>
       </c>
       <c r="D125" t="n">
-        <v>87488479</v>
+        <v>86087933</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>10187</v>
+        <v>10066</v>
       </c>
       <c r="D126" t="n">
-        <v>31136195</v>
+        <v>30377255</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>3241</v>
+        <v>3179</v>
       </c>
       <c r="D127" t="n">
-        <v>13374589</v>
+        <v>12976700</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>670</v>
+        <v>636</v>
       </c>
       <c r="D128" t="n">
-        <v>3643934</v>
+        <v>3392190</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5246,10 +5246,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D129" t="n">
-        <v>173657</v>
+        <v>145332</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>35157</v>
+        <v>34900</v>
       </c>
       <c r="D132" t="n">
-        <v>53845436</v>
+        <v>53306639</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>53952</v>
+        <v>53527</v>
       </c>
       <c r="D133" t="n">
-        <v>110919973</v>
+        <v>109409642</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>113022</v>
+        <v>112163</v>
       </c>
       <c r="D134" t="n">
-        <v>253243508</v>
+        <v>249713991</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>36597</v>
+        <v>36341</v>
       </c>
       <c r="D135" t="n">
-        <v>101053850</v>
+        <v>99570021</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>10841</v>
+        <v>10750</v>
       </c>
       <c r="D136" t="n">
-        <v>33593582</v>
+        <v>33081884</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>3435</v>
+        <v>3350</v>
       </c>
       <c r="D137" t="n">
-        <v>14230729</v>
+        <v>13693761</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>568</v>
+        <v>535</v>
       </c>
       <c r="D138" t="n">
-        <v>3148927</v>
+        <v>2912989</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D139" t="n">
-        <v>245914</v>
+        <v>231414</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>43919</v>
+        <v>43565</v>
       </c>
       <c r="D142" t="n">
-        <v>65938128</v>
+        <v>65204301</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>19704</v>
+        <v>19546</v>
       </c>
       <c r="D143" t="n">
-        <v>40577398</v>
+        <v>39958896</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>47880</v>
+        <v>47556</v>
       </c>
       <c r="D144" t="n">
-        <v>112931415</v>
+        <v>111384711</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>17993</v>
+        <v>17862</v>
       </c>
       <c r="D145" t="n">
-        <v>50542562</v>
+        <v>49680384</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>5189</v>
+        <v>5135</v>
       </c>
       <c r="D146" t="n">
-        <v>16096507</v>
+        <v>15754573</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1553</v>
+        <v>1521</v>
       </c>
       <c r="D147" t="n">
-        <v>6653390</v>
+        <v>6395903</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D148" t="n">
-        <v>2005932</v>
+        <v>1952601</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>14843</v>
+        <v>14729</v>
       </c>
       <c r="D152" t="n">
-        <v>23071971</v>
+        <v>22779622</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>53489</v>
+        <v>53062</v>
       </c>
       <c r="D153" t="n">
-        <v>110989877</v>
+        <v>109546919</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>124246</v>
+        <v>123345</v>
       </c>
       <c r="D154" t="n">
-        <v>287554965</v>
+        <v>283633712</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>39555</v>
+        <v>39228</v>
       </c>
       <c r="D155" t="n">
-        <v>113970213</v>
+        <v>112043561</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6272,10 +6272,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>11827</v>
+        <v>11707</v>
       </c>
       <c r="D156" t="n">
-        <v>39977043</v>
+        <v>39119102</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>4245</v>
+        <v>4189</v>
       </c>
       <c r="D157" t="n">
-        <v>19032399</v>
+        <v>18679934</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>863</v>
+        <v>846</v>
       </c>
       <c r="D158" t="n">
-        <v>5272801</v>
+        <v>5133371</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6386,10 +6386,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D159" t="n">
-        <v>256597</v>
+        <v>245097</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>41224</v>
+        <v>40833</v>
       </c>
       <c r="D160" t="n">
-        <v>64139481</v>
+        <v>63389154</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-12-29 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>56109</v>
+        <v>56232</v>
       </c>
       <c r="D2" t="n">
-        <v>114229261</v>
+        <v>114710489</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>136160</v>
+        <v>136430</v>
       </c>
       <c r="D3" t="n">
-        <v>319282363</v>
+        <v>320513794</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>49410</v>
+        <v>49522</v>
       </c>
       <c r="D4" t="n">
-        <v>143036325</v>
+        <v>143820446</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15610</v>
+        <v>15682</v>
       </c>
       <c r="D5" t="n">
-        <v>52500774</v>
+        <v>53020452</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5740</v>
+        <v>5770</v>
       </c>
       <c r="D6" t="n">
-        <v>26062899</v>
+        <v>26271871</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -610,10 +610,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1133</v>
+        <v>1147</v>
       </c>
       <c r="D7" t="n">
-        <v>6592279</v>
+        <v>6688434</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D8" t="n">
-        <v>469315</v>
+        <v>471481</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>58301</v>
+        <v>58502</v>
       </c>
       <c r="D12" t="n">
-        <v>92669294</v>
+        <v>93094711</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -838,10 +838,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>14239</v>
+        <v>14269</v>
       </c>
       <c r="D13" t="n">
-        <v>28639924</v>
+        <v>28744342</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>38325</v>
+        <v>38393</v>
       </c>
       <c r="D14" t="n">
-        <v>88336075</v>
+        <v>88628732</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>12733</v>
+        <v>12753</v>
       </c>
       <c r="D15" t="n">
-        <v>35159617</v>
+        <v>35299250</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3665</v>
+        <v>3671</v>
       </c>
       <c r="D16" t="n">
-        <v>11229437</v>
+        <v>11262269</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1195</v>
+        <v>1199</v>
       </c>
       <c r="D17" t="n">
-        <v>5128241</v>
+        <v>5157416</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1028,10 +1028,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="D18" t="n">
-        <v>1376157</v>
+        <v>1449487</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>14306</v>
+        <v>14333</v>
       </c>
       <c r="D20" t="n">
-        <v>22167461</v>
+        <v>22222419</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1142,10 +1142,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20012</v>
+        <v>20047</v>
       </c>
       <c r="D21" t="n">
-        <v>42247731</v>
+        <v>42393023</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>47440</v>
+        <v>47515</v>
       </c>
       <c r="D22" t="n">
-        <v>113864701</v>
+        <v>114256875</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>16436</v>
+        <v>16456</v>
       </c>
       <c r="D23" t="n">
-        <v>47323769</v>
+        <v>47445108</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4855</v>
+        <v>4869</v>
       </c>
       <c r="D24" t="n">
-        <v>15656106</v>
+        <v>15736377</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1294,10 +1294,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1552</v>
+        <v>1563</v>
       </c>
       <c r="D25" t="n">
-        <v>6450394</v>
+        <v>6523892</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>16014</v>
+        <v>16037</v>
       </c>
       <c r="D28" t="n">
-        <v>24680790</v>
+        <v>24728200</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>11313</v>
+        <v>11342</v>
       </c>
       <c r="D29" t="n">
-        <v>23070337</v>
+        <v>23167236</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>32781</v>
+        <v>32840</v>
       </c>
       <c r="D30" t="n">
-        <v>73916368</v>
+        <v>74200150</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>11819</v>
+        <v>11852</v>
       </c>
       <c r="D31" t="n">
-        <v>31837648</v>
+        <v>32067377</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1560,10 +1560,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3244</v>
+        <v>3258</v>
       </c>
       <c r="D32" t="n">
-        <v>9679015</v>
+        <v>9755112</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="D33" t="n">
-        <v>4291496</v>
+        <v>4334545</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="D34" t="n">
-        <v>875838</v>
+        <v>961324</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>11581</v>
+        <v>11602</v>
       </c>
       <c r="D36" t="n">
-        <v>17988706</v>
+        <v>18023081</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>5006</v>
+        <v>5016</v>
       </c>
       <c r="D37" t="n">
-        <v>10978059</v>
+        <v>11038077</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>11762</v>
+        <v>11784</v>
       </c>
       <c r="D38" t="n">
-        <v>27283967</v>
+        <v>27393981</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4865</v>
+        <v>4874</v>
       </c>
       <c r="D39" t="n">
-        <v>13817360</v>
+        <v>13872526</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1864,10 +1864,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1352</v>
+        <v>1355</v>
       </c>
       <c r="D40" t="n">
-        <v>4397400</v>
+        <v>4427400</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D41" t="n">
-        <v>2056184</v>
+        <v>2076184</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D42" t="n">
-        <v>308741</v>
+        <v>329772</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3560</v>
+        <v>3570</v>
       </c>
       <c r="D44" t="n">
-        <v>5477171</v>
+        <v>5496539</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>25629</v>
+        <v>25699</v>
       </c>
       <c r="D45" t="n">
-        <v>52882761</v>
+        <v>53145514</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>76113</v>
+        <v>76274</v>
       </c>
       <c r="D46" t="n">
-        <v>179356347</v>
+        <v>179920123</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>29263</v>
+        <v>29347</v>
       </c>
       <c r="D47" t="n">
-        <v>81407767</v>
+        <v>81916791</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2168,10 +2168,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>9521</v>
+        <v>9550</v>
       </c>
       <c r="D48" t="n">
-        <v>28938770</v>
+        <v>29099305</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3278</v>
+        <v>3287</v>
       </c>
       <c r="D49" t="n">
-        <v>13163538</v>
+        <v>13214539</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2244,10 +2244,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="D50" t="n">
-        <v>3170046</v>
+        <v>3184876</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2358,10 +2358,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>26204</v>
+        <v>26346</v>
       </c>
       <c r="D53" t="n">
-        <v>47955009</v>
+        <v>48368713</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2396,10 +2396,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2705</v>
+        <v>2707</v>
       </c>
       <c r="D54" t="n">
-        <v>4382992</v>
+        <v>4387992</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2434,10 +2434,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>9020</v>
+        <v>9040</v>
       </c>
       <c r="D55" t="n">
-        <v>14917774</v>
+        <v>14985554</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2472,10 +2472,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3031</v>
+        <v>3032</v>
       </c>
       <c r="D56" t="n">
-        <v>5345477</v>
+        <v>5346977</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2510,10 +2510,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="D57" t="n">
-        <v>1936183</v>
+        <v>1949513</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2662,10 +2662,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>9216</v>
+        <v>9243</v>
       </c>
       <c r="D61" t="n">
-        <v>13668842</v>
+        <v>13747465</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1823</v>
+        <v>1825</v>
       </c>
       <c r="D62" t="n">
-        <v>3973977</v>
+        <v>3980094</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2738,10 +2738,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>4311</v>
+        <v>4316</v>
       </c>
       <c r="D63" t="n">
-        <v>9343978</v>
+        <v>9361700</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2776,10 +2776,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1723</v>
+        <v>1727</v>
       </c>
       <c r="D64" t="n">
-        <v>3868959</v>
+        <v>3886459</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2852,10 +2852,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D66" t="n">
-        <v>469987</v>
+        <v>471487</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2827</v>
+        <v>2828</v>
       </c>
       <c r="D68" t="n">
-        <v>5590039</v>
+        <v>5597206</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>22841</v>
+        <v>22889</v>
       </c>
       <c r="D69" t="n">
-        <v>45114762</v>
+        <v>45278224</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3004,10 +3004,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>66280</v>
+        <v>66425</v>
       </c>
       <c r="D70" t="n">
-        <v>151028229</v>
+        <v>151647727</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>24215</v>
+        <v>24289</v>
       </c>
       <c r="D71" t="n">
-        <v>67034286</v>
+        <v>67498653</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>7573</v>
+        <v>7601</v>
       </c>
       <c r="D72" t="n">
-        <v>22850275</v>
+        <v>23010657</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>2450</v>
+        <v>2465</v>
       </c>
       <c r="D73" t="n">
-        <v>9896879</v>
+        <v>9967043</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -3156,10 +3156,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="D74" t="n">
-        <v>2673913</v>
+        <v>2742238</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D75" t="n">
-        <v>77119</v>
+        <v>88619</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -3308,10 +3308,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>21190</v>
+        <v>21234</v>
       </c>
       <c r="D78" t="n">
-        <v>32519668</v>
+        <v>32615041</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>83270</v>
+        <v>83469</v>
       </c>
       <c r="D79" t="n">
-        <v>170790139</v>
+        <v>171523501</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>226310</v>
+        <v>226810</v>
       </c>
       <c r="D80" t="n">
-        <v>509463899</v>
+        <v>511707455</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3422,10 +3422,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>102133</v>
+        <v>102420</v>
       </c>
       <c r="D81" t="n">
-        <v>285693395</v>
+        <v>287462800</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3460,10 +3460,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>37236</v>
+        <v>37346</v>
       </c>
       <c r="D82" t="n">
-        <v>124951614</v>
+        <v>125670917</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>13683</v>
+        <v>13776</v>
       </c>
       <c r="D83" t="n">
-        <v>61649660</v>
+        <v>62319089</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>2656</v>
+        <v>2697</v>
       </c>
       <c r="D84" t="n">
-        <v>17016509</v>
+        <v>17333162</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>79086</v>
+        <v>79255</v>
       </c>
       <c r="D90" t="n">
-        <v>125555569</v>
+        <v>125991855</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3802,10 +3802,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>5624</v>
+        <v>5634</v>
       </c>
       <c r="D91" t="n">
-        <v>8760651</v>
+        <v>8785893</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>13553</v>
+        <v>13575</v>
       </c>
       <c r="D92" t="n">
-        <v>21429147</v>
+        <v>21494096</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4353</v>
+        <v>4357</v>
       </c>
       <c r="D93" t="n">
-        <v>7044628</v>
+        <v>7076451</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -3954,10 +3954,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D95" t="n">
-        <v>917812</v>
+        <v>927812</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -4068,10 +4068,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>6358</v>
+        <v>6362</v>
       </c>
       <c r="D98" t="n">
-        <v>8755989</v>
+        <v>8757623</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -4106,10 +4106,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>2307</v>
+        <v>2310</v>
       </c>
       <c r="D99" t="n">
-        <v>4273860</v>
+        <v>4277260</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>7312</v>
+        <v>7328</v>
       </c>
       <c r="D100" t="n">
-        <v>14527982</v>
+        <v>14577009</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4182,10 +4182,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>2623</v>
+        <v>2629</v>
       </c>
       <c r="D101" t="n">
-        <v>5918186</v>
+        <v>5951843</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4258,10 +4258,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D103" t="n">
-        <v>1060276</v>
+        <v>1080276</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -4296,10 +4296,10 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D104" t="n">
-        <v>283559</v>
+        <v>304891</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -4372,10 +4372,10 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>4895</v>
+        <v>4913</v>
       </c>
       <c r="D106" t="n">
-        <v>7120564</v>
+        <v>7168362</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="D107" t="n">
-        <v>2334197</v>
+        <v>2358697</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -4638,10 +4638,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>16377</v>
+        <v>16402</v>
       </c>
       <c r="D113" t="n">
-        <v>34364941</v>
+        <v>34478606</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4676,10 +4676,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>43105</v>
+        <v>43177</v>
       </c>
       <c r="D114" t="n">
-        <v>100895497</v>
+        <v>101175041</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4714,10 +4714,10 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>15278</v>
+        <v>15318</v>
       </c>
       <c r="D115" t="n">
-        <v>42633772</v>
+        <v>42874672</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -4752,10 +4752,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>4709</v>
+        <v>4732</v>
       </c>
       <c r="D116" t="n">
-        <v>14843816</v>
+        <v>14986972</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -4790,10 +4790,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1459</v>
+        <v>1466</v>
       </c>
       <c r="D117" t="n">
-        <v>6173650</v>
+        <v>6207982</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -4828,10 +4828,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D118" t="n">
-        <v>1705408</v>
+        <v>1725408</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4980,10 +4980,10 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>13502</v>
+        <v>13527</v>
       </c>
       <c r="D122" t="n">
-        <v>20681950</v>
+        <v>20745951</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -5018,10 +5018,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>44622</v>
+        <v>44704</v>
       </c>
       <c r="D123" t="n">
-        <v>90323194</v>
+        <v>90644083</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -5056,10 +5056,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>95513</v>
+        <v>95673</v>
       </c>
       <c r="D124" t="n">
-        <v>214702796</v>
+        <v>215440980</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -5094,10 +5094,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>32277</v>
+        <v>32350</v>
       </c>
       <c r="D125" t="n">
-        <v>86577082</v>
+        <v>87050498</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5132,10 +5132,10 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>10104</v>
+        <v>10137</v>
       </c>
       <c r="D126" t="n">
-        <v>30630059</v>
+        <v>30842374</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>3193</v>
+        <v>3211</v>
       </c>
       <c r="D127" t="n">
-        <v>13073837</v>
+        <v>13185501</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -5208,10 +5208,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>646</v>
+        <v>656</v>
       </c>
       <c r="D128" t="n">
-        <v>3491290</v>
+        <v>3561327</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -5360,10 +5360,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>34984</v>
+        <v>35060</v>
       </c>
       <c r="D132" t="n">
-        <v>53504362</v>
+        <v>53649627</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>53709</v>
+        <v>53793</v>
       </c>
       <c r="D133" t="n">
-        <v>110087932</v>
+        <v>110422672</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -5436,10 +5436,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>112438</v>
+        <v>112625</v>
       </c>
       <c r="D134" t="n">
-        <v>250888944</v>
+        <v>251657072</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -5474,10 +5474,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>36412</v>
+        <v>36486</v>
       </c>
       <c r="D135" t="n">
-        <v>100005175</v>
+        <v>100462357</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -5512,10 +5512,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>10775</v>
+        <v>10794</v>
       </c>
       <c r="D136" t="n">
-        <v>33222496</v>
+        <v>33326206</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5550,10 +5550,10 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>3376</v>
+        <v>3397</v>
       </c>
       <c r="D137" t="n">
-        <v>13884927</v>
+        <v>14012897</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -5588,10 +5588,10 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="D138" t="n">
-        <v>2952989</v>
+        <v>2996655</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5626,10 +5626,10 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D139" t="n">
-        <v>231414</v>
+        <v>232914</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -5740,10 +5740,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>43707</v>
+        <v>43789</v>
       </c>
       <c r="D142" t="n">
-        <v>65498362</v>
+        <v>65645814</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>19603</v>
+        <v>19651</v>
       </c>
       <c r="D143" t="n">
-        <v>40173370</v>
+        <v>40380384</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -5816,10 +5816,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>47678</v>
+        <v>47766</v>
       </c>
       <c r="D144" t="n">
-        <v>111973086</v>
+        <v>112439990</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5854,10 +5854,10 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>17911</v>
+        <v>17938</v>
       </c>
       <c r="D145" t="n">
-        <v>50031605</v>
+        <v>50166526</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -5892,10 +5892,10 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>5150</v>
+        <v>5160</v>
       </c>
       <c r="D146" t="n">
-        <v>15841404</v>
+        <v>15914236</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -5930,10 +5930,10 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D147" t="n">
-        <v>6459569</v>
+        <v>6469569</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5968,10 +5968,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D148" t="n">
-        <v>1982434</v>
+        <v>1993100</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>14779</v>
+        <v>14802</v>
       </c>
       <c r="D152" t="n">
-        <v>22909362</v>
+        <v>22985169</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -6158,10 +6158,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>53216</v>
+        <v>53322</v>
       </c>
       <c r="D153" t="n">
-        <v>110057087</v>
+        <v>110424922</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -6196,10 +6196,10 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>123651</v>
+        <v>123864</v>
       </c>
       <c r="D154" t="n">
-        <v>285000278</v>
+        <v>285933329</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -6234,10 +6234,10 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>39333</v>
+        <v>39414</v>
       </c>
       <c r="D155" t="n">
-        <v>112744656</v>
+        <v>113194911</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -6272,10 +6272,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>11749</v>
+        <v>11777</v>
       </c>
       <c r="D156" t="n">
-        <v>39419081</v>
+        <v>39622126</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>4208</v>
+        <v>4218</v>
       </c>
       <c r="D157" t="n">
-        <v>18813979</v>
+        <v>18870920</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>852</v>
+        <v>857</v>
       </c>
       <c r="D158" t="n">
-        <v>5184370</v>
+        <v>5222135</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -6424,10 +6424,10 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>40986</v>
+        <v>41085</v>
       </c>
       <c r="D160" t="n">
-        <v>63650757</v>
+        <v>63838834</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2021-03-19 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -624,13 +624,13 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>71566</v>
+        <v>71995</v>
       </c>
       <c r="D2">
-        <v>18638</v>
+        <v>18643</v>
       </c>
       <c r="E2">
-        <v>190100176</v>
+        <v>192205033</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -653,13 +653,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>174237</v>
+        <v>175373</v>
       </c>
       <c r="D3">
-        <v>46588</v>
+        <v>46610</v>
       </c>
       <c r="E3">
-        <v>573875097</v>
+        <v>581756710</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -682,13 +682,13 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>67667</v>
+        <v>68203</v>
       </c>
       <c r="D4">
-        <v>18221</v>
+        <v>18235</v>
       </c>
       <c r="E4">
-        <v>310280909</v>
+        <v>315798649</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -711,13 +711,13 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>23740</v>
+        <v>23979</v>
       </c>
       <c r="D5">
-        <v>6348</v>
+        <v>6349</v>
       </c>
       <c r="E5">
-        <v>154122832</v>
+        <v>157452033</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -740,13 +740,13 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>10686</v>
+        <v>10830</v>
       </c>
       <c r="D6">
-        <v>3038</v>
+        <v>3042</v>
       </c>
       <c r="E6">
-        <v>128199575</v>
+        <v>132148881</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -769,13 +769,13 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>2986</v>
+        <v>3032</v>
       </c>
       <c r="D7">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="E7">
-        <v>85524672</v>
+        <v>88264601</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -798,13 +798,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="D8">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E8">
-        <v>20551212</v>
+        <v>21738922</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -827,13 +827,13 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9">
         <v>34</v>
       </c>
       <c r="E9">
-        <v>8374836</v>
+        <v>8384836</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -972,13 +972,13 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>75657</v>
+        <v>76130</v>
       </c>
       <c r="D14">
-        <v>20374</v>
+        <v>20385</v>
       </c>
       <c r="E14">
-        <v>139322529</v>
+        <v>140826841</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -1001,13 +1001,13 @@
         <v>10</v>
       </c>
       <c r="C15">
-        <v>17866</v>
+        <v>17975</v>
       </c>
       <c r="D15">
-        <v>4735</v>
+        <v>4737</v>
       </c>
       <c r="E15">
-        <v>46953856</v>
+        <v>47454839</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
@@ -1030,13 +1030,13 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>48675</v>
+        <v>49010</v>
       </c>
       <c r="D16">
-        <v>13319</v>
+        <v>13326</v>
       </c>
       <c r="E16">
-        <v>157634153</v>
+        <v>160109234</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -1059,13 +1059,13 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>17158</v>
+        <v>17302</v>
       </c>
       <c r="D17">
-        <v>4815</v>
+        <v>4821</v>
       </c>
       <c r="E17">
-        <v>74030760</v>
+        <v>75400097</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -1088,13 +1088,13 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>5397</v>
+        <v>5447</v>
       </c>
       <c r="D18">
-        <v>1546</v>
+        <v>1548</v>
       </c>
       <c r="E18">
-        <v>31145890</v>
+        <v>31881679</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -1117,13 +1117,13 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>2222</v>
+        <v>2252</v>
       </c>
       <c r="D19">
         <v>668</v>
       </c>
       <c r="E19">
-        <v>23810286</v>
+        <v>24294548</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -1146,13 +1146,13 @@
         <v>10</v>
       </c>
       <c r="C20">
-        <v>726</v>
+        <v>737</v>
       </c>
       <c r="D20">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E20">
-        <v>17179975</v>
+        <v>17463864</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -1175,13 +1175,13 @@
         <v>10</v>
       </c>
       <c r="C21">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E21">
-        <v>2675626</v>
+        <v>2943883</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -1233,13 +1233,13 @@
         <v>10</v>
       </c>
       <c r="C23">
-        <v>17479</v>
+        <v>17557</v>
       </c>
       <c r="D23">
-        <v>4974</v>
+        <v>4975</v>
       </c>
       <c r="E23">
-        <v>31083859</v>
+        <v>31312762</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
@@ -1262,13 +1262,13 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>25436</v>
+        <v>25625</v>
       </c>
       <c r="D24">
-        <v>6409</v>
+        <v>6410</v>
       </c>
       <c r="E24">
-        <v>76143781</v>
+        <v>77392260</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
@@ -1291,13 +1291,13 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>60600</v>
+        <v>61104</v>
       </c>
       <c r="D25">
-        <v>16257</v>
+        <v>16261</v>
       </c>
       <c r="E25">
-        <v>211873992</v>
+        <v>215750629</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
@@ -1320,13 +1320,13 @@
         <v>10</v>
       </c>
       <c r="C26">
-        <v>22410</v>
+        <v>22660</v>
       </c>
       <c r="D26">
-        <v>6319</v>
+        <v>6323</v>
       </c>
       <c r="E26">
-        <v>103013130</v>
+        <v>105318568</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
@@ -1349,13 +1349,13 @@
         <v>10</v>
       </c>
       <c r="C27">
-        <v>7220</v>
+        <v>7306</v>
       </c>
       <c r="D27">
-        <v>2133</v>
+        <v>2134</v>
       </c>
       <c r="E27">
-        <v>44112962</v>
+        <v>45202878</v>
       </c>
       <c r="F27" t="s">
         <v>13</v>
@@ -1378,13 +1378,13 @@
         <v>10</v>
       </c>
       <c r="C28">
-        <v>2918</v>
+        <v>2959</v>
       </c>
       <c r="D28">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="E28">
-        <v>31950582</v>
+        <v>32826843</v>
       </c>
       <c r="F28" t="s">
         <v>13</v>
@@ -1407,13 +1407,13 @@
         <v>10</v>
       </c>
       <c r="C29">
-        <v>765</v>
+        <v>784</v>
       </c>
       <c r="D29">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E29">
-        <v>23428902</v>
+        <v>24265527</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
@@ -1523,13 +1523,13 @@
         <v>10</v>
       </c>
       <c r="C33">
-        <v>19108</v>
+        <v>19213</v>
       </c>
       <c r="D33">
-        <v>5537</v>
+        <v>5539</v>
       </c>
       <c r="E33">
-        <v>34317497</v>
+        <v>34612307</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
@@ -1552,13 +1552,13 @@
         <v>10</v>
       </c>
       <c r="C34">
-        <v>14005</v>
+        <v>14076</v>
       </c>
       <c r="D34">
         <v>3721</v>
       </c>
       <c r="E34">
-        <v>37007952</v>
+        <v>37365952</v>
       </c>
       <c r="F34" t="s">
         <v>14</v>
@@ -1581,13 +1581,13 @@
         <v>10</v>
       </c>
       <c r="C35">
-        <v>41067</v>
+        <v>41330</v>
       </c>
       <c r="D35">
-        <v>11480</v>
+        <v>11482</v>
       </c>
       <c r="E35">
-        <v>128768105</v>
+        <v>130711046</v>
       </c>
       <c r="F35" t="s">
         <v>14</v>
@@ -1610,13 +1610,13 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>15620</v>
+        <v>15738</v>
       </c>
       <c r="D36">
-        <v>4528</v>
+        <v>4533</v>
       </c>
       <c r="E36">
-        <v>65900105</v>
+        <v>67101040</v>
       </c>
       <c r="F36" t="s">
         <v>14</v>
@@ -1639,13 +1639,13 @@
         <v>10</v>
       </c>
       <c r="C37">
-        <v>4588</v>
+        <v>4636</v>
       </c>
       <c r="D37">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="E37">
-        <v>25560807</v>
+        <v>26122985</v>
       </c>
       <c r="F37" t="s">
         <v>14</v>
@@ -1668,13 +1668,13 @@
         <v>10</v>
       </c>
       <c r="C38">
-        <v>1860</v>
+        <v>1886</v>
       </c>
       <c r="D38">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="E38">
-        <v>20784139</v>
+        <v>21346809</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -1697,13 +1697,13 @@
         <v>10</v>
       </c>
       <c r="C39">
-        <v>486</v>
+        <v>499</v>
       </c>
       <c r="D39">
         <v>174</v>
       </c>
       <c r="E39">
-        <v>11576157</v>
+        <v>12000268</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
@@ -1726,13 +1726,13 @@
         <v>10</v>
       </c>
       <c r="C40">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D40">
         <v>13</v>
       </c>
       <c r="E40">
-        <v>1375242</v>
+        <v>1478116</v>
       </c>
       <c r="F40" t="s">
         <v>14</v>
@@ -1755,13 +1755,13 @@
         <v>10</v>
       </c>
       <c r="C41">
-        <v>13850</v>
+        <v>13929</v>
       </c>
       <c r="D41">
-        <v>3907</v>
+        <v>3909</v>
       </c>
       <c r="E41">
-        <v>24319786</v>
+        <v>24537814</v>
       </c>
       <c r="F41" t="s">
         <v>14</v>
@@ -1784,13 +1784,13 @@
         <v>10</v>
       </c>
       <c r="C42">
-        <v>6982</v>
+        <v>7060</v>
       </c>
       <c r="D42">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="E42">
-        <v>22633560</v>
+        <v>23126572</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
@@ -1813,13 +1813,13 @@
         <v>10</v>
       </c>
       <c r="C43">
-        <v>15861</v>
+        <v>16013</v>
       </c>
       <c r="D43">
-        <v>3764</v>
+        <v>3765</v>
       </c>
       <c r="E43">
-        <v>53896914</v>
+        <v>54934242</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
@@ -1842,13 +1842,13 @@
         <v>10</v>
       </c>
       <c r="C44">
-        <v>7089</v>
+        <v>7144</v>
       </c>
       <c r="D44">
         <v>1727</v>
       </c>
       <c r="E44">
-        <v>33516269</v>
+        <v>34032846</v>
       </c>
       <c r="F44" t="s">
         <v>15</v>
@@ -1871,13 +1871,13 @@
         <v>10</v>
       </c>
       <c r="C45">
-        <v>2207</v>
+        <v>2241</v>
       </c>
       <c r="D45">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E45">
-        <v>14372026</v>
+        <v>14739698</v>
       </c>
       <c r="F45" t="s">
         <v>15</v>
@@ -1900,13 +1900,13 @@
         <v>10</v>
       </c>
       <c r="C46">
-        <v>883</v>
+        <v>896</v>
       </c>
       <c r="D46">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E46">
-        <v>10945475</v>
+        <v>11182682</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
@@ -1929,13 +1929,13 @@
         <v>10</v>
       </c>
       <c r="C47">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="D47">
         <v>68</v>
       </c>
       <c r="E47">
-        <v>5186844</v>
+        <v>5500940</v>
       </c>
       <c r="F47" t="s">
         <v>15</v>
@@ -1958,13 +1958,13 @@
         <v>10</v>
       </c>
       <c r="C48">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D48">
         <v>8</v>
       </c>
       <c r="E48">
-        <v>1374298</v>
+        <v>1463766</v>
       </c>
       <c r="F48" t="s">
         <v>15</v>
@@ -1987,13 +1987,13 @@
         <v>10</v>
       </c>
       <c r="C49">
-        <v>4498</v>
+        <v>4534</v>
       </c>
       <c r="D49">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="E49">
-        <v>7752595</v>
+        <v>7837870</v>
       </c>
       <c r="F49" t="s">
         <v>15</v>
@@ -2016,13 +2016,13 @@
         <v>10</v>
       </c>
       <c r="C50">
-        <v>32624</v>
+        <v>32818</v>
       </c>
       <c r="D50">
-        <v>9178</v>
+        <v>9186</v>
       </c>
       <c r="E50">
-        <v>87092244</v>
+        <v>88174278</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
@@ -2045,13 +2045,13 @@
         <v>10</v>
       </c>
       <c r="C51">
-        <v>97703</v>
+        <v>98377</v>
       </c>
       <c r="D51">
-        <v>28031</v>
+        <v>28063</v>
       </c>
       <c r="E51">
-        <v>316874171</v>
+        <v>321764207</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
@@ -2074,13 +2074,13 @@
         <v>10</v>
       </c>
       <c r="C52">
-        <v>39418</v>
+        <v>39773</v>
       </c>
       <c r="D52">
-        <v>11283</v>
+        <v>11300</v>
       </c>
       <c r="E52">
-        <v>170470092</v>
+        <v>173785805</v>
       </c>
       <c r="F52" t="s">
         <v>16</v>
@@ -2103,13 +2103,13 @@
         <v>10</v>
       </c>
       <c r="C53">
-        <v>13979</v>
+        <v>14119</v>
       </c>
       <c r="D53">
-        <v>3944</v>
+        <v>3951</v>
       </c>
       <c r="E53">
-        <v>80300964</v>
+        <v>82363301</v>
       </c>
       <c r="F53" t="s">
         <v>16</v>
@@ -2132,13 +2132,13 @@
         <v>10</v>
       </c>
       <c r="C54">
-        <v>5980</v>
+        <v>6046</v>
       </c>
       <c r="D54">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="E54">
-        <v>65490483</v>
+        <v>66810802</v>
       </c>
       <c r="F54" t="s">
         <v>16</v>
@@ -2161,13 +2161,13 @@
         <v>10</v>
       </c>
       <c r="C55">
-        <v>1513</v>
+        <v>1534</v>
       </c>
       <c r="D55">
         <v>547</v>
       </c>
       <c r="E55">
-        <v>41864979</v>
+        <v>42840708</v>
       </c>
       <c r="F55" t="s">
         <v>16</v>
@@ -2190,13 +2190,13 @@
         <v>10</v>
       </c>
       <c r="C56">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D56">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E56">
-        <v>7654367</v>
+        <v>8182360</v>
       </c>
       <c r="F56" t="s">
         <v>16</v>
@@ -2277,13 +2277,13 @@
         <v>10</v>
       </c>
       <c r="C59">
-        <v>35173</v>
+        <v>35452</v>
       </c>
       <c r="D59">
-        <v>11066</v>
+        <v>11077</v>
       </c>
       <c r="E59">
-        <v>77744862</v>
+        <v>78737280</v>
       </c>
       <c r="F59" t="s">
         <v>16</v>
@@ -2306,13 +2306,13 @@
         <v>10</v>
       </c>
       <c r="C60">
-        <v>2971</v>
+        <v>2979</v>
       </c>
       <c r="D60">
         <v>774</v>
       </c>
       <c r="E60">
-        <v>5286343</v>
+        <v>5311476</v>
       </c>
       <c r="F60" t="s">
         <v>17</v>
@@ -2335,13 +2335,13 @@
         <v>10</v>
       </c>
       <c r="C61">
-        <v>9784</v>
+        <v>9816</v>
       </c>
       <c r="D61">
         <v>2744</v>
       </c>
       <c r="E61">
-        <v>18224062</v>
+        <v>18383032</v>
       </c>
       <c r="F61" t="s">
         <v>17</v>
@@ -2364,13 +2364,13 @@
         <v>10</v>
       </c>
       <c r="C62">
-        <v>3271</v>
+        <v>3280</v>
       </c>
       <c r="D62">
         <v>996</v>
       </c>
       <c r="E62">
-        <v>6980739</v>
+        <v>7014604</v>
       </c>
       <c r="F62" t="s">
         <v>17</v>
@@ -2393,13 +2393,13 @@
         <v>10</v>
       </c>
       <c r="C63">
-        <v>1107</v>
+        <v>1111</v>
       </c>
       <c r="D63">
         <v>359</v>
       </c>
       <c r="E63">
-        <v>2988762</v>
+        <v>3055153</v>
       </c>
       <c r="F63" t="s">
         <v>17</v>
@@ -2422,13 +2422,13 @@
         <v>10</v>
       </c>
       <c r="C64">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D64">
         <v>101</v>
       </c>
       <c r="E64">
-        <v>1146537</v>
+        <v>1166597</v>
       </c>
       <c r="F64" t="s">
         <v>17</v>
@@ -2509,13 +2509,13 @@
         <v>10</v>
       </c>
       <c r="C67">
-        <v>10661</v>
+        <v>10694</v>
       </c>
       <c r="D67">
         <v>2585</v>
       </c>
       <c r="E67">
-        <v>16767949</v>
+        <v>16812682</v>
       </c>
       <c r="F67" t="s">
         <v>17</v>
@@ -2538,13 +2538,13 @@
         <v>10</v>
       </c>
       <c r="C68">
-        <v>2001</v>
+        <v>2003</v>
       </c>
       <c r="D68">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E68">
-        <v>4548672</v>
+        <v>4553172</v>
       </c>
       <c r="F68" t="s">
         <v>18</v>
@@ -2567,13 +2567,13 @@
         <v>10</v>
       </c>
       <c r="C69">
-        <v>4775</v>
+        <v>4777</v>
       </c>
       <c r="D69">
         <v>944</v>
       </c>
       <c r="E69">
-        <v>10814676</v>
+        <v>10820676</v>
       </c>
       <c r="F69" t="s">
         <v>18</v>
@@ -2596,13 +2596,13 @@
         <v>10</v>
       </c>
       <c r="C70">
-        <v>1898</v>
+        <v>1904</v>
       </c>
       <c r="D70">
         <v>405</v>
       </c>
       <c r="E70">
-        <v>4739703</v>
+        <v>4760853</v>
       </c>
       <c r="F70" t="s">
         <v>18</v>
@@ -2712,13 +2712,13 @@
         <v>10</v>
       </c>
       <c r="C74">
-        <v>3189</v>
+        <v>3192</v>
       </c>
       <c r="D74">
         <v>551</v>
       </c>
       <c r="E74">
-        <v>6288809</v>
+        <v>6294809</v>
       </c>
       <c r="F74" t="s">
         <v>18</v>
@@ -2741,13 +2741,13 @@
         <v>10</v>
       </c>
       <c r="C75">
-        <v>27891</v>
+        <v>28072</v>
       </c>
       <c r="D75">
-        <v>7346</v>
+        <v>7351</v>
       </c>
       <c r="E75">
-        <v>67794088</v>
+        <v>68740040</v>
       </c>
       <c r="F75" t="s">
         <v>19</v>
@@ -2770,13 +2770,13 @@
         <v>10</v>
       </c>
       <c r="C76">
-        <v>82489</v>
+        <v>82994</v>
       </c>
       <c r="D76">
-        <v>22413</v>
+        <v>22422</v>
       </c>
       <c r="E76">
-        <v>251868988</v>
+        <v>255144690</v>
       </c>
       <c r="F76" t="s">
         <v>19</v>
@@ -2799,13 +2799,13 @@
         <v>10</v>
       </c>
       <c r="C77">
-        <v>31896</v>
+        <v>32150</v>
       </c>
       <c r="D77">
-        <v>8833</v>
+        <v>8838</v>
       </c>
       <c r="E77">
-        <v>134803158</v>
+        <v>137242167</v>
       </c>
       <c r="F77" t="s">
         <v>19</v>
@@ -2828,13 +2828,13 @@
         <v>10</v>
       </c>
       <c r="C78">
-        <v>10699</v>
+        <v>10791</v>
       </c>
       <c r="D78">
-        <v>3095</v>
+        <v>3097</v>
       </c>
       <c r="E78">
-        <v>57445450</v>
+        <v>58592561</v>
       </c>
       <c r="F78" t="s">
         <v>19</v>
@@ -2857,13 +2857,13 @@
         <v>10</v>
       </c>
       <c r="C79">
-        <v>4317</v>
+        <v>4378</v>
       </c>
       <c r="D79">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="E79">
-        <v>45193544</v>
+        <v>46560324</v>
       </c>
       <c r="F79" t="s">
         <v>19</v>
@@ -2886,13 +2886,13 @@
         <v>10</v>
       </c>
       <c r="C80">
-        <v>1491</v>
+        <v>1518</v>
       </c>
       <c r="D80">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="E80">
-        <v>39600827</v>
+        <v>40959722</v>
       </c>
       <c r="F80" t="s">
         <v>19</v>
@@ -2915,13 +2915,13 @@
         <v>10</v>
       </c>
       <c r="C81">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D81">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E81">
-        <v>4788129</v>
+        <v>4901197</v>
       </c>
       <c r="F81" t="s">
         <v>19</v>
@@ -2973,13 +2973,13 @@
         <v>10</v>
       </c>
       <c r="C83">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D83">
         <v>4</v>
       </c>
       <c r="E83">
-        <v>1200490</v>
+        <v>1400490</v>
       </c>
       <c r="F83" t="s">
         <v>19</v>
@@ -3002,13 +3002,13 @@
         <v>10</v>
       </c>
       <c r="C84">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D84">
         <v>4</v>
       </c>
       <c r="E84">
-        <v>479693</v>
+        <v>679693</v>
       </c>
       <c r="F84" t="s">
         <v>19</v>
@@ -3060,13 +3060,13 @@
         <v>10</v>
       </c>
       <c r="C86">
-        <v>25466</v>
+        <v>25593</v>
       </c>
       <c r="D86">
-        <v>7100</v>
+        <v>7102</v>
       </c>
       <c r="E86">
-        <v>44421597</v>
+        <v>44744666</v>
       </c>
       <c r="F86" t="s">
         <v>19</v>
@@ -3089,13 +3089,13 @@
         <v>10</v>
       </c>
       <c r="C87">
-        <v>103754</v>
+        <v>104326</v>
       </c>
       <c r="D87">
-        <v>24158</v>
+        <v>24170</v>
       </c>
       <c r="E87">
-        <v>264583192</v>
+        <v>267230108</v>
       </c>
       <c r="F87" t="s">
         <v>20</v>
@@ -3118,13 +3118,13 @@
         <v>10</v>
       </c>
       <c r="C88">
-        <v>280814</v>
+        <v>282490</v>
       </c>
       <c r="D88">
-        <v>69354</v>
+        <v>69385</v>
       </c>
       <c r="E88">
-        <v>833546146</v>
+        <v>844352852</v>
       </c>
       <c r="F88" t="s">
         <v>20</v>
@@ -3147,13 +3147,13 @@
         <v>10</v>
       </c>
       <c r="C89">
-        <v>134500</v>
+        <v>135501</v>
       </c>
       <c r="D89">
-        <v>33303</v>
+        <v>33326</v>
       </c>
       <c r="E89">
-        <v>583148396</v>
+        <v>592925361</v>
       </c>
       <c r="F89" t="s">
         <v>20</v>
@@ -3176,13 +3176,13 @@
         <v>10</v>
       </c>
       <c r="C90">
-        <v>54454</v>
+        <v>54965</v>
       </c>
       <c r="D90">
-        <v>13226</v>
+        <v>13236</v>
       </c>
       <c r="E90">
-        <v>338956645</v>
+        <v>345628640</v>
       </c>
       <c r="F90" t="s">
         <v>20</v>
@@ -3205,13 +3205,13 @@
         <v>10</v>
       </c>
       <c r="C91">
-        <v>24618</v>
+        <v>24948</v>
       </c>
       <c r="D91">
-        <v>6501</v>
+        <v>6514</v>
       </c>
       <c r="E91">
-        <v>284128617</v>
+        <v>291428543</v>
       </c>
       <c r="F91" t="s">
         <v>20</v>
@@ -3234,13 +3234,13 @@
         <v>10</v>
       </c>
       <c r="C92">
-        <v>6624</v>
+        <v>6714</v>
       </c>
       <c r="D92">
-        <v>2205</v>
+        <v>2207</v>
       </c>
       <c r="E92">
-        <v>196288666</v>
+        <v>201464794</v>
       </c>
       <c r="F92" t="s">
         <v>20</v>
@@ -3263,13 +3263,13 @@
         <v>10</v>
       </c>
       <c r="C93">
-        <v>568</v>
+        <v>582</v>
       </c>
       <c r="D93">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E93">
-        <v>41156095</v>
+        <v>42356070</v>
       </c>
       <c r="F93" t="s">
         <v>20</v>
@@ -3292,13 +3292,13 @@
         <v>10</v>
       </c>
       <c r="C94">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D94">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E94">
-        <v>19302548</v>
+        <v>19821676</v>
       </c>
       <c r="F94" t="s">
         <v>20</v>
@@ -3321,13 +3321,13 @@
         <v>10</v>
       </c>
       <c r="C95">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D95">
         <v>21</v>
       </c>
       <c r="E95">
-        <v>4519337</v>
+        <v>4719337</v>
       </c>
       <c r="F95" t="s">
         <v>20</v>
@@ -3379,13 +3379,13 @@
         <v>10</v>
       </c>
       <c r="C97">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D97">
         <v>18</v>
       </c>
       <c r="E97">
-        <v>4759376</v>
+        <v>5159376</v>
       </c>
       <c r="F97" t="s">
         <v>20</v>
@@ -3437,13 +3437,13 @@
         <v>10</v>
       </c>
       <c r="C99">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D99">
         <v>4</v>
       </c>
       <c r="E99">
-        <v>800000</v>
+        <v>1000000</v>
       </c>
       <c r="F99" t="s">
         <v>20</v>
@@ -3466,13 +3466,13 @@
         <v>10</v>
       </c>
       <c r="C100">
-        <v>96383</v>
+        <v>96913</v>
       </c>
       <c r="D100">
-        <v>22375</v>
+        <v>22385</v>
       </c>
       <c r="E100">
-        <v>171458343</v>
+        <v>172869655</v>
       </c>
       <c r="F100" t="s">
         <v>20</v>
@@ -3495,13 +3495,13 @@
         <v>10</v>
       </c>
       <c r="C101">
-        <v>6212</v>
+        <v>6222</v>
       </c>
       <c r="D101">
         <v>1886</v>
       </c>
       <c r="E101">
-        <v>10664403</v>
+        <v>10717912</v>
       </c>
       <c r="F101" t="s">
         <v>21</v>
@@ -3524,13 +3524,13 @@
         <v>10</v>
       </c>
       <c r="C102">
-        <v>14538</v>
+        <v>14572</v>
       </c>
       <c r="D102">
-        <v>4937</v>
+        <v>4939</v>
       </c>
       <c r="E102">
-        <v>25759327</v>
+        <v>25887321</v>
       </c>
       <c r="F102" t="s">
         <v>21</v>
@@ -3553,13 +3553,13 @@
         <v>10</v>
       </c>
       <c r="C103">
-        <v>4622</v>
+        <v>4625</v>
       </c>
       <c r="D103">
         <v>1830</v>
       </c>
       <c r="E103">
-        <v>9130046</v>
+        <v>9151999</v>
       </c>
       <c r="F103" t="s">
         <v>21</v>
@@ -3582,13 +3582,13 @@
         <v>10</v>
       </c>
       <c r="C104">
-        <v>1662</v>
+        <v>1664</v>
       </c>
       <c r="D104">
         <v>682</v>
       </c>
       <c r="E104">
-        <v>4045331</v>
+        <v>4080291</v>
       </c>
       <c r="F104" t="s">
         <v>21</v>
@@ -3611,13 +3611,13 @@
         <v>10</v>
       </c>
       <c r="C105">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="D105">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E105">
-        <v>3122986</v>
+        <v>3241319</v>
       </c>
       <c r="F105" t="s">
         <v>21</v>
@@ -3640,13 +3640,13 @@
         <v>10</v>
       </c>
       <c r="C106">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D106">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E106">
-        <v>1624960</v>
+        <v>1635027</v>
       </c>
       <c r="F106" t="s">
         <v>21</v>
@@ -3698,13 +3698,13 @@
         <v>10</v>
       </c>
       <c r="C108">
-        <v>6932</v>
+        <v>6948</v>
       </c>
       <c r="D108">
         <v>2058</v>
       </c>
       <c r="E108">
-        <v>9789311</v>
+        <v>9814612</v>
       </c>
       <c r="F108" t="s">
         <v>21</v>
@@ -3727,13 +3727,13 @@
         <v>10</v>
       </c>
       <c r="C109">
-        <v>2566</v>
+        <v>2579</v>
       </c>
       <c r="D109">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="E109">
-        <v>5278769</v>
+        <v>5314524</v>
       </c>
       <c r="F109" t="s">
         <v>22</v>
@@ -3756,13 +3756,13 @@
         <v>10</v>
       </c>
       <c r="C110">
-        <v>8044</v>
+        <v>8065</v>
       </c>
       <c r="D110">
         <v>2211</v>
       </c>
       <c r="E110">
-        <v>18029791</v>
+        <v>18162274</v>
       </c>
       <c r="F110" t="s">
         <v>22</v>
@@ -3785,13 +3785,13 @@
         <v>10</v>
       </c>
       <c r="C111">
-        <v>2875</v>
+        <v>2887</v>
       </c>
       <c r="D111">
         <v>932</v>
       </c>
       <c r="E111">
-        <v>7860010</v>
+        <v>8013518</v>
       </c>
       <c r="F111" t="s">
         <v>22</v>
@@ -3814,13 +3814,13 @@
         <v>10</v>
       </c>
       <c r="C112">
-        <v>1087</v>
+        <v>1091</v>
       </c>
       <c r="D112">
         <v>357</v>
       </c>
       <c r="E112">
-        <v>3325870</v>
+        <v>3388529</v>
       </c>
       <c r="F112" t="s">
         <v>22</v>
@@ -3843,13 +3843,13 @@
         <v>10</v>
       </c>
       <c r="C113">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D113">
         <v>138</v>
       </c>
       <c r="E113">
-        <v>1905342</v>
+        <v>1920361</v>
       </c>
       <c r="F113" t="s">
         <v>22</v>
@@ -3930,13 +3930,13 @@
         <v>10</v>
       </c>
       <c r="C116">
-        <v>5567</v>
+        <v>5577</v>
       </c>
       <c r="D116">
         <v>1404</v>
       </c>
       <c r="E116">
-        <v>8395241</v>
+        <v>8430291</v>
       </c>
       <c r="F116" t="s">
         <v>22</v>
@@ -3959,13 +3959,13 @@
         <v>10</v>
       </c>
       <c r="C117">
-        <v>1149</v>
+        <v>1153</v>
       </c>
       <c r="D117">
         <v>235</v>
       </c>
       <c r="E117">
-        <v>3073384</v>
+        <v>3111442</v>
       </c>
       <c r="F117" t="s">
         <v>23</v>
@@ -3988,13 +3988,13 @@
         <v>10</v>
       </c>
       <c r="C118">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D118">
         <v>135</v>
       </c>
       <c r="E118">
-        <v>2199659</v>
+        <v>2201159</v>
       </c>
       <c r="F118" t="s">
         <v>23</v>
@@ -4075,13 +4075,13 @@
         <v>10</v>
       </c>
       <c r="C121">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D121">
         <v>8</v>
       </c>
       <c r="E121">
-        <v>154123</v>
+        <v>155623</v>
       </c>
       <c r="F121" t="s">
         <v>23</v>
@@ -4133,13 +4133,13 @@
         <v>10</v>
       </c>
       <c r="C123">
-        <v>20299</v>
+        <v>20428</v>
       </c>
       <c r="D123">
         <v>5173</v>
       </c>
       <c r="E123">
-        <v>55788367</v>
+        <v>56468319</v>
       </c>
       <c r="F123" t="s">
         <v>24</v>
@@ -4162,13 +4162,13 @@
         <v>10</v>
       </c>
       <c r="C124">
-        <v>54060</v>
+        <v>54421</v>
       </c>
       <c r="D124">
-        <v>14916</v>
+        <v>14923</v>
       </c>
       <c r="E124">
-        <v>176364330</v>
+        <v>178935331</v>
       </c>
       <c r="F124" t="s">
         <v>24</v>
@@ -4191,13 +4191,13 @@
         <v>10</v>
       </c>
       <c r="C125">
-        <v>20308</v>
+        <v>20507</v>
       </c>
       <c r="D125">
-        <v>5673</v>
+        <v>5678</v>
       </c>
       <c r="E125">
-        <v>88629120</v>
+        <v>90552355</v>
       </c>
       <c r="F125" t="s">
         <v>24</v>
@@ -4220,13 +4220,13 @@
         <v>10</v>
       </c>
       <c r="C126">
-        <v>6819</v>
+        <v>6905</v>
       </c>
       <c r="D126">
-        <v>1964</v>
+        <v>1967</v>
       </c>
       <c r="E126">
-        <v>39782706</v>
+        <v>40836086</v>
       </c>
       <c r="F126" t="s">
         <v>24</v>
@@ -4249,13 +4249,13 @@
         <v>10</v>
       </c>
       <c r="C127">
-        <v>2676</v>
+        <v>2718</v>
       </c>
       <c r="D127">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="E127">
-        <v>29450974</v>
+        <v>30352480</v>
       </c>
       <c r="F127" t="s">
         <v>24</v>
@@ -4278,13 +4278,13 @@
         <v>10</v>
       </c>
       <c r="C128">
-        <v>780</v>
+        <v>803</v>
       </c>
       <c r="D128">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E128">
-        <v>20258944</v>
+        <v>21045030</v>
       </c>
       <c r="F128" t="s">
         <v>24</v>
@@ -4307,13 +4307,13 @@
         <v>10</v>
       </c>
       <c r="C129">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D129">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E129">
-        <v>2521321</v>
+        <v>3015244</v>
       </c>
       <c r="F129" t="s">
         <v>24</v>
@@ -4365,13 +4365,13 @@
         <v>10</v>
       </c>
       <c r="C131">
-        <v>15943</v>
+        <v>16019</v>
       </c>
       <c r="D131">
-        <v>4577</v>
+        <v>4580</v>
       </c>
       <c r="E131">
-        <v>27857658</v>
+        <v>28067993</v>
       </c>
       <c r="F131" t="s">
         <v>24</v>
@@ -4394,13 +4394,13 @@
         <v>10</v>
       </c>
       <c r="C132">
-        <v>56841</v>
+        <v>57213</v>
       </c>
       <c r="D132">
-        <v>14661</v>
+        <v>14668</v>
       </c>
       <c r="E132">
-        <v>158272871</v>
+        <v>160410542</v>
       </c>
       <c r="F132" t="s">
         <v>25</v>
@@ -4423,13 +4423,13 @@
         <v>10</v>
       </c>
       <c r="C133">
-        <v>119821</v>
+        <v>120678</v>
       </c>
       <c r="D133">
-        <v>34126</v>
+        <v>34158</v>
       </c>
       <c r="E133">
-        <v>378590871</v>
+        <v>384635011</v>
       </c>
       <c r="F133" t="s">
         <v>25</v>
@@ -4452,13 +4452,13 @@
         <v>10</v>
       </c>
       <c r="C134">
-        <v>43218</v>
+        <v>43586</v>
       </c>
       <c r="D134">
-        <v>12548</v>
+        <v>12563</v>
       </c>
       <c r="E134">
-        <v>184712340</v>
+        <v>188250575</v>
       </c>
       <c r="F134" t="s">
         <v>25</v>
@@ -4481,13 +4481,13 @@
         <v>10</v>
       </c>
       <c r="C135">
-        <v>14843</v>
+        <v>15013</v>
       </c>
       <c r="D135">
-        <v>4383</v>
+        <v>4388</v>
       </c>
       <c r="E135">
-        <v>84761773</v>
+        <v>86836000</v>
       </c>
       <c r="F135" t="s">
         <v>25</v>
@@ -4510,13 +4510,13 @@
         <v>10</v>
       </c>
       <c r="C136">
-        <v>6085</v>
+        <v>6165</v>
       </c>
       <c r="D136">
-        <v>1800</v>
+        <v>1801</v>
       </c>
       <c r="E136">
-        <v>67333922</v>
+        <v>68959843</v>
       </c>
       <c r="F136" t="s">
         <v>25</v>
@@ -4539,13 +4539,13 @@
         <v>10</v>
       </c>
       <c r="C137">
-        <v>1826</v>
+        <v>1852</v>
       </c>
       <c r="D137">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E137">
-        <v>52054519</v>
+        <v>53567846</v>
       </c>
       <c r="F137" t="s">
         <v>25</v>
@@ -4568,13 +4568,13 @@
         <v>10</v>
       </c>
       <c r="C138">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D138">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E138">
-        <v>6751046</v>
+        <v>6806586</v>
       </c>
       <c r="F138" t="s">
         <v>25</v>
@@ -4684,13 +4684,13 @@
         <v>10</v>
       </c>
       <c r="C142">
-        <v>42029</v>
+        <v>42272</v>
       </c>
       <c r="D142">
-        <v>12688</v>
+        <v>12707</v>
       </c>
       <c r="E142">
-        <v>72402119</v>
+        <v>73134157</v>
       </c>
       <c r="F142" t="s">
         <v>25</v>
@@ -4713,13 +4713,13 @@
         <v>10</v>
       </c>
       <c r="C143">
-        <v>69816</v>
+        <v>70290</v>
       </c>
       <c r="D143">
-        <v>16989</v>
+        <v>16991</v>
       </c>
       <c r="E143">
-        <v>195447744</v>
+        <v>198200628</v>
       </c>
       <c r="F143" t="s">
         <v>26</v>
@@ -4742,13 +4742,13 @@
         <v>10</v>
       </c>
       <c r="C144">
-        <v>143108</v>
+        <v>144081</v>
       </c>
       <c r="D144">
-        <v>38414</v>
+        <v>38442</v>
       </c>
       <c r="E144">
-        <v>444743181</v>
+        <v>450946133</v>
       </c>
       <c r="F144" t="s">
         <v>26</v>
@@ -4771,13 +4771,13 @@
         <v>10</v>
       </c>
       <c r="C145">
-        <v>48829</v>
+        <v>49191</v>
       </c>
       <c r="D145">
-        <v>13508</v>
+        <v>13520</v>
       </c>
       <c r="E145">
-        <v>209649417</v>
+        <v>213278720</v>
       </c>
       <c r="F145" t="s">
         <v>26</v>
@@ -4800,13 +4800,13 @@
         <v>10</v>
       </c>
       <c r="C146">
-        <v>15648</v>
+        <v>15830</v>
       </c>
       <c r="D146">
-        <v>4446</v>
+        <v>4452</v>
       </c>
       <c r="E146">
-        <v>88806932</v>
+        <v>90873902</v>
       </c>
       <c r="F146" t="s">
         <v>26</v>
@@ -4829,13 +4829,13 @@
         <v>10</v>
       </c>
       <c r="C147">
-        <v>6226</v>
+        <v>6330</v>
       </c>
       <c r="D147">
-        <v>1835</v>
+        <v>1840</v>
       </c>
       <c r="E147">
-        <v>65623892</v>
+        <v>67531595</v>
       </c>
       <c r="F147" t="s">
         <v>26</v>
@@ -4858,13 +4858,13 @@
         <v>10</v>
       </c>
       <c r="C148">
-        <v>1666</v>
+        <v>1708</v>
       </c>
       <c r="D148">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E148">
-        <v>48660147</v>
+        <v>50480419</v>
       </c>
       <c r="F148" t="s">
         <v>26</v>
@@ -4887,13 +4887,13 @@
         <v>10</v>
       </c>
       <c r="C149">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D149">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E149">
-        <v>6978191</v>
+        <v>7175738</v>
       </c>
       <c r="F149" t="s">
         <v>26</v>
@@ -4916,13 +4916,13 @@
         <v>10</v>
       </c>
       <c r="C150">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D150">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E150">
-        <v>2371328</v>
+        <v>2391182</v>
       </c>
       <c r="F150" t="s">
         <v>26</v>
@@ -5003,13 +5003,13 @@
         <v>10</v>
       </c>
       <c r="C153">
-        <v>53015</v>
+        <v>53261</v>
       </c>
       <c r="D153">
-        <v>15112</v>
+        <v>15118</v>
       </c>
       <c r="E153">
-        <v>87687219</v>
+        <v>88304269</v>
       </c>
       <c r="F153" t="s">
         <v>26</v>
@@ -5032,13 +5032,13 @@
         <v>10</v>
       </c>
       <c r="C154">
-        <v>24571</v>
+        <v>24713</v>
       </c>
       <c r="D154">
-        <v>6393</v>
+        <v>6396</v>
       </c>
       <c r="E154">
-        <v>68312262</v>
+        <v>69203752</v>
       </c>
       <c r="F154" t="s">
         <v>27</v>
@@ -5061,13 +5061,13 @@
         <v>10</v>
       </c>
       <c r="C155">
-        <v>59752</v>
+        <v>60112</v>
       </c>
       <c r="D155">
-        <v>16811</v>
+        <v>16820</v>
       </c>
       <c r="E155">
-        <v>199414555</v>
+        <v>202181883</v>
       </c>
       <c r="F155" t="s">
         <v>27</v>
@@ -5090,13 +5090,13 @@
         <v>10</v>
       </c>
       <c r="C156">
-        <v>23889</v>
+        <v>24083</v>
       </c>
       <c r="D156">
-        <v>6906</v>
+        <v>6907</v>
       </c>
       <c r="E156">
-        <v>105670980</v>
+        <v>107645688</v>
       </c>
       <c r="F156" t="s">
         <v>27</v>
@@ -5119,13 +5119,13 @@
         <v>10</v>
       </c>
       <c r="C157">
-        <v>7440</v>
+        <v>7502</v>
       </c>
       <c r="D157">
         <v>2324</v>
       </c>
       <c r="E157">
-        <v>43299917</v>
+        <v>44099620</v>
       </c>
       <c r="F157" t="s">
         <v>27</v>
@@ -5148,13 +5148,13 @@
         <v>10</v>
       </c>
       <c r="C158">
-        <v>3033</v>
+        <v>3081</v>
       </c>
       <c r="D158">
-        <v>987</v>
+        <v>990</v>
       </c>
       <c r="E158">
-        <v>35397010</v>
+        <v>36276970</v>
       </c>
       <c r="F158" t="s">
         <v>27</v>
@@ -5177,13 +5177,13 @@
         <v>10</v>
       </c>
       <c r="C159">
-        <v>966</v>
+        <v>979</v>
       </c>
       <c r="D159">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E159">
-        <v>27933198</v>
+        <v>28374295</v>
       </c>
       <c r="F159" t="s">
         <v>27</v>
@@ -5264,13 +5264,13 @@
         <v>10</v>
       </c>
       <c r="C162">
-        <v>17407</v>
+        <v>17481</v>
       </c>
       <c r="D162">
         <v>5143</v>
       </c>
       <c r="E162">
-        <v>30383124</v>
+        <v>30631764</v>
       </c>
       <c r="F162" t="s">
         <v>27</v>
@@ -5293,13 +5293,13 @@
         <v>10</v>
       </c>
       <c r="C163">
-        <v>68545</v>
+        <v>69082</v>
       </c>
       <c r="D163">
-        <v>16518</v>
+        <v>16529</v>
       </c>
       <c r="E163">
-        <v>189563873</v>
+        <v>192400726</v>
       </c>
       <c r="F163" t="s">
         <v>28</v>
@@ -5322,13 +5322,13 @@
         <v>10</v>
       </c>
       <c r="C164">
-        <v>159389</v>
+        <v>160477</v>
       </c>
       <c r="D164">
-        <v>40182</v>
+        <v>40203</v>
       </c>
       <c r="E164">
-        <v>508723488</v>
+        <v>515832830</v>
       </c>
       <c r="F164" t="s">
         <v>28</v>
@@ -5351,13 +5351,13 @@
         <v>10</v>
       </c>
       <c r="C165">
-        <v>53821</v>
+        <v>54299</v>
       </c>
       <c r="D165">
-        <v>13718</v>
+        <v>13728</v>
       </c>
       <c r="E165">
-        <v>244015689</v>
+        <v>248494871</v>
       </c>
       <c r="F165" t="s">
         <v>28</v>
@@ -5380,13 +5380,13 @@
         <v>10</v>
       </c>
       <c r="C166">
-        <v>17627</v>
+        <v>17867</v>
       </c>
       <c r="D166">
-        <v>4532</v>
+        <v>4537</v>
       </c>
       <c r="E166">
-        <v>111879147</v>
+        <v>115002219</v>
       </c>
       <c r="F166" t="s">
         <v>28</v>
@@ -5409,13 +5409,13 @@
         <v>10</v>
       </c>
       <c r="C167">
-        <v>7761</v>
+        <v>7871</v>
       </c>
       <c r="D167">
-        <v>2096</v>
+        <v>2098</v>
       </c>
       <c r="E167">
-        <v>89566728</v>
+        <v>92011909</v>
       </c>
       <c r="F167" t="s">
         <v>28</v>
@@ -5438,13 +5438,13 @@
         <v>10</v>
       </c>
       <c r="C168">
-        <v>2168</v>
+        <v>2215</v>
       </c>
       <c r="D168">
         <v>737</v>
       </c>
       <c r="E168">
-        <v>65019460</v>
+        <v>67208837</v>
       </c>
       <c r="F168" t="s">
         <v>28</v>
@@ -5467,13 +5467,13 @@
         <v>10</v>
       </c>
       <c r="C169">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="D169">
         <v>96</v>
       </c>
       <c r="E169">
-        <v>14572639</v>
+        <v>15042644</v>
       </c>
       <c r="F169" t="s">
         <v>28</v>
@@ -5583,13 +5583,13 @@
         <v>10</v>
       </c>
       <c r="C173">
-        <v>50330</v>
+        <v>50609</v>
       </c>
       <c r="D173">
-        <v>13398</v>
+        <v>13408</v>
       </c>
       <c r="E173">
-        <v>86607151</v>
+        <v>87350265</v>
       </c>
       <c r="F173" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2021-03-30 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-classe-effectif-latest.xlsx
@@ -624,13 +624,13 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>74045</v>
+        <v>74392</v>
       </c>
       <c r="D2">
-        <v>18690</v>
+        <v>18705</v>
       </c>
       <c r="E2">
-        <v>202594094</v>
+        <v>204151571</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -653,13 +653,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>180252</v>
+        <v>181093</v>
       </c>
       <c r="D3">
-        <v>46713</v>
+        <v>46749</v>
       </c>
       <c r="E3">
-        <v>614692630</v>
+        <v>620202667</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -682,13 +682,13 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>70436</v>
+        <v>70821</v>
       </c>
       <c r="D4">
-        <v>18292</v>
+        <v>18322</v>
       </c>
       <c r="E4">
-        <v>337995526</v>
+        <v>341661190</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -711,13 +711,13 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>24919</v>
+        <v>25086</v>
       </c>
       <c r="D5">
-        <v>6387</v>
+        <v>6395</v>
       </c>
       <c r="E5">
-        <v>170804194</v>
+        <v>173118147</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -740,13 +740,13 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>11395</v>
+        <v>11484</v>
       </c>
       <c r="D6">
-        <v>3069</v>
+        <v>3075</v>
       </c>
       <c r="E6">
-        <v>147064877</v>
+        <v>149050589</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -769,13 +769,13 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>3255</v>
+        <v>3299</v>
       </c>
       <c r="D7">
-        <v>1075</v>
+        <v>1083</v>
       </c>
       <c r="E7">
-        <v>99297800</v>
+        <v>101163208</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -798,13 +798,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="D8">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E8">
-        <v>25298316</v>
+        <v>25498895</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -827,13 +827,13 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D9">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9">
-        <v>9841504</v>
+        <v>9841505</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -856,13 +856,13 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10">
-        <v>1451500</v>
+        <v>1451501</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -972,13 +972,13 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>78743</v>
+        <v>79203</v>
       </c>
       <c r="D14">
-        <v>20459</v>
+        <v>20477</v>
       </c>
       <c r="E14">
-        <v>148828258</v>
+        <v>150224666</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -1001,13 +1001,13 @@
         <v>10</v>
       </c>
       <c r="C15">
-        <v>18461</v>
+        <v>18544</v>
       </c>
       <c r="D15">
-        <v>4753</v>
+        <v>4760</v>
       </c>
       <c r="E15">
-        <v>49994693</v>
+        <v>50409470</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
@@ -1030,13 +1030,13 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>50377</v>
+        <v>50559</v>
       </c>
       <c r="D16">
-        <v>13367</v>
+        <v>13383</v>
       </c>
       <c r="E16">
-        <v>169538756</v>
+        <v>170774075</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -1059,13 +1059,13 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>17891</v>
+        <v>17985</v>
       </c>
       <c r="D17">
-        <v>4849</v>
+        <v>4862</v>
       </c>
       <c r="E17">
-        <v>80897798</v>
+        <v>81679702</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -1088,13 +1088,13 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>5660</v>
+        <v>5700</v>
       </c>
       <c r="D18">
-        <v>1559</v>
+        <v>1564</v>
       </c>
       <c r="E18">
-        <v>34364086</v>
+        <v>34834377</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -1117,13 +1117,13 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>2393</v>
+        <v>2413</v>
       </c>
       <c r="D19">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="E19">
-        <v>27346078</v>
+        <v>27784759</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -1146,13 +1146,13 @@
         <v>10</v>
       </c>
       <c r="C20">
-        <v>789</v>
+        <v>802</v>
       </c>
       <c r="D20">
         <v>261</v>
       </c>
       <c r="E20">
-        <v>19539189</v>
+        <v>20100870</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -1175,13 +1175,13 @@
         <v>10</v>
       </c>
       <c r="C21">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21">
         <v>21</v>
       </c>
       <c r="E21">
-        <v>3442156</v>
+        <v>3509669</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -1233,13 +1233,13 @@
         <v>10</v>
       </c>
       <c r="C23">
-        <v>17932</v>
+        <v>18013</v>
       </c>
       <c r="D23">
-        <v>4980</v>
+        <v>4991</v>
       </c>
       <c r="E23">
-        <v>32338762</v>
+        <v>32565981</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
@@ -1262,13 +1262,13 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>26377</v>
+        <v>26483</v>
       </c>
       <c r="D24">
-        <v>6422</v>
+        <v>6424</v>
       </c>
       <c r="E24">
-        <v>81985824</v>
+        <v>82553488</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
@@ -1291,13 +1291,13 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>62840</v>
+        <v>63092</v>
       </c>
       <c r="D25">
-        <v>16287</v>
+        <v>16295</v>
       </c>
       <c r="E25">
-        <v>228868086</v>
+        <v>230667929</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
@@ -1320,13 +1320,13 @@
         <v>10</v>
       </c>
       <c r="C26">
-        <v>23439</v>
+        <v>23537</v>
       </c>
       <c r="D26">
-        <v>6347</v>
+        <v>6354</v>
       </c>
       <c r="E26">
-        <v>112781829</v>
+        <v>113571355</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
@@ -1349,13 +1349,13 @@
         <v>10</v>
       </c>
       <c r="C27">
-        <v>7602</v>
+        <v>7644</v>
       </c>
       <c r="D27">
-        <v>2142</v>
+        <v>2148</v>
       </c>
       <c r="E27">
-        <v>48787949</v>
+        <v>49283343</v>
       </c>
       <c r="F27" t="s">
         <v>13</v>
@@ -1378,13 +1378,13 @@
         <v>10</v>
       </c>
       <c r="C28">
-        <v>3126</v>
+        <v>3144</v>
       </c>
       <c r="D28">
-        <v>928</v>
+        <v>931</v>
       </c>
       <c r="E28">
-        <v>36218590</v>
+        <v>36520376</v>
       </c>
       <c r="F28" t="s">
         <v>13</v>
@@ -1407,13 +1407,13 @@
         <v>10</v>
       </c>
       <c r="C29">
-        <v>858</v>
+        <v>864</v>
       </c>
       <c r="D29">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E29">
-        <v>27850358</v>
+        <v>28045462</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
@@ -1436,13 +1436,13 @@
         <v>10</v>
       </c>
       <c r="C30">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D30">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E30">
-        <v>3119188</v>
+        <v>3119189</v>
       </c>
       <c r="F30" t="s">
         <v>13</v>
@@ -1523,13 +1523,13 @@
         <v>10</v>
       </c>
       <c r="C33">
-        <v>19661</v>
+        <v>19740</v>
       </c>
       <c r="D33">
-        <v>5546</v>
+        <v>5548</v>
       </c>
       <c r="E33">
-        <v>36000259</v>
+        <v>36220225</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
@@ -1552,13 +1552,13 @@
         <v>10</v>
       </c>
       <c r="C34">
-        <v>14402</v>
+        <v>14458</v>
       </c>
       <c r="D34">
-        <v>3728</v>
+        <v>3731</v>
       </c>
       <c r="E34">
-        <v>39034487</v>
+        <v>39362320</v>
       </c>
       <c r="F34" t="s">
         <v>14</v>
@@ -1581,13 +1581,13 @@
         <v>10</v>
       </c>
       <c r="C35">
-        <v>42387</v>
+        <v>42541</v>
       </c>
       <c r="D35">
-        <v>11501</v>
+        <v>11508</v>
       </c>
       <c r="E35">
-        <v>137784448</v>
+        <v>138820563</v>
       </c>
       <c r="F35" t="s">
         <v>14</v>
@@ -1610,13 +1610,13 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>16223</v>
+        <v>16281</v>
       </c>
       <c r="D36">
-        <v>4551</v>
+        <v>4556</v>
       </c>
       <c r="E36">
-        <v>71557760</v>
+        <v>72060541</v>
       </c>
       <c r="F36" t="s">
         <v>14</v>
@@ -1639,13 +1639,13 @@
         <v>10</v>
       </c>
       <c r="C37">
-        <v>4810</v>
+        <v>4843</v>
       </c>
       <c r="D37">
-        <v>1364</v>
+        <v>1371</v>
       </c>
       <c r="E37">
-        <v>28285923</v>
+        <v>28607988</v>
       </c>
       <c r="F37" t="s">
         <v>14</v>
@@ -1668,13 +1668,13 @@
         <v>10</v>
       </c>
       <c r="C38">
-        <v>1996</v>
+        <v>2007</v>
       </c>
       <c r="D38">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="E38">
-        <v>23842534</v>
+        <v>24051258</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -1697,13 +1697,13 @@
         <v>10</v>
       </c>
       <c r="C39">
-        <v>525</v>
+        <v>535</v>
       </c>
       <c r="D39">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E39">
-        <v>13264222</v>
+        <v>13477675</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
@@ -1726,13 +1726,13 @@
         <v>10</v>
       </c>
       <c r="C40">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D40">
         <v>14</v>
       </c>
       <c r="E40">
-        <v>1990172</v>
+        <v>2031704</v>
       </c>
       <c r="F40" t="s">
         <v>14</v>
@@ -1755,13 +1755,13 @@
         <v>10</v>
       </c>
       <c r="C41">
-        <v>14174</v>
+        <v>14225</v>
       </c>
       <c r="D41">
-        <v>3917</v>
+        <v>3921</v>
       </c>
       <c r="E41">
-        <v>25301749</v>
+        <v>25485012</v>
       </c>
       <c r="F41" t="s">
         <v>14</v>
@@ -1784,13 +1784,13 @@
         <v>10</v>
       </c>
       <c r="C42">
-        <v>7339</v>
+        <v>7375</v>
       </c>
       <c r="D42">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="E42">
-        <v>24623818</v>
+        <v>24817735</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
@@ -1813,13 +1813,13 @@
         <v>10</v>
       </c>
       <c r="C43">
-        <v>16550</v>
+        <v>16614</v>
       </c>
       <c r="D43">
-        <v>3776</v>
+        <v>3778</v>
       </c>
       <c r="E43">
-        <v>58349352</v>
+        <v>58738030</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
@@ -1842,13 +1842,13 @@
         <v>10</v>
       </c>
       <c r="C44">
-        <v>7437</v>
+        <v>7470</v>
       </c>
       <c r="D44">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="E44">
-        <v>36816061</v>
+        <v>37069201</v>
       </c>
       <c r="F44" t="s">
         <v>15</v>
@@ -1871,13 +1871,13 @@
         <v>10</v>
       </c>
       <c r="C45">
-        <v>2368</v>
+        <v>2387</v>
       </c>
       <c r="D45">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="E45">
-        <v>16347271</v>
+        <v>16616170</v>
       </c>
       <c r="F45" t="s">
         <v>15</v>
@@ -1900,13 +1900,13 @@
         <v>10</v>
       </c>
       <c r="C46">
-        <v>954</v>
+        <v>965</v>
       </c>
       <c r="D46">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E46">
-        <v>12650832</v>
+        <v>12855785</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
@@ -1929,13 +1929,13 @@
         <v>10</v>
       </c>
       <c r="C47">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D47">
         <v>72</v>
       </c>
       <c r="E47">
-        <v>7308267</v>
+        <v>7363342</v>
       </c>
       <c r="F47" t="s">
         <v>15</v>
@@ -1958,13 +1958,13 @@
         <v>10</v>
       </c>
       <c r="C48">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D48">
         <v>10</v>
       </c>
       <c r="E48">
-        <v>1825852</v>
+        <v>1852533</v>
       </c>
       <c r="F48" t="s">
         <v>15</v>
@@ -1987,13 +1987,13 @@
         <v>10</v>
       </c>
       <c r="C49">
-        <v>4646</v>
+        <v>4665</v>
       </c>
       <c r="D49">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="E49">
-        <v>8079294</v>
+        <v>8108452</v>
       </c>
       <c r="F49" t="s">
         <v>15</v>
@@ -2016,13 +2016,13 @@
         <v>10</v>
       </c>
       <c r="C50">
-        <v>33927</v>
+        <v>34126</v>
       </c>
       <c r="D50">
-        <v>9230</v>
+        <v>9239</v>
       </c>
       <c r="E50">
-        <v>93944031</v>
+        <v>94885356</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
@@ -2045,13 +2045,13 @@
         <v>10</v>
       </c>
       <c r="C51">
-        <v>101670</v>
+        <v>102293</v>
       </c>
       <c r="D51">
-        <v>28219</v>
+        <v>28260</v>
       </c>
       <c r="E51">
-        <v>343445906</v>
+        <v>347177072</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
@@ -2074,13 +2074,13 @@
         <v>10</v>
       </c>
       <c r="C52">
-        <v>41187</v>
+        <v>41425</v>
       </c>
       <c r="D52">
-        <v>11375</v>
+        <v>11402</v>
       </c>
       <c r="E52">
-        <v>186930193</v>
+        <v>188977826</v>
       </c>
       <c r="F52" t="s">
         <v>16</v>
@@ -2103,13 +2103,13 @@
         <v>10</v>
       </c>
       <c r="C53">
-        <v>14742</v>
+        <v>14835</v>
       </c>
       <c r="D53">
-        <v>3975</v>
+        <v>3984</v>
       </c>
       <c r="E53">
-        <v>89661985</v>
+        <v>90689624</v>
       </c>
       <c r="F53" t="s">
         <v>16</v>
@@ -2132,13 +2132,13 @@
         <v>10</v>
       </c>
       <c r="C54">
-        <v>6422</v>
+        <v>6473</v>
       </c>
       <c r="D54">
-        <v>1705</v>
+        <v>1713</v>
       </c>
       <c r="E54">
-        <v>74844907</v>
+        <v>75729149</v>
       </c>
       <c r="F54" t="s">
         <v>16</v>
@@ -2161,13 +2161,13 @@
         <v>10</v>
       </c>
       <c r="C55">
-        <v>1660</v>
+        <v>1691</v>
       </c>
       <c r="D55">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="E55">
-        <v>48749507</v>
+        <v>49807344</v>
       </c>
       <c r="F55" t="s">
         <v>16</v>
@@ -2277,13 +2277,13 @@
         <v>10</v>
       </c>
       <c r="C59">
-        <v>36961</v>
+        <v>37305</v>
       </c>
       <c r="D59">
-        <v>11157</v>
+        <v>11183</v>
       </c>
       <c r="E59">
-        <v>83853792</v>
+        <v>85313946</v>
       </c>
       <c r="F59" t="s">
         <v>16</v>
@@ -2306,13 +2306,13 @@
         <v>10</v>
       </c>
       <c r="C60">
-        <v>3019</v>
+        <v>3027</v>
       </c>
       <c r="D60">
         <v>774</v>
       </c>
       <c r="E60">
-        <v>5416554</v>
+        <v>5435796</v>
       </c>
       <c r="F60" t="s">
         <v>17</v>
@@ -2335,13 +2335,13 @@
         <v>10</v>
       </c>
       <c r="C61">
-        <v>9940</v>
+        <v>9975</v>
       </c>
       <c r="D61">
-        <v>2747</v>
+        <v>2748</v>
       </c>
       <c r="E61">
-        <v>18897666</v>
+        <v>19101864</v>
       </c>
       <c r="F61" t="s">
         <v>17</v>
@@ -2364,13 +2364,13 @@
         <v>10</v>
       </c>
       <c r="C62">
-        <v>3307</v>
+        <v>3313</v>
       </c>
       <c r="D62">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="E62">
-        <v>7193413</v>
+        <v>7237113</v>
       </c>
       <c r="F62" t="s">
         <v>17</v>
@@ -2393,13 +2393,13 @@
         <v>10</v>
       </c>
       <c r="C63">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="D63">
         <v>359</v>
       </c>
       <c r="E63">
-        <v>3088153</v>
+        <v>3110771</v>
       </c>
       <c r="F63" t="s">
         <v>17</v>
@@ -2422,13 +2422,13 @@
         <v>10</v>
       </c>
       <c r="C64">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D64">
         <v>103</v>
       </c>
       <c r="E64">
-        <v>1387845</v>
+        <v>1401588</v>
       </c>
       <c r="F64" t="s">
         <v>17</v>
@@ -2509,13 +2509,13 @@
         <v>10</v>
       </c>
       <c r="C67">
-        <v>10943</v>
+        <v>10989</v>
       </c>
       <c r="D67">
         <v>2593</v>
       </c>
       <c r="E67">
-        <v>17149089</v>
+        <v>17244167</v>
       </c>
       <c r="F67" t="s">
         <v>17</v>
@@ -2538,13 +2538,13 @@
         <v>10</v>
       </c>
       <c r="C68">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="D68">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E68">
-        <v>4612991</v>
+        <v>4614491</v>
       </c>
       <c r="F68" t="s">
         <v>18</v>
@@ -2567,13 +2567,13 @@
         <v>10</v>
       </c>
       <c r="C69">
-        <v>4822</v>
+        <v>4823</v>
       </c>
       <c r="D69">
         <v>944</v>
       </c>
       <c r="E69">
-        <v>10993763</v>
+        <v>11003763</v>
       </c>
       <c r="F69" t="s">
         <v>18</v>
@@ -2596,13 +2596,13 @@
         <v>10</v>
       </c>
       <c r="C70">
-        <v>1911</v>
+        <v>1914</v>
       </c>
       <c r="D70">
         <v>405</v>
       </c>
       <c r="E70">
-        <v>4807835</v>
+        <v>4837835</v>
       </c>
       <c r="F70" t="s">
         <v>18</v>
@@ -2654,13 +2654,13 @@
         <v>10</v>
       </c>
       <c r="C72">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D72">
         <v>56</v>
       </c>
       <c r="E72">
-        <v>709716</v>
+        <v>755765</v>
       </c>
       <c r="F72" t="s">
         <v>18</v>
@@ -2712,13 +2712,13 @@
         <v>10</v>
       </c>
       <c r="C74">
-        <v>3232</v>
+        <v>3236</v>
       </c>
       <c r="D74">
         <v>551</v>
       </c>
       <c r="E74">
-        <v>6360362</v>
+        <v>6364404</v>
       </c>
       <c r="F74" t="s">
         <v>18</v>
@@ -2741,13 +2741,13 @@
         <v>10</v>
       </c>
       <c r="C75">
-        <v>28808</v>
+        <v>28912</v>
       </c>
       <c r="D75">
-        <v>7362</v>
+        <v>7366</v>
       </c>
       <c r="E75">
-        <v>72036512</v>
+        <v>72408671</v>
       </c>
       <c r="F75" t="s">
         <v>19</v>
@@ -2770,13 +2770,13 @@
         <v>10</v>
       </c>
       <c r="C76">
-        <v>85295</v>
+        <v>85604</v>
       </c>
       <c r="D76">
-        <v>22461</v>
+        <v>22474</v>
       </c>
       <c r="E76">
-        <v>269928007</v>
+        <v>271600736</v>
       </c>
       <c r="F76" t="s">
         <v>19</v>
@@ -2799,13 +2799,13 @@
         <v>10</v>
       </c>
       <c r="C77">
-        <v>33230</v>
+        <v>33368</v>
       </c>
       <c r="D77">
-        <v>8862</v>
+        <v>8870</v>
       </c>
       <c r="E77">
-        <v>146673668</v>
+        <v>147922520</v>
       </c>
       <c r="F77" t="s">
         <v>19</v>
@@ -2828,13 +2828,13 @@
         <v>10</v>
       </c>
       <c r="C78">
-        <v>11208</v>
+        <v>11267</v>
       </c>
       <c r="D78">
-        <v>3104</v>
+        <v>3115</v>
       </c>
       <c r="E78">
-        <v>63391286</v>
+        <v>63936149</v>
       </c>
       <c r="F78" t="s">
         <v>19</v>
@@ -2857,13 +2857,13 @@
         <v>10</v>
       </c>
       <c r="C79">
-        <v>4601</v>
+        <v>4642</v>
       </c>
       <c r="D79">
-        <v>1292</v>
+        <v>1297</v>
       </c>
       <c r="E79">
-        <v>50605713</v>
+        <v>51285511</v>
       </c>
       <c r="F79" t="s">
         <v>19</v>
@@ -2886,13 +2886,13 @@
         <v>10</v>
       </c>
       <c r="C80">
-        <v>1621</v>
+        <v>1638</v>
       </c>
       <c r="D80">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="E80">
-        <v>45280773</v>
+        <v>46035819</v>
       </c>
       <c r="F80" t="s">
         <v>19</v>
@@ -2915,13 +2915,13 @@
         <v>10</v>
       </c>
       <c r="C81">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D81">
         <v>46</v>
       </c>
       <c r="E81">
-        <v>7042079</v>
+        <v>7072904</v>
       </c>
       <c r="F81" t="s">
         <v>19</v>
@@ -3002,13 +3002,13 @@
         <v>10</v>
       </c>
       <c r="C84">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D84">
         <v>5</v>
       </c>
       <c r="E84">
-        <v>746386</v>
+        <v>810705</v>
       </c>
       <c r="F84" t="s">
         <v>19</v>
@@ -3060,13 +3060,13 @@
         <v>10</v>
       </c>
       <c r="C86">
-        <v>26161</v>
+        <v>26232</v>
       </c>
       <c r="D86">
-        <v>7129</v>
+        <v>7134</v>
       </c>
       <c r="E86">
-        <v>46270577</v>
+        <v>46453439</v>
       </c>
       <c r="F86" t="s">
         <v>19</v>
@@ -3089,13 +3089,13 @@
         <v>10</v>
       </c>
       <c r="C87">
-        <v>107087</v>
+        <v>107492</v>
       </c>
       <c r="D87">
-        <v>24247</v>
+        <v>24263</v>
       </c>
       <c r="E87">
-        <v>280232509</v>
+        <v>282009929</v>
       </c>
       <c r="F87" t="s">
         <v>20</v>
@@ -3118,13 +3118,13 @@
         <v>10</v>
       </c>
       <c r="C88">
-        <v>290035</v>
+        <v>291169</v>
       </c>
       <c r="D88">
-        <v>69579</v>
+        <v>69633</v>
       </c>
       <c r="E88">
-        <v>889299732</v>
+        <v>895318917</v>
       </c>
       <c r="F88" t="s">
         <v>20</v>
@@ -3147,13 +3147,13 @@
         <v>10</v>
       </c>
       <c r="C89">
-        <v>139811</v>
+        <v>140401</v>
       </c>
       <c r="D89">
-        <v>33435</v>
+        <v>33464</v>
       </c>
       <c r="E89">
-        <v>634833515</v>
+        <v>640140839</v>
       </c>
       <c r="F89" t="s">
         <v>20</v>
@@ -3176,13 +3176,13 @@
         <v>10</v>
       </c>
       <c r="C90">
-        <v>57120</v>
+        <v>57432</v>
       </c>
       <c r="D90">
-        <v>13290</v>
+        <v>13310</v>
       </c>
       <c r="E90">
-        <v>375322945</v>
+        <v>379074036</v>
       </c>
       <c r="F90" t="s">
         <v>20</v>
@@ -3205,13 +3205,13 @@
         <v>10</v>
       </c>
       <c r="C91">
-        <v>26322</v>
+        <v>26515</v>
       </c>
       <c r="D91">
-        <v>6584</v>
+        <v>6602</v>
       </c>
       <c r="E91">
-        <v>323156334</v>
+        <v>326890788</v>
       </c>
       <c r="F91" t="s">
         <v>20</v>
@@ -3234,13 +3234,13 @@
         <v>10</v>
       </c>
       <c r="C92">
-        <v>7230</v>
+        <v>7313</v>
       </c>
       <c r="D92">
-        <v>2265</v>
+        <v>2275</v>
       </c>
       <c r="E92">
-        <v>228189026</v>
+        <v>231851317</v>
       </c>
       <c r="F92" t="s">
         <v>20</v>
@@ -3263,13 +3263,13 @@
         <v>10</v>
       </c>
       <c r="C93">
-        <v>663</v>
+        <v>677</v>
       </c>
       <c r="D93">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E93">
-        <v>51839890</v>
+        <v>52991432</v>
       </c>
       <c r="F93" t="s">
         <v>20</v>
@@ -3292,13 +3292,13 @@
         <v>10</v>
       </c>
       <c r="C94">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D94">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E94">
-        <v>25756665</v>
+        <v>25977965</v>
       </c>
       <c r="F94" t="s">
         <v>20</v>
@@ -3321,13 +3321,13 @@
         <v>10</v>
       </c>
       <c r="C95">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D95">
         <v>24</v>
       </c>
       <c r="E95">
-        <v>5539887</v>
+        <v>5939887</v>
       </c>
       <c r="F95" t="s">
         <v>20</v>
@@ -3379,13 +3379,13 @@
         <v>10</v>
       </c>
       <c r="C97">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D97">
         <v>20</v>
       </c>
       <c r="E97">
-        <v>5559376</v>
+        <v>5959376</v>
       </c>
       <c r="F97" t="s">
         <v>20</v>
@@ -3408,13 +3408,13 @@
         <v>10</v>
       </c>
       <c r="C98">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D98">
         <v>9</v>
       </c>
       <c r="E98">
-        <v>2620260</v>
+        <v>2820260</v>
       </c>
       <c r="F98" t="s">
         <v>20</v>
@@ -3466,13 +3466,13 @@
         <v>10</v>
       </c>
       <c r="C100">
-        <v>99294</v>
+        <v>99670</v>
       </c>
       <c r="D100">
-        <v>22434</v>
+        <v>22455</v>
       </c>
       <c r="E100">
-        <v>179203255</v>
+        <v>180193270</v>
       </c>
       <c r="F100" t="s">
         <v>20</v>
@@ -3495,13 +3495,13 @@
         <v>10</v>
       </c>
       <c r="C101">
-        <v>6319</v>
+        <v>6332</v>
       </c>
       <c r="D101">
         <v>1887</v>
       </c>
       <c r="E101">
-        <v>11013296</v>
+        <v>11067776</v>
       </c>
       <c r="F101" t="s">
         <v>21</v>
@@ -3524,13 +3524,13 @@
         <v>10</v>
       </c>
       <c r="C102">
-        <v>14707</v>
+        <v>14730</v>
       </c>
       <c r="D102">
-        <v>4940</v>
+        <v>4941</v>
       </c>
       <c r="E102">
-        <v>26483701</v>
+        <v>26632980</v>
       </c>
       <c r="F102" t="s">
         <v>21</v>
@@ -3553,13 +3553,13 @@
         <v>10</v>
       </c>
       <c r="C103">
-        <v>4668</v>
+        <v>4679</v>
       </c>
       <c r="D103">
         <v>1836</v>
       </c>
       <c r="E103">
-        <v>9507365</v>
+        <v>9585677</v>
       </c>
       <c r="F103" t="s">
         <v>21</v>
@@ -3582,13 +3582,13 @@
         <v>10</v>
       </c>
       <c r="C104">
-        <v>1687</v>
+        <v>1693</v>
       </c>
       <c r="D104">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="E104">
-        <v>4451597</v>
+        <v>4577405</v>
       </c>
       <c r="F104" t="s">
         <v>21</v>
@@ -3611,13 +3611,13 @@
         <v>10</v>
       </c>
       <c r="C105">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D105">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E105">
-        <v>3638811</v>
+        <v>3648811</v>
       </c>
       <c r="F105" t="s">
         <v>21</v>
@@ -3698,13 +3698,13 @@
         <v>10</v>
       </c>
       <c r="C108">
-        <v>7042</v>
+        <v>7066</v>
       </c>
       <c r="D108">
         <v>2059</v>
       </c>
       <c r="E108">
-        <v>9967826</v>
+        <v>10007527</v>
       </c>
       <c r="F108" t="s">
         <v>21</v>
@@ -3727,13 +3727,13 @@
         <v>10</v>
       </c>
       <c r="C109">
-        <v>2620</v>
+        <v>2624</v>
       </c>
       <c r="D109">
         <v>684</v>
       </c>
       <c r="E109">
-        <v>5468297</v>
+        <v>5495025</v>
       </c>
       <c r="F109" t="s">
         <v>22</v>
@@ -3756,13 +3756,13 @@
         <v>10</v>
       </c>
       <c r="C110">
-        <v>8174</v>
+        <v>8190</v>
       </c>
       <c r="D110">
-        <v>2211</v>
+        <v>2212</v>
       </c>
       <c r="E110">
-        <v>18690213</v>
+        <v>18751883</v>
       </c>
       <c r="F110" t="s">
         <v>22</v>
@@ -3785,13 +3785,13 @@
         <v>10</v>
       </c>
       <c r="C111">
-        <v>2907</v>
+        <v>2910</v>
       </c>
       <c r="D111">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E111">
-        <v>8154878</v>
+        <v>8167878</v>
       </c>
       <c r="F111" t="s">
         <v>22</v>
@@ -3814,13 +3814,13 @@
         <v>10</v>
       </c>
       <c r="C112">
-        <v>1100</v>
+        <v>1104</v>
       </c>
       <c r="D112">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E112">
-        <v>3515905</v>
+        <v>3564910</v>
       </c>
       <c r="F112" t="s">
         <v>22</v>
@@ -3872,13 +3872,13 @@
         <v>10</v>
       </c>
       <c r="C114">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D114">
         <v>40</v>
       </c>
       <c r="E114">
-        <v>1117430</v>
+        <v>1194410</v>
       </c>
       <c r="F114" t="s">
         <v>22</v>
@@ -3930,13 +3930,13 @@
         <v>10</v>
       </c>
       <c r="C116">
-        <v>5687</v>
+        <v>5699</v>
       </c>
       <c r="D116">
         <v>1405</v>
       </c>
       <c r="E116">
-        <v>8613698</v>
+        <v>8630179</v>
       </c>
       <c r="F116" t="s">
         <v>22</v>
@@ -3959,13 +3959,13 @@
         <v>10</v>
       </c>
       <c r="C117">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="D117">
         <v>235</v>
       </c>
       <c r="E117">
-        <v>3178493</v>
+        <v>3188493</v>
       </c>
       <c r="F117" t="s">
         <v>23</v>
@@ -3988,13 +3988,13 @@
         <v>10</v>
       </c>
       <c r="C118">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D118">
         <v>135</v>
       </c>
       <c r="E118">
-        <v>2240745</v>
+        <v>2242245</v>
       </c>
       <c r="F118" t="s">
         <v>23</v>
@@ -4133,13 +4133,13 @@
         <v>10</v>
       </c>
       <c r="C123">
-        <v>20931</v>
+        <v>21006</v>
       </c>
       <c r="D123">
         <v>5181</v>
       </c>
       <c r="E123">
-        <v>59205728</v>
+        <v>59670806</v>
       </c>
       <c r="F123" t="s">
         <v>24</v>
@@ -4162,13 +4162,13 @@
         <v>10</v>
       </c>
       <c r="C124">
-        <v>55814</v>
+        <v>55993</v>
       </c>
       <c r="D124">
-        <v>14945</v>
+        <v>14951</v>
       </c>
       <c r="E124">
-        <v>188610355</v>
+        <v>189674874</v>
       </c>
       <c r="F124" t="s">
         <v>24</v>
@@ -4191,13 +4191,13 @@
         <v>10</v>
       </c>
       <c r="C125">
-        <v>21195</v>
+        <v>21275</v>
       </c>
       <c r="D125">
-        <v>5701</v>
+        <v>5704</v>
       </c>
       <c r="E125">
-        <v>97109122</v>
+        <v>97840230</v>
       </c>
       <c r="F125" t="s">
         <v>24</v>
@@ -4220,13 +4220,13 @@
         <v>10</v>
       </c>
       <c r="C126">
-        <v>7199</v>
+        <v>7239</v>
       </c>
       <c r="D126">
-        <v>1970</v>
+        <v>1972</v>
       </c>
       <c r="E126">
-        <v>44408506</v>
+        <v>44965782</v>
       </c>
       <c r="F126" t="s">
         <v>24</v>
@@ -4249,13 +4249,13 @@
         <v>10</v>
       </c>
       <c r="C127">
-        <v>2888</v>
+        <v>2910</v>
       </c>
       <c r="D127">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="E127">
-        <v>33771632</v>
+        <v>34037847</v>
       </c>
       <c r="F127" t="s">
         <v>24</v>
@@ -4278,13 +4278,13 @@
         <v>10</v>
       </c>
       <c r="C128">
-        <v>880</v>
+        <v>890</v>
       </c>
       <c r="D128">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E128">
-        <v>24247620</v>
+        <v>24809205</v>
       </c>
       <c r="F128" t="s">
         <v>24</v>
@@ -4307,13 +4307,13 @@
         <v>10</v>
       </c>
       <c r="C129">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D129">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E129">
-        <v>4133953</v>
+        <v>4242309</v>
       </c>
       <c r="F129" t="s">
         <v>24</v>
@@ -4336,13 +4336,13 @@
         <v>10</v>
       </c>
       <c r="C130">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D130">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E130">
-        <v>1897637</v>
+        <v>1897638</v>
       </c>
       <c r="F130" t="s">
         <v>24</v>
@@ -4394,13 +4394,13 @@
         <v>10</v>
       </c>
       <c r="C132">
-        <v>16389</v>
+        <v>16456</v>
       </c>
       <c r="D132">
-        <v>4584</v>
+        <v>4587</v>
       </c>
       <c r="E132">
-        <v>29238257</v>
+        <v>29421043</v>
       </c>
       <c r="F132" t="s">
         <v>24</v>
@@ -4423,13 +4423,13 @@
         <v>10</v>
       </c>
       <c r="C133">
-        <v>58862</v>
+        <v>59133</v>
       </c>
       <c r="D133">
-        <v>14706</v>
+        <v>14722</v>
       </c>
       <c r="E133">
-        <v>169836022</v>
+        <v>171338621</v>
       </c>
       <c r="F133" t="s">
         <v>25</v>
@@ -4452,13 +4452,13 @@
         <v>10</v>
       </c>
       <c r="C134">
-        <v>123852</v>
+        <v>124321</v>
       </c>
       <c r="D134">
-        <v>34297</v>
+        <v>34331</v>
       </c>
       <c r="E134">
-        <v>406410180</v>
+        <v>409501754</v>
       </c>
       <c r="F134" t="s">
         <v>25</v>
@@ -4481,13 +4481,13 @@
         <v>10</v>
       </c>
       <c r="C135">
-        <v>44965</v>
+        <v>45171</v>
       </c>
       <c r="D135">
-        <v>12638</v>
+        <v>12655</v>
       </c>
       <c r="E135">
-        <v>201160098</v>
+        <v>202970250</v>
       </c>
       <c r="F135" t="s">
         <v>25</v>
@@ -4510,13 +4510,13 @@
         <v>10</v>
       </c>
       <c r="C136">
-        <v>15615</v>
+        <v>15719</v>
       </c>
       <c r="D136">
-        <v>4421</v>
+        <v>4435</v>
       </c>
       <c r="E136">
-        <v>94742256</v>
+        <v>96122805</v>
       </c>
       <c r="F136" t="s">
         <v>25</v>
@@ -4539,13 +4539,13 @@
         <v>10</v>
       </c>
       <c r="C137">
-        <v>6506</v>
+        <v>6556</v>
       </c>
       <c r="D137">
-        <v>1825</v>
+        <v>1837</v>
       </c>
       <c r="E137">
-        <v>76455322</v>
+        <v>77221477</v>
       </c>
       <c r="F137" t="s">
         <v>25</v>
@@ -4568,13 +4568,13 @@
         <v>10</v>
       </c>
       <c r="C138">
-        <v>2009</v>
+        <v>2044</v>
       </c>
       <c r="D138">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="E138">
-        <v>61065988</v>
+        <v>62332289</v>
       </c>
       <c r="F138" t="s">
         <v>25</v>
@@ -4597,13 +4597,13 @@
         <v>10</v>
       </c>
       <c r="C139">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D139">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E139">
-        <v>8427958</v>
+        <v>8579586</v>
       </c>
       <c r="F139" t="s">
         <v>25</v>
@@ -4713,13 +4713,13 @@
         <v>10</v>
       </c>
       <c r="C143">
-        <v>43207</v>
+        <v>43397</v>
       </c>
       <c r="D143">
-        <v>12772</v>
+        <v>12795</v>
       </c>
       <c r="E143">
-        <v>75913747</v>
+        <v>76502646</v>
       </c>
       <c r="F143" t="s">
         <v>25</v>
@@ -4742,13 +4742,13 @@
         <v>10</v>
       </c>
       <c r="C144">
-        <v>72388</v>
+        <v>72741</v>
       </c>
       <c r="D144">
-        <v>17030</v>
+        <v>17044</v>
       </c>
       <c r="E144">
-        <v>209428849</v>
+        <v>211167596</v>
       </c>
       <c r="F144" t="s">
         <v>26</v>
@@ -4771,13 +4771,13 @@
         <v>10</v>
       </c>
       <c r="C145">
-        <v>148191</v>
+        <v>148871</v>
       </c>
       <c r="D145">
-        <v>38551</v>
+        <v>38588</v>
       </c>
       <c r="E145">
-        <v>476957087</v>
+        <v>480628604</v>
       </c>
       <c r="F145" t="s">
         <v>26</v>
@@ -4800,13 +4800,13 @@
         <v>10</v>
       </c>
       <c r="C146">
-        <v>50794</v>
+        <v>51048</v>
       </c>
       <c r="D146">
-        <v>13573</v>
+        <v>13586</v>
       </c>
       <c r="E146">
-        <v>227622814</v>
+        <v>229864206</v>
       </c>
       <c r="F146" t="s">
         <v>26</v>
@@ -4829,13 +4829,13 @@
         <v>10</v>
       </c>
       <c r="C147">
-        <v>16459</v>
+        <v>16574</v>
       </c>
       <c r="D147">
-        <v>4477</v>
+        <v>4486</v>
       </c>
       <c r="E147">
-        <v>98726548</v>
+        <v>100052516</v>
       </c>
       <c r="F147" t="s">
         <v>26</v>
@@ -4858,13 +4858,13 @@
         <v>10</v>
       </c>
       <c r="C148">
-        <v>6671</v>
+        <v>6730</v>
       </c>
       <c r="D148">
-        <v>1863</v>
+        <v>1865</v>
       </c>
       <c r="E148">
-        <v>74547600</v>
+        <v>75500595</v>
       </c>
       <c r="F148" t="s">
         <v>26</v>
@@ -4887,13 +4887,13 @@
         <v>10</v>
       </c>
       <c r="C149">
-        <v>1848</v>
+        <v>1873</v>
       </c>
       <c r="D149">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="E149">
-        <v>56853778</v>
+        <v>58150413</v>
       </c>
       <c r="F149" t="s">
         <v>26</v>
@@ -4916,13 +4916,13 @@
         <v>10</v>
       </c>
       <c r="C150">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D150">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E150">
-        <v>10401492</v>
+        <v>10414047</v>
       </c>
       <c r="F150" t="s">
         <v>26</v>
@@ -4945,13 +4945,13 @@
         <v>10</v>
       </c>
       <c r="C151">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D151">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E151">
-        <v>2991182</v>
+        <v>3191183</v>
       </c>
       <c r="F151" t="s">
         <v>26</v>
@@ -5032,13 +5032,13 @@
         <v>10</v>
       </c>
       <c r="C154">
-        <v>54525</v>
+        <v>54752</v>
       </c>
       <c r="D154">
-        <v>15161</v>
+        <v>15176</v>
       </c>
       <c r="E154">
-        <v>91534716</v>
+        <v>92142088</v>
       </c>
       <c r="F154" t="s">
         <v>26</v>
@@ -5061,13 +5061,13 @@
         <v>10</v>
       </c>
       <c r="C155">
-        <v>25362</v>
+        <v>25469</v>
       </c>
       <c r="D155">
         <v>6404</v>
       </c>
       <c r="E155">
-        <v>72901424</v>
+        <v>73396966</v>
       </c>
       <c r="F155" t="s">
         <v>27</v>
@@ -5090,13 +5090,13 @@
         <v>10</v>
       </c>
       <c r="C156">
-        <v>61629</v>
+        <v>61840</v>
       </c>
       <c r="D156">
-        <v>16856</v>
+        <v>16863</v>
       </c>
       <c r="E156">
-        <v>213394337</v>
+        <v>214810324</v>
       </c>
       <c r="F156" t="s">
         <v>27</v>
@@ -5119,13 +5119,13 @@
         <v>10</v>
       </c>
       <c r="C157">
-        <v>24849</v>
+        <v>24950</v>
       </c>
       <c r="D157">
-        <v>6934</v>
+        <v>6939</v>
       </c>
       <c r="E157">
-        <v>115196075</v>
+        <v>116119270</v>
       </c>
       <c r="F157" t="s">
         <v>27</v>
@@ -5148,13 +5148,13 @@
         <v>10</v>
       </c>
       <c r="C158">
-        <v>7789</v>
+        <v>7830</v>
       </c>
       <c r="D158">
-        <v>2337</v>
+        <v>2339</v>
       </c>
       <c r="E158">
-        <v>48202672</v>
+        <v>48702077</v>
       </c>
       <c r="F158" t="s">
         <v>27</v>
@@ -5177,13 +5177,13 @@
         <v>10</v>
       </c>
       <c r="C159">
-        <v>3257</v>
+        <v>3285</v>
       </c>
       <c r="D159">
-        <v>995</v>
+        <v>999</v>
       </c>
       <c r="E159">
-        <v>39760385</v>
+        <v>40338848</v>
       </c>
       <c r="F159" t="s">
         <v>27</v>
@@ -5206,13 +5206,13 @@
         <v>10</v>
       </c>
       <c r="C160">
-        <v>1064</v>
+        <v>1074</v>
       </c>
       <c r="D160">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="E160">
-        <v>32503979</v>
+        <v>32857486</v>
       </c>
       <c r="F160" t="s">
         <v>27</v>
@@ -5235,13 +5235,13 @@
         <v>10</v>
       </c>
       <c r="C161">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D161">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E161">
-        <v>3111078</v>
+        <v>3211114</v>
       </c>
       <c r="F161" t="s">
         <v>27</v>
@@ -5293,13 +5293,13 @@
         <v>10</v>
       </c>
       <c r="C163">
-        <v>17813</v>
+        <v>17870</v>
       </c>
       <c r="D163">
-        <v>5153</v>
+        <v>5154</v>
       </c>
       <c r="E163">
-        <v>31643587</v>
+        <v>31781012</v>
       </c>
       <c r="F163" t="s">
         <v>27</v>
@@ -5322,13 +5322,13 @@
         <v>10</v>
       </c>
       <c r="C164">
-        <v>71231</v>
+        <v>71559</v>
       </c>
       <c r="D164">
-        <v>16570</v>
+        <v>16580</v>
       </c>
       <c r="E164">
-        <v>203488830</v>
+        <v>205124974</v>
       </c>
       <c r="F164" t="s">
         <v>28</v>
@@ -5351,13 +5351,13 @@
         <v>10</v>
       </c>
       <c r="C165">
-        <v>165145</v>
+        <v>165803</v>
       </c>
       <c r="D165">
-        <v>40309</v>
+        <v>40337</v>
       </c>
       <c r="E165">
-        <v>544917912</v>
+        <v>548685548</v>
       </c>
       <c r="F165" t="s">
         <v>28</v>
@@ -5380,13 +5380,13 @@
         <v>10</v>
       </c>
       <c r="C166">
-        <v>56206</v>
+        <v>56469</v>
       </c>
       <c r="D166">
-        <v>13777</v>
+        <v>13798</v>
       </c>
       <c r="E166">
-        <v>266879035</v>
+        <v>269331178</v>
       </c>
       <c r="F166" t="s">
         <v>28</v>
@@ -5409,13 +5409,13 @@
         <v>10</v>
       </c>
       <c r="C167">
-        <v>18604</v>
+        <v>18714</v>
       </c>
       <c r="D167">
-        <v>4558</v>
+        <v>4563</v>
       </c>
       <c r="E167">
-        <v>125068640</v>
+        <v>126475956</v>
       </c>
       <c r="F167" t="s">
         <v>28</v>
@@ -5438,13 +5438,13 @@
         <v>10</v>
       </c>
       <c r="C168">
-        <v>8267</v>
+        <v>8330</v>
       </c>
       <c r="D168">
-        <v>2115</v>
+        <v>2121</v>
       </c>
       <c r="E168">
-        <v>100965272</v>
+        <v>102014966</v>
       </c>
       <c r="F168" t="s">
         <v>28</v>
@@ -5467,13 +5467,13 @@
         <v>10</v>
       </c>
       <c r="C169">
-        <v>2396</v>
+        <v>2424</v>
       </c>
       <c r="D169">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="E169">
-        <v>77529339</v>
+        <v>78700225</v>
       </c>
       <c r="F169" t="s">
         <v>28</v>
@@ -5496,13 +5496,13 @@
         <v>10</v>
       </c>
       <c r="C170">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D170">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E170">
-        <v>17474570</v>
+        <v>17807367</v>
       </c>
       <c r="F170" t="s">
         <v>28</v>
@@ -5554,13 +5554,13 @@
         <v>10</v>
       </c>
       <c r="C172">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D172">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E172">
-        <v>1167990</v>
+        <v>1167991</v>
       </c>
       <c r="F172" t="s">
         <v>28</v>
@@ -5612,13 +5612,13 @@
         <v>10</v>
       </c>
       <c r="C174">
-        <v>51885</v>
+        <v>52073</v>
       </c>
       <c r="D174">
-        <v>13454</v>
+        <v>13465</v>
       </c>
       <c r="E174">
-        <v>90588822</v>
+        <v>91164440</v>
       </c>
       <c r="F174" t="s">
         <v>28</v>

</xml_diff>